<commit_message>
some scratch xls update
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="66">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -434,6 +434,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,7 +476,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31"/>
   </cellXfs>
-  <cellStyles count="66">
+  <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -524,6 +526,8 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1155,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I40"/>
+    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1202,8 +1206,8 @@
         <v>106</v>
       </c>
       <c r="I2" t="str">
-        <f>$A$1&amp;$B$1&amp;C2&amp;$D$1&amp;E2&amp;"-"&amp;F2&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beathappening-angelgone-7inch.mp3\"&gt;Beat Happening-Angel Gone bw Zombie Limbo Time-&lt;/option&gt;");</v>
+        <f t="shared" ref="I2:I40" si="0">$A$1&amp;$B$1&amp;C2&amp;$D$1&amp;E2&amp;"-"&amp;F2&amp;"-"&amp;G2&amp;$H$1</f>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beathappening-angelgone-7inch.mp3\"&gt;Beat Happening-Angel Gone bw Zombie Limbo Time-Side Only&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1220,8 +1224,8 @@
         <v>48</v>
       </c>
       <c r="I3" t="str">
-        <f>$A$1&amp;$B$1&amp;C3&amp;$D$1&amp;E3&amp;"-"&amp;F3&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beathappening-blackcandy-sidea.mp3\"&gt;Beat Happening-Black Candy-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beathappening-blackcandy-sidea.mp3\"&gt;Beat Happening-Black Candy-Side A&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1238,8 +1242,8 @@
         <v>49</v>
       </c>
       <c r="I4" t="str">
-        <f>$A$1&amp;$B$1&amp;C4&amp;$D$1&amp;E4&amp;"-"&amp;F4&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beathappening-blackcandy-sideb.mp3\"&gt;Beat Happening-Black Candy-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beathappening-blackcandy-sideb.mp3\"&gt;Beat Happening-Black Candy-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1256,8 +1260,8 @@
         <v>48</v>
       </c>
       <c r="I5" t="str">
-        <f>$A$1&amp;$B$1&amp;C5&amp;$D$1&amp;E5&amp;"-"&amp;F5&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sidea.mp3\"&gt;Beck-One Foot In The Grave-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sidea.mp3\"&gt;Beck-One Foot In The Grave-Side A&lt;/option&gt;");</v>
       </c>
       <c r="M5" s="1"/>
     </row>
@@ -1275,8 +1279,8 @@
         <v>49</v>
       </c>
       <c r="I6" t="str">
-        <f>$A$1&amp;$B$1&amp;C6&amp;$D$1&amp;E6&amp;"-"&amp;F6&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sideb.mp3\"&gt;Beck-One Foot In The Grave-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sideb.mp3\"&gt;Beck-One Foot In The Grave-Side B&lt;/option&gt;");</v>
       </c>
       <c r="J6" s="1"/>
       <c r="M6" s="1"/>
@@ -1295,8 +1299,8 @@
         <v>51</v>
       </c>
       <c r="I7" t="str">
-        <f>$A$1&amp;$B$1&amp;C7&amp;$D$1&amp;E7&amp;"-"&amp;F7&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sidec.mp3\"&gt;Beck-One Foot In The Grave-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sidec.mp3\"&gt;Beck-One Foot In The Grave-Side C&lt;/option&gt;");</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -1314,8 +1318,8 @@
         <v>50</v>
       </c>
       <c r="I8" t="str">
-        <f>$A$1&amp;$B$1&amp;C8&amp;$D$1&amp;E8&amp;"-"&amp;F8&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sided.mp3\"&gt;Beck-One Foot In The Grave-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/beck-onefootinthegrave-sided.mp3\"&gt;Beck-One Foot In The Grave-Side D&lt;/option&gt;");</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -1333,8 +1337,8 @@
         <v>48</v>
       </c>
       <c r="I9" t="str">
-        <f>$A$1&amp;$B$1&amp;C9&amp;$D$1&amp;E9&amp;"-"&amp;F9&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/gits-frenchingthebully-sidea.mp3\"&gt;Gits-Frenching the Bully-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/gits-frenchingthebully-sidea.mp3\"&gt;Gits-Frenching the Bully-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -1352,8 +1356,8 @@
         <v>49</v>
       </c>
       <c r="I10" t="str">
-        <f>$A$1&amp;$B$1&amp;C10&amp;$D$1&amp;E10&amp;"-"&amp;F10&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/gits-frenchingthebully-sideb.mp3\"&gt;Gits-Frenching the Bully-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/gits-frenchingthebully-sideb.mp3\"&gt;Gits-Frenching the Bully-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1370,8 +1374,8 @@
         <v>48</v>
       </c>
       <c r="I11" t="str">
-        <f>$A$1&amp;$B$1&amp;C11&amp;$D$1&amp;E11&amp;"-"&amp;F11&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/greenriver-rehabdoll-sidea.mp3\"&gt;Greenriver-Rehab Doll-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/greenriver-rehabdoll-sidea.mp3\"&gt;Greenriver-Rehab Doll-Side A&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1388,8 +1392,8 @@
         <v>49</v>
       </c>
       <c r="I12" t="str">
-        <f>$A$1&amp;$B$1&amp;C12&amp;$D$1&amp;E12&amp;"-"&amp;F12&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/greenriver-rehabdoll-sideb.mp3\"&gt;Greenriver-Rehab Doll-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/greenriver-rehabdoll-sideb.mp3\"&gt;Greenriver-Rehab Doll-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1406,8 +1410,8 @@
         <v>48</v>
       </c>
       <c r="I13" t="str">
-        <f>$A$1&amp;$B$1&amp;C13&amp;$D$1&amp;E13&amp;"-"&amp;F13&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/halobenders-goddontmakenojunk-sidea.mp3\"&gt;Halo Benders-God Dont Make No Junk-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/halobenders-goddontmakenojunk-sidea.mp3\"&gt;Halo Benders-God Dont Make No Junk-Side A&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1424,8 +1428,8 @@
         <v>49</v>
       </c>
       <c r="I14" t="str">
-        <f>$A$1&amp;$B$1&amp;C14&amp;$D$1&amp;E14&amp;"-"&amp;F14&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/halobenders-goddontmakenojunk-sideb.mp3\"&gt;Halo Benders-God Dont Make No Junk-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/halobenders-goddontmakenojunk-sideb.mp3\"&gt;Halo Benders-God Dont Make No Junk-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1442,8 +1446,8 @@
         <v>48</v>
       </c>
       <c r="I15" t="str">
-        <f>$A$1&amp;$B$1&amp;C15&amp;$D$1&amp;E15&amp;"-"&amp;F15&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sidea.mp3\"&gt;ICU-Chotto Matte A Moment-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sidea.mp3\"&gt;ICU-Chotto Matte A Moment-Side A&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1460,8 +1464,8 @@
         <v>49</v>
       </c>
       <c r="I16" t="str">
-        <f>$A$1&amp;$B$1&amp;C16&amp;$D$1&amp;E16&amp;"-"&amp;F16&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sideb.mp3\"&gt;ICU-Chotto Matte A Moment-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sideb.mp3\"&gt;ICU-Chotto Matte A Moment-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="17" spans="3:10">
@@ -1478,8 +1482,8 @@
         <v>51</v>
       </c>
       <c r="I17" t="str">
-        <f>$A$1&amp;$B$1&amp;C17&amp;$D$1&amp;E17&amp;"-"&amp;F17&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sidec.mp3\"&gt;ICU-Chotto Matte A Moment-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sidec.mp3\"&gt;ICU-Chotto Matte A Moment-Side C&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="18" spans="3:10">
@@ -1496,8 +1500,8 @@
         <v>50</v>
       </c>
       <c r="I18" t="str">
-        <f>$A$1&amp;$B$1&amp;C18&amp;$D$1&amp;E18&amp;"-"&amp;F18&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sided.mp3\"&gt;ICU-Chotto Matte A Moment-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-chottomatteamoment-sided.mp3\"&gt;ICU-Chotto Matte A Moment-Side D&lt;/option&gt;");</v>
       </c>
       <c r="J18" s="1"/>
     </row>
@@ -1515,8 +1519,8 @@
         <v>106</v>
       </c>
       <c r="I19" t="str">
-        <f>$A$1&amp;$B$1&amp;C19&amp;$D$1&amp;E19&amp;"-"&amp;F19&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-dothetwistBWrussianrhapsody.mp3\"&gt;ICU-Do the Twist bw Russian Rhapsody-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/icu-dothetwistBWrussianrhapsody.mp3\"&gt;ICU-Do the Twist bw Russian Rhapsody-Side Only&lt;/option&gt;");</v>
       </c>
       <c r="J19" s="1"/>
     </row>
@@ -1534,8 +1538,8 @@
         <v>48</v>
       </c>
       <c r="I20" t="str">
-        <f>$A$1&amp;$B$1&amp;C20&amp;$D$1&amp;E20&amp;"-"&amp;F20&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/kingbuzzo-thismachinekillsartists-sidea.mp3\"&gt;King Buzzo-This Machine Kills Artists-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/kingbuzzo-thismachinekillsartists-sidea.mp3\"&gt;King Buzzo-This Machine Kills Artists-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J20" s="1"/>
     </row>
@@ -1553,8 +1557,8 @@
         <v>49</v>
       </c>
       <c r="I21" t="str">
-        <f>$A$1&amp;$B$1&amp;C21&amp;$D$1&amp;E21&amp;"-"&amp;F21&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/kingbuzzo-thismachinekillsartists-sideb.mp3\"&gt;King Buzzo-This Machine Kills Artists-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/kingbuzzo-thismachinekillsartists-sideb.mp3\"&gt;King Buzzo-This Machine Kills Artists-Side B&lt;/option&gt;");</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -1572,8 +1576,8 @@
         <v>48</v>
       </c>
       <c r="I22" t="str">
-        <f>$A$1&amp;$B$1&amp;C22&amp;$D$1&amp;E22&amp;"-"&amp;F22&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sidea.mp3\"&gt;Mad Season-Above-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sidea.mp3\"&gt;Mad Season-Above-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J22" s="1"/>
     </row>
@@ -1591,8 +1595,8 @@
         <v>49</v>
       </c>
       <c r="I23" t="str">
-        <f>$A$1&amp;$B$1&amp;C23&amp;$D$1&amp;E23&amp;"-"&amp;F23&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sideb.mp3\"&gt;Mad Season-Above-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sideb.mp3\"&gt;Mad Season-Above-Side B&lt;/option&gt;");</v>
       </c>
       <c r="J23" s="1"/>
     </row>
@@ -1610,8 +1614,8 @@
         <v>51</v>
       </c>
       <c r="I24" t="str">
-        <f>$A$1&amp;$B$1&amp;C24&amp;$D$1&amp;E24&amp;"-"&amp;F24&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sidec.mp3\"&gt;Mad Season-Above-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sidec.mp3\"&gt;Mad Season-Above-Side C&lt;/option&gt;");</v>
       </c>
       <c r="J24" s="1"/>
     </row>
@@ -1629,8 +1633,8 @@
         <v>50</v>
       </c>
       <c r="I25" t="str">
-        <f>$A$1&amp;$B$1&amp;C25&amp;$D$1&amp;E25&amp;"-"&amp;F25&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sided.mp3\"&gt;Mad Season-Above-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/madseason-above-sided.mp3\"&gt;Mad Season-Above-Side D&lt;/option&gt;");</v>
       </c>
       <c r="J25" s="1"/>
     </row>
@@ -1651,8 +1655,8 @@
         <v>48</v>
       </c>
       <c r="I26" t="str">
-        <f>$A$1&amp;$B$1&amp;C26&amp;$D$1&amp;E26&amp;"-"&amp;F26&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sidea.mp3\"&gt;Pearl Jam-Ten-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sidea.mp3\"&gt;Pearl Jam-Ten-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J26" s="1"/>
     </row>
@@ -1670,8 +1674,8 @@
         <v>49</v>
       </c>
       <c r="I27" t="str">
-        <f>$A$1&amp;$B$1&amp;C27&amp;$D$1&amp;E27&amp;"-"&amp;F27&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sideb.mp3\"&gt;Pearl Jam-Ten-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sideb.mp3\"&gt;Pearl Jam-Ten-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="28" spans="3:10">
@@ -1688,8 +1692,8 @@
         <v>51</v>
       </c>
       <c r="I28" t="str">
-        <f>$A$1&amp;$B$1&amp;C28&amp;$D$1&amp;E28&amp;"-"&amp;F28&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sidec.mp3\"&gt;Pearl Jam-Ten-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sidec.mp3\"&gt;Pearl Jam-Ten-Side C&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="29" spans="3:10">
@@ -1706,8 +1710,8 @@
         <v>50</v>
       </c>
       <c r="I29" t="str">
-        <f>$A$1&amp;$B$1&amp;C29&amp;$D$1&amp;E29&amp;"-"&amp;F29&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sided.mp3\"&gt;Pearl Jam-Ten-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-tenremix-sided.mp3\"&gt;Pearl Jam-Ten-Side D&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="30" spans="3:10">
@@ -1724,8 +1728,8 @@
         <v>48</v>
       </c>
       <c r="I30" t="str">
-        <f>$A$1&amp;$B$1&amp;C30&amp;$D$1&amp;E30&amp;"-"&amp;F30&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-vs-sidea.mp3\"&gt;Pearl Jam-VS-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-vs-sidea.mp3\"&gt;Pearl Jam-VS-Side A&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="31" spans="3:10">
@@ -1742,8 +1746,8 @@
         <v>49</v>
       </c>
       <c r="I31" t="str">
-        <f>$A$1&amp;$B$1&amp;C31&amp;$D$1&amp;E31&amp;"-"&amp;F31&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-vs-sideb.mp3\"&gt;Pearl Jam-VS-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/pearljam-vs-sideb.mp3\"&gt;Pearl Jam-VS-Side B&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="32" spans="3:10">
@@ -1760,8 +1764,8 @@
         <v>48</v>
       </c>
       <c r="I32" t="str">
-        <f>$A$1&amp;$B$1&amp;C32&amp;$D$1&amp;E32&amp;"-"&amp;F32&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/resolution-tape-sidea.mp3\"&gt;Resolution-Tape-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/resolution-tape-sidea.mp3\"&gt;Resolution-Tape-Side A&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="33" spans="3:11">
@@ -1778,8 +1782,8 @@
         <v>49</v>
       </c>
       <c r="I33" t="str">
-        <f>$A$1&amp;$B$1&amp;C33&amp;$D$1&amp;E33&amp;"-"&amp;F33&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/resolution-tape-sideb.mp3\"&gt;Resolution-Tape-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/resolution-tape-sideb.mp3\"&gt;Resolution-Tape-Side B&lt;/option&gt;");</v>
       </c>
       <c r="K33" s="1"/>
     </row>
@@ -1797,8 +1801,8 @@
         <v>106</v>
       </c>
       <c r="I34" t="str">
-        <f>$A$1&amp;$B$1&amp;C34&amp;$D$1&amp;E34&amp;"-"&amp;F34&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-dilaudid-7inch.mp3\"&gt;Zeke-Dilaudid-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-dilaudid-7inch.mp3\"&gt;Zeke-Dilaudid-Side Only&lt;/option&gt;");</v>
       </c>
     </row>
     <row r="35" spans="3:11">
@@ -1815,8 +1819,8 @@
         <v>48</v>
       </c>
       <c r="I35" t="str">
-        <f>$A$1&amp;$B$1&amp;C35&amp;$D$1&amp;E35&amp;"-"&amp;F35&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-flattracker-sidea.mp3\"&gt;Zeke-Flat Tracker-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-flattracker-sidea.mp3\"&gt;Zeke-Flat Tracker-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J35" s="1"/>
     </row>
@@ -1834,8 +1838,8 @@
         <v>49</v>
       </c>
       <c r="I36" t="str">
-        <f>$A$1&amp;$B$1&amp;C36&amp;$D$1&amp;E36&amp;"-"&amp;F36&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-flattracker-sideb.mp3\"&gt;Zeke-Flat Tracker-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-flattracker-sideb.mp3\"&gt;Zeke-Flat Tracker-Side B&lt;/option&gt;");</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -1853,8 +1857,8 @@
         <v>48</v>
       </c>
       <c r="I37" t="str">
-        <f>$A$1&amp;$B$1&amp;C37&amp;$D$1&amp;E37&amp;"-"&amp;F37&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-kickedintheteeth-sidea.mp3\"&gt;Zeke-Kicked in the Teeth-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-kickedintheteeth-sidea.mp3\"&gt;Zeke-Kicked in the Teeth-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J37" s="1"/>
     </row>
@@ -1872,8 +1876,8 @@
         <v>49</v>
       </c>
       <c r="I38" t="str">
-        <f>$A$1&amp;$B$1&amp;C38&amp;$D$1&amp;E38&amp;"-"&amp;F38&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-kickedintheteeth-sideb.mp3\"&gt;Zeke-Kicked in the Teeth-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-kickedintheteeth-sideb.mp3\"&gt;Zeke-Kicked in the Teeth-Side B&lt;/option&gt;");</v>
       </c>
       <c r="J38" s="1"/>
     </row>
@@ -1891,8 +1895,8 @@
         <v>48</v>
       </c>
       <c r="I39" t="str">
-        <f>$A$1&amp;$B$1&amp;C39&amp;$D$1&amp;E39&amp;"-"&amp;F39&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-supersoundracing-sidea.mp3\"&gt;Zeke-Super Sound Racing-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-supersoundracing-sidea.mp3\"&gt;Zeke-Super Sound Racing-Side A&lt;/option&gt;");</v>
       </c>
       <c r="J39" s="1"/>
     </row>
@@ -1910,8 +1914,8 @@
         <v>49</v>
       </c>
       <c r="I40" t="str">
-        <f>$A$1&amp;$B$1&amp;C40&amp;$D$1&amp;E40&amp;"-"&amp;F40&amp;"-"&amp;$H$1</f>
-        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-supersoundracing-sideb.mp3\"&gt;Zeke-Super Sound Racing-&lt;/option&gt;");</v>
+        <f t="shared" si="0"/>
+        <v>document.write("&lt;option value=\"http://analogarchive.com/analogarchive/analog/zeke-supersoundracing-sideb.mp3\"&gt;Zeke-Super Sound Racing-Side B&lt;/option&gt;");</v>
       </c>
       <c r="J40" s="1"/>
     </row>

</xml_diff>

<commit_message>
updates to spreadsheet and added json file
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="133">
   <si>
     <t>bettyphotosessionone01.jpg</t>
   </si>
@@ -353,6 +354,72 @@
   </si>
   <si>
     <t>&lt;/option&gt;");</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/analogarchive/live/ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3</t>
   </si>
 </sst>
 </file>
@@ -401,7 +468,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -434,6 +501,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -476,7 +550,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="31"/>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -528,6 +602,13 @@
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1159,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1954,4 +2035,161 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"{'httpmp3filepath':'"&amp;A1&amp;"','tracktitle':'"&amp;B1&amp;"'}"</f>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C11" si="0">"{'httpmp3filepath':'"&amp;A2&amp;"','tracktitle':'"&amp;B2&amp;"'}"</f>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>{'httpmp3filepath':'http://analogarchive.com/analogarchive/live/ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3','tracktitle':'ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3'}</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new json sheet
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="41620" windowHeight="24500" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="OPTION" sheetId="1" r:id="rId1"/>
+    <sheet name="JSON" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="140">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -323,39 +323,21 @@
     <t>skerik15-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
-    <t>skerik1.JPG</t>
-  </si>
-  <si>
     <t>skerik1-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
-    <t>skerik2.JPG</t>
-  </si>
-  <si>
     <t>skerik2-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
-    <t>skerik3.JPG</t>
-  </si>
-  <si>
     <t>skerik3-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
-    <t>skerik4.JPG</t>
-  </si>
-  <si>
     <t>skerik4-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
-    <t>skerik5.JPG</t>
-  </si>
-  <si>
     <t>skerik5-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
-    <t>skerik6.JPG</t>
-  </si>
-  <si>
     <t>skerik6-SkerikTrio-OwlnThistle-20130206.mp3</t>
   </si>
   <si>
@@ -366,6 +348,99 @@
   </si>
   <si>
     <t>skerik9-SkerikTrio-OwlnThistle-20130206.mp3</t>
+  </si>
+  <si>
+    <t>filepath</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>album</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>http://analogarchive.com/live/</t>
+  </si>
+  <si>
+    <t>roxhill locals</t>
+  </si>
+  <si>
+    <t>roxhill sessions 20150827</t>
+  </si>
+  <si>
+    <t>http://seattlerules.com/vinyl.jpeg</t>
+  </si>
+  <si>
+    <t>skerik trio</t>
+  </si>
+  <si>
+    <t>owl n thistle 20130206</t>
+  </si>
+  <si>
+    <t>owl n thistle 20130213</t>
+  </si>
+  <si>
+    <t>ZOOM0001-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0002-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0003-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0006-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0007-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0008-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0009-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0014-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0015-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0016-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0017-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0018-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0019-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0020-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0021-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>track</t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -421,8 +496,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -462,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -480,6 +563,10 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -497,6 +584,10 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -828,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38:F69"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1294,10 +1385,10 @@
     </row>
     <row r="38" spans="2:6">
       <c r="B38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -1378,10 +1469,10 @@
     </row>
     <row r="45" spans="2:6">
       <c r="B45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -1390,10 +1481,10 @@
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -1402,10 +1493,10 @@
     </row>
     <row r="47" spans="2:6">
       <c r="B47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
@@ -1414,10 +1505,10 @@
     </row>
     <row r="48" spans="2:6">
       <c r="B48" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
@@ -1426,10 +1517,10 @@
     </row>
     <row r="49" spans="2:6">
       <c r="B49" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
@@ -1438,10 +1529,10 @@
     </row>
     <row r="50" spans="2:6">
       <c r="B50" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
@@ -1450,10 +1541,10 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D51" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
@@ -1462,10 +1553,10 @@
     </row>
     <row r="52" spans="2:6">
       <c r="B52" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
@@ -1689,97 +1780,1382 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="G29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
+      </c>
+      <c r="G32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34">
+        <v>33</v>
+      </c>
+      <c r="G34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35">
+        <v>34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36">
+        <v>35</v>
+      </c>
+      <c r="G36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37">
+        <v>36</v>
+      </c>
+      <c r="G37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38">
+        <v>37</v>
+      </c>
+      <c r="G38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="G45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="G46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="G48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50">
+        <v>6</v>
+      </c>
+      <c r="G50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="G51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="G52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>108</v>
+      </c>
+      <c r="E53">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="D54" t="s">
+        <v>119</v>
+      </c>
+      <c r="G54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="G55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="G56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="G57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="G58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="G59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="G60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="G61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+      <c r="G62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+      <c r="G63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="G64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+      <c r="G65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+      <c r="G66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+      <c r="G67" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+      <c r="G68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>113</v>
+      </c>
+      <c r="B69" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="G69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" t="s">
         <v>93</v>
+      </c>
+      <c r="G70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" t="s">
+        <v>120</v>
+      </c>
+      <c r="G71" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" t="s">
+        <v>121</v>
+      </c>
+      <c r="G72" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" t="s">
+        <v>122</v>
+      </c>
+      <c r="G73" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" t="s">
+        <v>123</v>
+      </c>
+      <c r="G74" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>113</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="G75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76" t="s">
+        <v>125</v>
+      </c>
+      <c r="G76" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>113</v>
+      </c>
+      <c r="B77" t="s">
+        <v>126</v>
+      </c>
+      <c r="G77" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" t="s">
+        <v>127</v>
+      </c>
+      <c r="G78" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+      <c r="G79" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" t="s">
+        <v>129</v>
+      </c>
+      <c r="G80" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" t="s">
+        <v>130</v>
+      </c>
+      <c r="G81" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" t="s">
+        <v>131</v>
+      </c>
+      <c r="G82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>113</v>
+      </c>
+      <c r="B83" t="s">
+        <v>132</v>
+      </c>
+      <c r="G83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" t="s">
+        <v>133</v>
+      </c>
+      <c r="G84" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" t="s">
+        <v>134</v>
+      </c>
+      <c r="G85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>113</v>
+      </c>
+      <c r="B86" t="s">
+        <v>135</v>
+      </c>
+      <c r="G86" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" t="s">
+        <v>136</v>
+      </c>
+      <c r="G87" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>113</v>
+      </c>
+      <c r="B88" t="s">
+        <v>137</v>
+      </c>
+      <c r="G88" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1795,123 +3171,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A15"/>
+      <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A1:A21">
-    <sortCondition ref="A1"/>
-  </sortState>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
took out lex and put in some suffering
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="42840" windowHeight="22900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OPTION" sheetId="1" r:id="rId1"/>
     <sheet name="JSON" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="IMG" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="222">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -441,6 +441,252 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>ZOOM0001-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0002-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0003-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0006-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0007-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0008-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0008-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0008-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0009-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0009-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0010-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0010-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0011-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0011-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0011-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0013-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0013-sufferingfuckheads-coppergate-20130326.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0013-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0014-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0014-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0015-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0015-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0016-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0016-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0017-sufferingfuckheads-coppergate-20130604.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0018-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0019-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0019-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0020-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0021-sufferingfuckheads-coppergate-20130205.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0022-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0023-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0025-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0026-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0028-sufferingfuckheads-coppergate-20130423.mp3</t>
+  </si>
+  <si>
+    <t>Suffering Fuckheads - Coppergate - March 26th, 2013</t>
+  </si>
+  <si>
+    <t>Suffering Fuckheads - Coppergate - February 12th, 2013</t>
+  </si>
+  <si>
+    <t>Suffering Fuckheads - Coppergate - February 5th, 2013</t>
+  </si>
+  <si>
+    <t>Suffering Fuckheads - Coppergate - June 4th, 2013</t>
+  </si>
+  <si>
+    <t>Suffering Fuckheads - Coppergate - April 23rd, 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">05 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">07 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">08 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">09 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 </t>
+  </si>
+  <si>
+    <t>suffering201306071854a.JPG</t>
+  </si>
+  <si>
+    <t>suffering201306071854.JPG</t>
+  </si>
+  <si>
+    <t>suffering201304252109.JPG</t>
+  </si>
+  <si>
+    <t>suffering201303272002b.JPG</t>
+  </si>
+  <si>
+    <t>suffering201303272002a.JPG</t>
+  </si>
+  <si>
+    <t>suffering201303272001a.JPG</t>
+  </si>
+  <si>
+    <t>suffering201303272001.JPG</t>
+  </si>
+  <si>
+    <t>suffering201302131850.JPG</t>
+  </si>
+  <si>
+    <t>suffering201302060154c.JPG</t>
+  </si>
+  <si>
+    <t>suffering201302060154b.JPG</t>
+  </si>
+  <si>
+    <t>suffering201302060154a.JPG</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='</t>
+  </si>
+  <si>
+    <t>'&gt;&lt;/a&gt;&lt;br /&gt;</t>
   </si>
 </sst>
 </file>
@@ -496,7 +742,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -540,12 +786,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="80">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -567,6 +852,25 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -588,6 +892,24 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -917,20 +1239,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B69"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78.1640625" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.1640625" customWidth="1"/>
+    <col min="7" max="7" width="142.6640625" customWidth="1"/>
+    <col min="8" max="8" width="78.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -940,836 +1262,1608 @@
       <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="str">
-        <f>$A$1&amp;B1&amp;$C$1&amp;D1&amp;$E$1</f>
+      <c r="G1" t="str">
+        <f>$A$1&amp;B1&amp;$C$1&amp;D1&amp;E1&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001roxhillsessions20150827.mp3\"&gt;01roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F65" si="0">$A$1&amp;B2&amp;$C$1&amp;D2&amp;$E$1</f>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G65" si="0">$A$1&amp;B2&amp;$C$1&amp;D2&amp;E2&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002roxhillsessions20150827.mp3\"&gt;02roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003roxhillsessions20150827.mp3\"&gt;03roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004roxhillsessions20150827.mp3\"&gt;04roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005roxhillsessions20150827.mp3\"&gt;05roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006roxhillsessions20150827.mp3\"&gt;06roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007roxhillsessions20150827.mp3\"&gt;07roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>46</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008roxhillsessions20150827.mp3\"&gt;08roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009roxhillsessions20150827.mp3\"&gt;09roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010roxhillsessions20150827.mp3\"&gt;10roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011roxhillsessions20150827.mp3\"&gt;11roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012roxhillsessions20150827.mp3\"&gt;12roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013roxhillsessions20150827.mp3\"&gt;13roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>52</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014roxhillsessions20150827.mp3\"&gt;14roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015roxhillsessions20150827.mp3\"&gt;15roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016roxhillsessions20150827.mp3\"&gt;16roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>55</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017roxhillsessions20150827.mp3\"&gt;17roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:7">
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018roxhillsessions20150827.mp3\"&gt;18roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:7">
       <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>57</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019roxhillsessions20150827.mp3\"&gt;19roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:7">
       <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>58</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020roxhillsessions20150827.mp3\"&gt;20roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:7">
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>59</v>
       </c>
-      <c r="F21" t="str">
+      <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0021roxhillsessions20150827.mp3\"&gt;21roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:7">
       <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>60</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0022roxhillsessions20150827.mp3\"&gt;22roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:7">
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>61</v>
       </c>
-      <c r="F23" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0023roxhillsessions20150827.mp3\"&gt;23roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:7">
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>62</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0024roxhillsessions20150827.mp3\"&gt;24roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:7">
       <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>63</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0025roxhillsessions20150827.mp3\"&gt;25roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:7">
       <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>64</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0026roxhillsessions20150827.mp3\"&gt;26roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:7">
       <c r="B27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>65</v>
       </c>
-      <c r="F27" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0027roxhillsessions20150827.mp3\"&gt;27roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:7">
       <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>66</v>
       </c>
-      <c r="F28" t="str">
-        <f>$A$1&amp;B28&amp;$C$1&amp;D28&amp;$E$1</f>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0028roxhillsessions20150827.mp3\"&gt;28roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:7">
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>67</v>
       </c>
-      <c r="F29" t="str">
+      <c r="G29" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0029roxhillsessions20150827.mp3\"&gt;29roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:7">
       <c r="B30" t="s">
         <v>35</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>68</v>
       </c>
-      <c r="F30" t="str">
+      <c r="G30" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0030roxhillsessions20150827.mp3\"&gt;30roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:7">
       <c r="B31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>69</v>
       </c>
-      <c r="F31" t="str">
+      <c r="G31" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0031roxhillsessions20150827.mp3\"&gt;31roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:7">
       <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>70</v>
       </c>
-      <c r="F32" t="str">
+      <c r="G32" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0032roxhillsessions20150827.mp3\"&gt;32roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:7">
       <c r="B33" t="s">
         <v>22</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>71</v>
       </c>
-      <c r="F33" t="str">
+      <c r="G33" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0033roxhillsessions20150827.mp3\"&gt;33roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:7">
       <c r="B34" t="s">
         <v>29</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>72</v>
       </c>
-      <c r="F34" t="str">
+      <c r="G34" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0034roxhillsessions20150827.mp3\"&gt;34roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:7">
       <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>73</v>
       </c>
-      <c r="F35" t="str">
+      <c r="G35" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0035roxhillsessions20150827.mp3\"&gt;35roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:7">
       <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F36" t="str">
+      <c r="G36" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0036roxhillsessions20150827.mp3\"&gt;36roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:7">
       <c r="B37" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F37" t="str">
+      <c r="G37" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0037roxhillsessions20150827.mp3\"&gt;37roxhillsessions20150827.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:7">
       <c r="B38" t="s">
         <v>100</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>100</v>
       </c>
-      <c r="F38" t="str">
+      <c r="G38" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik1-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik1-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:7">
       <c r="B39" t="s">
         <v>94</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>94</v>
       </c>
-      <c r="F39" t="str">
+      <c r="G39" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik10-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik10-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:7">
       <c r="B40" t="s">
         <v>95</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>95</v>
       </c>
-      <c r="F40" t="str">
+      <c r="G40" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik11-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik11-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:7">
       <c r="B41" t="s">
         <v>96</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>96</v>
       </c>
-      <c r="F41" t="str">
+      <c r="G41" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik12-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik12-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:7">
       <c r="B42" t="s">
         <v>97</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>97</v>
       </c>
-      <c r="F42" t="str">
+      <c r="G42" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik13-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik13-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:7">
       <c r="B43" t="s">
         <v>98</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>98</v>
       </c>
-      <c r="F43" t="str">
+      <c r="G43" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik14-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik14-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:7">
       <c r="B44" t="s">
         <v>99</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>99</v>
       </c>
-      <c r="F44" t="str">
+      <c r="G44" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik15-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik15-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
+    <row r="45" spans="2:7">
       <c r="B45" t="s">
         <v>101</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>101</v>
       </c>
-      <c r="F45" t="str">
+      <c r="G45" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik2-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik2-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
+    <row r="46" spans="2:7">
       <c r="B46" t="s">
         <v>102</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>102</v>
       </c>
-      <c r="F46" t="str">
+      <c r="G46" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik3-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik3-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:7">
       <c r="B47" t="s">
         <v>103</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>103</v>
       </c>
-      <c r="F47" t="str">
+      <c r="G47" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik4-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik4-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="2:7">
       <c r="B48" t="s">
         <v>104</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>104</v>
       </c>
-      <c r="F48" t="str">
+      <c r="G48" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik5-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik5-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:7">
       <c r="B49" t="s">
         <v>105</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>105</v>
       </c>
-      <c r="F49" t="str">
+      <c r="G49" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik6-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik6-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:7">
       <c r="B50" t="s">
         <v>106</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>106</v>
       </c>
-      <c r="F50" t="str">
+      <c r="G50" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik7-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik7-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:7">
       <c r="B51" t="s">
         <v>107</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>107</v>
       </c>
-      <c r="F51" t="str">
+      <c r="G51" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik8-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik8-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:7">
       <c r="B52" t="s">
         <v>108</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>108</v>
       </c>
-      <c r="F52" t="str">
+      <c r="G52" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik9-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik9-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:7">
       <c r="B53" t="s">
         <v>77</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>77</v>
       </c>
-      <c r="F53" t="str">
+      <c r="G53" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0001-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:7">
       <c r="B54" t="s">
         <v>78</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>78</v>
       </c>
-      <c r="F54" t="str">
+      <c r="G54" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0002-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:7">
       <c r="B55" t="s">
         <v>79</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>79</v>
       </c>
-      <c r="F55" t="str">
+      <c r="G55" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0003-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:7">
       <c r="B56" t="s">
         <v>80</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>80</v>
       </c>
-      <c r="F56" t="str">
+      <c r="G56" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0004-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:7">
       <c r="B57" t="s">
         <v>81</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>81</v>
       </c>
-      <c r="F57" t="str">
+      <c r="G57" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0005-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:7">
       <c r="B58" t="s">
         <v>82</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>82</v>
       </c>
-      <c r="F58" t="str">
+      <c r="G58" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0006-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:7">
       <c r="B59" t="s">
         <v>83</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>83</v>
       </c>
-      <c r="F59" t="str">
+      <c r="G59" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0007-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:7">
       <c r="B60" t="s">
         <v>84</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>84</v>
       </c>
-      <c r="F60" t="str">
+      <c r="G60" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0008-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:7">
       <c r="B61" t="s">
         <v>85</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>85</v>
       </c>
-      <c r="F61" t="str">
+      <c r="G61" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0009-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" spans="2:7">
       <c r="B62" t="s">
         <v>86</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>86</v>
       </c>
-      <c r="F62" t="str">
+      <c r="G62" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0010-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:7">
       <c r="B63" t="s">
         <v>87</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>87</v>
       </c>
-      <c r="F63" t="str">
+      <c r="G63" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0011-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:7">
       <c r="B64" t="s">
         <v>88</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>88</v>
       </c>
-      <c r="F64" t="str">
+      <c r="G64" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0012-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:7">
       <c r="B65" t="s">
         <v>89</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>89</v>
       </c>
-      <c r="F65" t="str">
+      <c r="G65" t="str">
         <f t="shared" si="0"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0013-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:7">
       <c r="B66" t="s">
         <v>90</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>90</v>
       </c>
-      <c r="F66" t="str">
-        <f t="shared" ref="F66:F69" si="1">$A$1&amp;B66&amp;$C$1&amp;D66&amp;$E$1</f>
+      <c r="G66" t="str">
+        <f t="shared" ref="G66:G101" si="1">$A$1&amp;B66&amp;$C$1&amp;D66&amp;E66&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0014-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:7">
       <c r="B67" t="s">
         <v>91</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>91</v>
       </c>
-      <c r="F67" t="str">
+      <c r="G67" t="str">
         <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0015-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:7">
       <c r="B68" t="s">
         <v>92</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>92</v>
       </c>
-      <c r="F68" t="str">
+      <c r="G68" t="str">
         <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0016-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:7">
       <c r="B69" t="s">
         <v>93</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>93</v>
       </c>
-      <c r="F69" t="str">
+      <c r="G69" t="str">
         <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0017-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
+    <row r="70" spans="2:7">
+      <c r="B70" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" ref="G70:G77" si="2">$A$1&amp;B70&amp;$C$1&amp;D70&amp;E70&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-sufferingfuckheads-coppergate-20130205.mp3\"&gt;01 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-sufferingfuckheads-coppergate-20130205.mp3\"&gt;02 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-sufferingfuckheads-coppergate-20130205.mp3\"&gt;03 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-sufferingfuckheads-coppergate-20130205.mp3\"&gt;04 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" t="s">
+        <v>170</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-sufferingfuckheads-coppergate-20130205.mp3\"&gt;05 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7">
+      <c r="B75" t="s">
+        <v>176</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-sufferingfuckheads-coppergate-20130205.mp3\"&gt;06 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7">
+      <c r="B76" t="s">
+        <v>178</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-sufferingfuckheads-coppergate-20130205.mp3\"&gt;07 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="B77" t="s">
+        <v>182</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0021-sufferingfuckheads-coppergate-20130205.mp3\"&gt;08 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="B78" t="s">
+        <v>143</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3\"&gt;01 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="B79" t="s">
+        <v>146</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3\"&gt;02 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7">
+      <c r="B80" t="s">
+        <v>148</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3\"&gt;03 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3\"&gt;04 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3\"&gt;05 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3\"&gt;06 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3\"&gt;07 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" t="s">
+        <v>180</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3\"&gt;08 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="B86" t="s">
+        <v>185</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3\"&gt;09 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87" t="s">
+        <v>186</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3\"&gt;10 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" t="s">
+        <v>188</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3\"&gt;11 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" t="s">
+        <v>140</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E89" t="s">
+        <v>191</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-sufferingfuckheads-coppergate-20130326.mp3\"&gt;01 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90" t="s">
+        <v>141</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E90" t="s">
+        <v>191</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-sufferingfuckheads-coppergate-20130326.mp3\"&gt;02 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7">
+      <c r="B91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E91" t="s">
+        <v>191</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-sufferingfuckheads-coppergate-20130326.mp3\"&gt;03 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7">
+      <c r="B92" t="s">
+        <v>144</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E92" t="s">
+        <v>191</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-sufferingfuckheads-coppergate-20130326.mp3\"&gt;04 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E93" t="s">
+        <v>191</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-sufferingfuckheads-coppergate-20130326.mp3\"&gt;05 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7">
+      <c r="B94" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E94" t="s">
+        <v>191</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-sufferingfuckheads-coppergate-20130326.mp3\"&gt;06 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7">
+      <c r="B95" t="s">
+        <v>150</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E95" t="s">
+        <v>191</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-sufferingfuckheads-coppergate-20130326.mp3\"&gt;07 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96" t="s">
+        <v>152</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E96" t="s">
+        <v>191</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-sufferingfuckheads-coppergate-20130326.mp3\"&gt;08 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" t="s">
+        <v>154</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E97" t="s">
+        <v>191</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-sufferingfuckheads-coppergate-20130326.mp3\"&gt;09 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7">
+      <c r="B98" t="s">
+        <v>156</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E98" t="s">
+        <v>191</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-sufferingfuckheads-coppergate-20130326.mp3\"&gt;10 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7">
+      <c r="B99" t="s">
+        <v>159</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E99" t="s">
+        <v>191</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-sufferingfuckheads-coppergate-20130326.mp3\"&gt;11 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7">
+      <c r="B100" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E100" t="s">
+        <v>191</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-sufferingfuckheads-coppergate-20130326.mp3\"&gt;12 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7">
+      <c r="B101" t="s">
+        <v>165</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E101" t="s">
+        <v>191</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-sufferingfuckheads-coppergate-20130326.mp3\"&gt;13 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102" t="s">
+        <v>168</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G102" t="str">
+        <f t="shared" ref="G102:G120" si="3">$A$1&amp;B102&amp;$C$1&amp;D102&amp;E102&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-sufferingfuckheads-coppergate-20130423.mp3\"&gt;01 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" t="s">
+        <v>173</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-sufferingfuckheads-coppergate-20130423.mp3\"&gt;02 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" t="s">
+        <v>179</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-sufferingfuckheads-coppergate-20130423.mp3\"&gt;03 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105" t="s">
+        <v>181</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G105" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-sufferingfuckheads-coppergate-20130423.mp3\"&gt;04 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="B106" t="s">
+        <v>183</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G106" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0022-sufferingfuckheads-coppergate-20130423.mp3\"&gt;05 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7">
+      <c r="B107" t="s">
+        <v>184</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0023-sufferingfuckheads-coppergate-20130423.mp3\"&gt;06 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7">
+      <c r="B108" t="s">
+        <v>187</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0025-sufferingfuckheads-coppergate-20130423.mp3\"&gt;07 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7">
+      <c r="B109" t="s">
+        <v>189</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0026-sufferingfuckheads-coppergate-20130423.mp3\"&gt;08 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="B110" t="s">
+        <v>190</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G110" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0028-sufferingfuckheads-coppergate-20130423.mp3\"&gt;09 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7">
+      <c r="B111" t="s">
+        <v>153</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E111" t="s">
+        <v>194</v>
+      </c>
+      <c r="G111" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-sufferingfuckheads-coppergate-20130604.mp3\"&gt;01 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7">
+      <c r="B112" t="s">
+        <v>155</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E112" t="s">
+        <v>194</v>
+      </c>
+      <c r="G112" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-sufferingfuckheads-coppergate-20130604.mp3\"&gt;02 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="B113" t="s">
+        <v>157</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E113" t="s">
+        <v>194</v>
+      </c>
+      <c r="G113" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-sufferingfuckheads-coppergate-20130604.mp3\"&gt;03 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7">
+      <c r="B114" t="s">
+        <v>160</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E114" t="s">
+        <v>194</v>
+      </c>
+      <c r="G114" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-sufferingfuckheads-coppergate-20130604.mp3\"&gt;04 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7">
+      <c r="B115" t="s">
+        <v>163</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E115" t="s">
+        <v>194</v>
+      </c>
+      <c r="G115" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-sufferingfuckheads-coppergate-20130604.mp3\"&gt;05 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7">
+      <c r="B116" t="s">
+        <v>166</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E116" t="s">
+        <v>194</v>
+      </c>
+      <c r="G116" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-sufferingfuckheads-coppergate-20130604.mp3\"&gt;06 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="B117" t="s">
+        <v>169</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E117" t="s">
+        <v>194</v>
+      </c>
+      <c r="G117" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-sufferingfuckheads-coppergate-20130604.mp3\"&gt;07 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" t="s">
+        <v>172</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E118" t="s">
+        <v>194</v>
+      </c>
+      <c r="G118" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-sufferingfuckheads-coppergate-20130604.mp3\"&gt;08 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" t="s">
+        <v>174</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E119" t="s">
+        <v>194</v>
+      </c>
+      <c r="G119" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-sufferingfuckheads-coppergate-20130604.mp3\"&gt;09 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120" t="s">
+        <v>175</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E120" t="s">
+        <v>194</v>
+      </c>
+      <c r="G120" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-sufferingfuckheads-coppergate-20130604.mp3\"&gt;10 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A70:G120">
+    <sortCondition ref="E70:E120"/>
+    <sortCondition ref="B70:B120"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="D71:D120" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1782,7 +2876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3171,14 +4265,129 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="9" width="58" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="str">
+        <f>$A$1&amp;$B$1&amp;C1&amp;$D$1</f>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201302060154a.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="C2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E11" si="0">$A$1&amp;$B$1&amp;C2&amp;$D$1</f>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201302060154b.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201302060154c.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201302131850.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201303272001.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201303272001a.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201303272002a.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201303272002b.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201304252109.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201306071854.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;a href='https://seattleruiles.com'&gt;&lt;img src='http://analogarchive.com/live/suffering201306071854a.JPG'&gt;&lt;/a&gt;&lt;br /&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
put in som bts options
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="46440" windowHeight="24660" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OPTION" sheetId="1" r:id="rId1"/>
     <sheet name="IMG" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="540">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -981,6 +983,666 @@
   </si>
   <si>
     <t>Crack Sabbath - Royal Room - June 22nd, 2024</t>
+  </si>
+  <si>
+    <t>01goingagainstyourmind-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>02inthemorning-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>03theplan-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>04strange-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>05untrustable-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>06else-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>07messwithtime-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>08iwouldhurtafly-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>09getalife-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>10joyride-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>11stab-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>12carrythezero-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>13youwereright-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>14bigdipper-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>15dontfearthereaper-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>16conventionalwisdom-BuiltToSpill-Freemont-20140620.mp3</t>
+  </si>
+  <si>
+    <t>bts-center-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-fly-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-goingagainst-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-inthemorning-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-madeupdreams-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-sidewalk-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-soundcheck-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-theplan-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-untitled-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>bts-youwereright-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_10-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_11-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_12-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_13-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_14-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_15-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_16-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_17-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_18-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_19-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_1-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_2-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_3-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_4-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_5-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_6-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_7-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_8-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl_9-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>Vinyl-zeke-elcorazon-2013.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0001bigbusinessportlandwonderballroom20150907.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0001-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0001-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0002bigbusinessportlandwonderballroom20150907.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0002-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0002-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0003bigbusinessportlandwonderballroom20150907.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0003-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0003-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004bigbusinessportlandwonderballroom20150907.mp3</t>
+  </si>
+  <si>
+    <t>Going</t>
+  </si>
+  <si>
+    <t>Against</t>
+  </si>
+  <si>
+    <t>Your</t>
+  </si>
+  <si>
+    <t>Mind-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>Morning-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>Universe-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Plan-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Planting</t>
+  </si>
+  <si>
+    <t>Seeds-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Kicked</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>Sun-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Life-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Made</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Sidewalk-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Dont</t>
+  </si>
+  <si>
+    <t>Fear</t>
+  </si>
+  <si>
+    <t>Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Pavement-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Goin</t>
+  </si>
+  <si>
+    <t>Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>You</t>
+  </si>
+  <si>
+    <t>were</t>
+  </si>
+  <si>
+    <t>right-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Conventional</t>
+  </si>
+  <si>
+    <t>Wisdom-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Of</t>
+  </si>
+  <si>
+    <t>Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>Martsch-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Carry</t>
+  </si>
+  <si>
+    <t>Zero-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>Instrumental</t>
+  </si>
+  <si>
+    <t>dont</t>
+  </si>
+  <si>
+    <t>know-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>How</t>
+  </si>
+  <si>
+    <t>Soon</t>
+  </si>
+  <si>
+    <t>Is</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>would</t>
+  </si>
+  <si>
+    <t>hurt</t>
+  </si>
+  <si>
+    <t>fly-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Consent</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Order-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Smiths-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Car-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0004-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005bigbusinessportlandwonderballroom20150907.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0005-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0006-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0006-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0007-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0007-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0008-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0008-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0009-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0009-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0010-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0011-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-SkerikTrio-OwlnThistle-20130227.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0012-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0013-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0014-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0015-zeke-highline-20140822.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0038-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0039-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0040-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0041-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0042-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0043-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0044-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0045-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0046-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0047-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0048-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0049-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0050-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0051-lastgasp-highline-2014.mp3</t>
+  </si>
+  <si>
+    <t>01goingagainstyourmind-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>1%20Going%20Against%20Your%20Mind-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>1%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>02inthemorning-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>2%20In%20The%20Morning-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>2%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>3%20Center%20of%20the%20Universe-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>3%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>03theplan-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>04strange-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>4%20The%20Plan-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>5%20Planting%20Seeds-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>5%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>05untrustable-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>06else-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>6%20Kicked%20It%20In%20the%20Sun-BuiltToSpill-LiveatNeumos20131227.mp3%20%20</t>
+  </si>
+  <si>
+    <t>6%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>7%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>7%20Get%20a%20Life-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>07messwithtime-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>08iwouldhurtafly-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>8%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>8%20Sidewalk-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>9%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>09getalife-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>9%20Here%20-%20Pavement-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>10%20Goin%20Against%20Your%20Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>10joyride-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>10%20You%20were%20right-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>11%20Conventional%20Wisdom-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>11%20Kicked%20It%20In%20The%20Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3%20%20</t>
+  </si>
+  <si>
+    <t>11stab-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>12carrythezero-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>12%20Center%20Of%20The%20Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>12%20Heart%20-%20Doug%20Martsch-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>13%20Carry%20the%20Zero-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</t>
+  </si>
+  <si>
+    <t>13%20Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>13youwereright-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>14bigdipper-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>14%20Instrumental%20-%20dont%20know-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</t>
+  </si>
+  <si>
+    <t>14%20Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>15dontfearthereaper-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>15%20How%20Soon%20Is%20Now%20-%20Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3%20</t>
+  </si>
+  <si>
+    <t>15%20I%20would%20hurt%20a%20fly-BuiltToSpill-LiveatNeumos20131227.mp3%20%20</t>
+  </si>
+  <si>
+    <t>16%20Age%20of%20Consent%20-%20New%20Order-BuiltToSpill-LiveatNeumos20131227.mp3%20</t>
+  </si>
+  <si>
+    <t>16conventionalwisdom-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>17%20How%20Soon%20is%20Now%20-%20The%20Smiths-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>18%20Car-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-center-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-fly-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-goingagainst-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-inthemorning-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-madeupdreams-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-sidewalk-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-soundcheck-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-theplan-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-untitled-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
+  </si>
+  <si>
+    <t>bts-youwereright-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1698,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="136">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1115,6 +1777,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1181,7 +1854,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="136">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1278,6 +1951,17 @@
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1648,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="G209" sqref="G209:G220"/>
+    <sheetView topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="B221" sqref="B221:B278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2136,7 +2820,7 @@
         <v>101</v>
       </c>
       <c r="G39" t="str">
-        <f>$A$1&amp;B39&amp;$C$1&amp;D39&amp;E39&amp;$F$1</f>
+        <f t="shared" ref="G39:G46" si="1">$A$1&amp;B39&amp;$C$1&amp;D39&amp;E39&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik2-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik2-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2148,7 +2832,7 @@
         <v>102</v>
       </c>
       <c r="G40" t="str">
-        <f>$A$1&amp;B40&amp;$C$1&amp;D40&amp;E40&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik3-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik3-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2160,7 +2844,7 @@
         <v>103</v>
       </c>
       <c r="G41" t="str">
-        <f>$A$1&amp;B41&amp;$C$1&amp;D41&amp;E41&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik4-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik4-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2172,7 +2856,7 @@
         <v>104</v>
       </c>
       <c r="G42" t="str">
-        <f>$A$1&amp;B42&amp;$C$1&amp;D42&amp;E42&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik5-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik5-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2184,7 +2868,7 @@
         <v>105</v>
       </c>
       <c r="G43" t="str">
-        <f>$A$1&amp;B43&amp;$C$1&amp;D43&amp;E43&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik6-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik6-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2196,7 +2880,7 @@
         <v>106</v>
       </c>
       <c r="G44" t="str">
-        <f>$A$1&amp;B44&amp;$C$1&amp;D44&amp;E44&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik7-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik7-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2208,7 +2892,7 @@
         <v>107</v>
       </c>
       <c r="G45" t="str">
-        <f>$A$1&amp;B45&amp;$C$1&amp;D45&amp;E45&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik8-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik8-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2220,7 +2904,7 @@
         <v>108</v>
       </c>
       <c r="G46" t="str">
-        <f>$A$1&amp;B46&amp;$C$1&amp;D46&amp;E46&amp;$F$1</f>
+        <f t="shared" si="1"/>
         <v>&lt;option value=\"http://analogarchive.com/live/skerik9-SkerikTrio-OwlnThistle-20130206.mp3\"&gt;skerik9-SkerikTrio-OwlnThistle-20130206.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2460,7 +3144,7 @@
         <v>90</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" ref="G66:G101" si="1">$A$1&amp;B66&amp;$C$1&amp;D66&amp;E66&amp;$F$1</f>
+        <f t="shared" ref="G66:G101" si="2">$A$1&amp;B66&amp;$C$1&amp;D66&amp;E66&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0014-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2472,7 +3156,7 @@
         <v>91</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0015-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2484,7 +3168,7 @@
         <v>92</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0016-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2496,7 +3180,7 @@
         <v>93</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-SkerikTrio-OwlnThistle-20130213.mp3\"&gt;ZOOM0017-SkerikTrio-OwlnThistle-20130213.mp3&lt;/option&gt;</v>
       </c>
     </row>
@@ -2511,7 +3195,7 @@
         <v>163</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" ref="G70:G77" si="2">$A$1&amp;B70&amp;$C$1&amp;D70&amp;E70&amp;$F$1</f>
+        <f t="shared" ref="G70:G77" si="3">$A$1&amp;B70&amp;$C$1&amp;D70&amp;E70&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-sufferingfuckheads-coppergate-20130205.mp3\"&gt;01 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2526,7 +3210,7 @@
         <v>163</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-sufferingfuckheads-coppergate-20130205.mp3\"&gt;02 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2541,7 +3225,7 @@
         <v>163</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-sufferingfuckheads-coppergate-20130205.mp3\"&gt;03 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2556,7 +3240,7 @@
         <v>163</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-sufferingfuckheads-coppergate-20130205.mp3\"&gt;04 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2571,7 +3255,7 @@
         <v>163</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-sufferingfuckheads-coppergate-20130205.mp3\"&gt;05 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2586,7 +3270,7 @@
         <v>163</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-sufferingfuckheads-coppergate-20130205.mp3\"&gt;06 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2601,7 +3285,7 @@
         <v>163</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-sufferingfuckheads-coppergate-20130205.mp3\"&gt;07 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2616,7 +3300,7 @@
         <v>163</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0021-sufferingfuckheads-coppergate-20130205.mp3\"&gt;08 Suffering Fuckheads - Coppergate - February 5th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2631,7 +3315,7 @@
         <v>162</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-sufferingfuckheads-coppergate-20130212.mp3\"&gt;01 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2646,7 +3330,7 @@
         <v>162</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-sufferingfuckheads-coppergate-20130212.mp3\"&gt;02 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2661,7 +3345,7 @@
         <v>162</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-sufferingfuckheads-coppergate-20130212.mp3\"&gt;03 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2676,7 +3360,7 @@
         <v>162</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-sufferingfuckheads-coppergate-20130212.mp3\"&gt;04 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2691,7 +3375,7 @@
         <v>162</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-sufferingfuckheads-coppergate-20130212.mp3\"&gt;05 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2706,7 +3390,7 @@
         <v>162</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-sufferingfuckheads-coppergate-20130212.mp3\"&gt;06 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2721,7 +3405,7 @@
         <v>162</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-sufferingfuckheads-coppergate-20130212.mp3\"&gt;07 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2736,7 +3420,7 @@
         <v>162</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-sufferingfuckheads-coppergate-20130212.mp3\"&gt;08 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2751,7 +3435,7 @@
         <v>162</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0024-sufferingfuckheads-coppergate-20130212.mp3\"&gt;09 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2766,7 +3450,7 @@
         <v>162</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0025-sufferingfuckheads-coppergate-20130212.mp3\"&gt;10 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2781,7 +3465,7 @@
         <v>162</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0026-sufferingfuckheads-coppergate-20130212.mp3\"&gt;11 Suffering Fuckheads - Coppergate - February 12th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2796,7 +3480,7 @@
         <v>161</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-sufferingfuckheads-coppergate-20130326.mp3\"&gt;01 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2811,7 +3495,7 @@
         <v>161</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-sufferingfuckheads-coppergate-20130326.mp3\"&gt;02 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2826,7 +3510,7 @@
         <v>161</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-sufferingfuckheads-coppergate-20130326.mp3\"&gt;03 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2841,7 +3525,7 @@
         <v>161</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-sufferingfuckheads-coppergate-20130326.mp3\"&gt;04 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2856,7 +3540,7 @@
         <v>161</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-sufferingfuckheads-coppergate-20130326.mp3\"&gt;05 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2871,7 +3555,7 @@
         <v>161</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-sufferingfuckheads-coppergate-20130326.mp3\"&gt;06 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2886,7 +3570,7 @@
         <v>161</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-sufferingfuckheads-coppergate-20130326.mp3\"&gt;07 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2901,7 +3585,7 @@
         <v>161</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-sufferingfuckheads-coppergate-20130326.mp3\"&gt;08 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2916,7 +3600,7 @@
         <v>161</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-sufferingfuckheads-coppergate-20130326.mp3\"&gt;09 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2931,7 +3615,7 @@
         <v>161</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-sufferingfuckheads-coppergate-20130326.mp3\"&gt;10 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2946,7 +3630,7 @@
         <v>161</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-sufferingfuckheads-coppergate-20130326.mp3\"&gt;11 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2961,7 +3645,7 @@
         <v>161</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-sufferingfuckheads-coppergate-20130326.mp3\"&gt;12 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2976,7 +3660,7 @@
         <v>161</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-sufferingfuckheads-coppergate-20130326.mp3\"&gt;13 Suffering Fuckheads - Coppergate - March 26th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -2991,7 +3675,7 @@
         <v>165</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" ref="G102:G165" si="3">$A$1&amp;B102&amp;$C$1&amp;D102&amp;E102&amp;$F$1</f>
+        <f t="shared" ref="G102:G165" si="4">$A$1&amp;B102&amp;$C$1&amp;D102&amp;E102&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-sufferingfuckheads-coppergate-20130423.mp3\"&gt;01 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3006,7 +3690,7 @@
         <v>165</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-sufferingfuckheads-coppergate-20130423.mp3\"&gt;02 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3021,7 +3705,7 @@
         <v>165</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-sufferingfuckheads-coppergate-20130423.mp3\"&gt;03 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3036,7 +3720,7 @@
         <v>165</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-sufferingfuckheads-coppergate-20130423.mp3\"&gt;04 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3051,7 +3735,7 @@
         <v>165</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0022-sufferingfuckheads-coppergate-20130423.mp3\"&gt;05 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3066,7 +3750,7 @@
         <v>165</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0023-sufferingfuckheads-coppergate-20130423.mp3\"&gt;06 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3081,7 +3765,7 @@
         <v>165</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0025-sufferingfuckheads-coppergate-20130423.mp3\"&gt;07 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3096,7 +3780,7 @@
         <v>165</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0026-sufferingfuckheads-coppergate-20130423.mp3\"&gt;08 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3111,7 +3795,7 @@
         <v>165</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0028-sufferingfuckheads-coppergate-20130423.mp3\"&gt;09 Suffering Fuckheads - Coppergate - April 23rd, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3126,7 +3810,7 @@
         <v>164</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-sufferingfuckheads-coppergate-20130604.mp3\"&gt;01 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3141,7 +3825,7 @@
         <v>164</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-sufferingfuckheads-coppergate-20130604.mp3\"&gt;02 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3156,7 +3840,7 @@
         <v>164</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-sufferingfuckheads-coppergate-20130604.mp3\"&gt;03 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3171,7 +3855,7 @@
         <v>164</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-sufferingfuckheads-coppergate-20130604.mp3\"&gt;04 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3186,7 +3870,7 @@
         <v>164</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-sufferingfuckheads-coppergate-20130604.mp3\"&gt;05 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3201,7 +3885,7 @@
         <v>164</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-sufferingfuckheads-coppergate-20130604.mp3\"&gt;06 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3216,7 +3900,7 @@
         <v>164</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-sufferingfuckheads-coppergate-20130604.mp3\"&gt;07 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3231,7 +3915,7 @@
         <v>164</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-sufferingfuckheads-coppergate-20130604.mp3\"&gt;08 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3246,7 +3930,7 @@
         <v>164</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-sufferingfuckheads-coppergate-20130604.mp3\"&gt;09 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3261,7 +3945,7 @@
         <v>164</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-sufferingfuckheads-coppergate-20130604.mp3\"&gt;10 Suffering Fuckheads - Coppergate - June 4th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -3276,7 +3960,7 @@
         <v>201</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006melvinsportlandwonderballroom20150907.mp3\"&gt;01 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3291,7 +3975,7 @@
         <v>201</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007melvinsportlandwonderballroom20150907.mp3\"&gt;02 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3306,7 +3990,7 @@
         <v>201</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008melvinsportlandwonderballroom20150907.mp3\"&gt;03 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3321,7 +4005,7 @@
         <v>201</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009melvinsportlandwonderballroom20150907.mp3\"&gt;04 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3336,7 +4020,7 @@
         <v>201</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010melvinsportlandwonderballroom20150907.mp3\"&gt;05 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3351,7 +4035,7 @@
         <v>201</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011melvinsportlandwonderballroom20150907.mp3\"&gt;06 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3366,7 +4050,7 @@
         <v>201</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012melvinsportlandwonderballroom20150907.mp3\"&gt;07 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3381,7 +4065,7 @@
         <v>201</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013melvinsportlandwonderballroom20150907.mp3\"&gt;08 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3396,7 +4080,7 @@
         <v>201</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014melvinsportlandwonderballroom20150907.mp3\"&gt;09 Melvins - Wonder Ballroom - Portland - September 7th, 2015&lt;/option&gt;</v>
       </c>
     </row>
@@ -3411,7 +4095,7 @@
         <v>216</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-melvins-showboxmarket-20141018.mp3\"&gt;01 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3426,7 +4110,7 @@
         <v>216</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-melvins-showboxmarket-20141018.mp3\"&gt;02 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3441,7 +4125,7 @@
         <v>216</v>
       </c>
       <c r="G132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-melvins-showboxmarket-20141018.mp3\"&gt;03 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3456,7 +4140,7 @@
         <v>216</v>
       </c>
       <c r="G133" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-melvins-showboxmarket-20141018.mp3\"&gt;04 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3471,7 +4155,7 @@
         <v>216</v>
       </c>
       <c r="G134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-melvins-showboxmarket-20141018.mp3\"&gt;05 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3486,7 +4170,7 @@
         <v>216</v>
       </c>
       <c r="G135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-melvins-showboxmarket-20141018.mp3\"&gt;01 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3501,7 +4185,7 @@
         <v>216</v>
       </c>
       <c r="G136" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-melvins-showboxmarket-20141018.mp3\"&gt;02 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3516,7 +4200,7 @@
         <v>216</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-melvins-showboxmarket-20141018.mp3\"&gt;03 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3531,7 +4215,7 @@
         <v>216</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-melvins-showboxmarket-20141018.mp3\"&gt;04 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3546,7 +4230,7 @@
         <v>216</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-melvins-showboxmarket-20141018.mp3\"&gt;05 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3561,7 +4245,7 @@
         <v>216</v>
       </c>
       <c r="G140" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-melvins-showboxmarket-20141018.mp3\"&gt;06 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3576,7 +4260,7 @@
         <v>216</v>
       </c>
       <c r="G141" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-melvins-showboxmarket-20141018.mp3\"&gt;07 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3591,7 +4275,7 @@
         <v>216</v>
       </c>
       <c r="G142" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-melvins-showboxmarket-20141018.mp3\"&gt;08 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3606,7 +4290,7 @@
         <v>216</v>
       </c>
       <c r="G143" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-melvins-showboxmarket-20141018.mp3\"&gt;09 Melvins - Showbox Market - October 18th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3621,7 +4305,7 @@
         <v>282</v>
       </c>
       <c r="G144" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-01.mp3\"&gt;01 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3636,7 +4320,7 @@
         <v>282</v>
       </c>
       <c r="G145" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-02.mp3\"&gt;02 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3651,7 +4335,7 @@
         <v>282</v>
       </c>
       <c r="G146" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-03.mp3\"&gt;03 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3666,7 +4350,7 @@
         <v>282</v>
       </c>
       <c r="G147" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-04.mp3\"&gt;04 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3681,7 +4365,7 @@
         <v>282</v>
       </c>
       <c r="G148" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-05.mp3\"&gt;05 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3696,7 +4380,7 @@
         <v>282</v>
       </c>
       <c r="G149" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-06.mp3\"&gt;01 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3711,7 +4395,7 @@
         <v>282</v>
       </c>
       <c r="G150" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-07.mp3\"&gt;02 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3726,7 +4410,7 @@
         <v>282</v>
       </c>
       <c r="G151" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-08.mp3\"&gt;03 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3741,7 +4425,7 @@
         <v>282</v>
       </c>
       <c r="G152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-09.mp3\"&gt;04 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3756,7 +4440,7 @@
         <v>282</v>
       </c>
       <c r="G153" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-10.mp3\"&gt;05 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3771,7 +4455,7 @@
         <v>282</v>
       </c>
       <c r="G154" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-11.mp3\"&gt;06 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3786,7 +4470,7 @@
         <v>282</v>
       </c>
       <c r="G155" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-12.mp3\"&gt;07 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3801,7 +4485,7 @@
         <v>282</v>
       </c>
       <c r="G156" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-13.mp3\"&gt;08 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3816,7 +4500,7 @@
         <v>282</v>
       </c>
       <c r="G157" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-14.mp3\"&gt;09 Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3831,7 +4515,7 @@
         <v>282</v>
       </c>
       <c r="G158" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-15.mp3\"&gt;10Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3846,7 +4530,7 @@
         <v>282</v>
       </c>
       <c r="G159" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-16.mp3\"&gt;11Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3861,7 +4545,7 @@
         <v>282</v>
       </c>
       <c r="G160" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-17.mp3\"&gt;12Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3876,7 +4560,7 @@
         <v>282</v>
       </c>
       <c r="G161" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-18.mp3\"&gt;13Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3891,7 +4575,7 @@
         <v>282</v>
       </c>
       <c r="G162" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-19.mp3\"&gt;14Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3906,7 +4590,7 @@
         <v>282</v>
       </c>
       <c r="G163" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-20.mp3\"&gt;15Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3921,7 +4605,7 @@
         <v>282</v>
       </c>
       <c r="G164" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-21.mp3\"&gt;16Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3936,7 +4620,7 @@
         <v>282</v>
       </c>
       <c r="G165" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-22.mp3\"&gt;17Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3951,7 +4635,7 @@
         <v>282</v>
       </c>
       <c r="G166" t="str">
-        <f t="shared" ref="G166:G220" si="4">$A$1&amp;B166&amp;$C$1&amp;D166&amp;E166&amp;$F$1</f>
+        <f t="shared" ref="G166:G220" si="5">$A$1&amp;B166&amp;$C$1&amp;D166&amp;E166&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-23.mp3\"&gt;18Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3966,7 +4650,7 @@
         <v>282</v>
       </c>
       <c r="G167" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-24.mp3\"&gt;19Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3981,7 +4665,7 @@
         <v>282</v>
       </c>
       <c r="G168" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-25.mp3\"&gt;20Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -3996,7 +4680,7 @@
         <v>283</v>
       </c>
       <c r="G169" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-cracksabbath-themix-20130920.mp3\"&gt;01 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4011,7 +4695,7 @@
         <v>283</v>
       </c>
       <c r="G170" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-cracksabbath-themix-20130920.mp3\"&gt;02 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4026,7 +4710,7 @@
         <v>283</v>
       </c>
       <c r="G171" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-cracksabbath-themix-20130920.mp3\"&gt;03 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4041,7 +4725,7 @@
         <v>283</v>
       </c>
       <c r="G172" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-cracksabbath-themix-20130920.mp3\"&gt;04 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4056,7 +4740,7 @@
         <v>283</v>
       </c>
       <c r="G173" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-cracksabbath-themix-20130920.mp3\"&gt;05 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4071,7 +4755,7 @@
         <v>283</v>
       </c>
       <c r="G174" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-cracksabbath-themix-20130920.mp3\"&gt;01 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4086,7 +4770,7 @@
         <v>283</v>
       </c>
       <c r="G175" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-cracksabbath-themix-20130920.mp3\"&gt;02 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4101,7 +4785,7 @@
         <v>283</v>
       </c>
       <c r="G176" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-cracksabbath-themix-20130920.mp3\"&gt;03 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4116,7 +4800,7 @@
         <v>283</v>
       </c>
       <c r="G177" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-cracksabbath-themix-20130920.mp3\"&gt;04 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4131,7 +4815,7 @@
         <v>283</v>
       </c>
       <c r="G178" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-cracksabbath-themix-20130920.mp3\"&gt;05 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4146,7 +4830,7 @@
         <v>283</v>
       </c>
       <c r="G179" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-cracksabbath-themix-20130920.mp3\"&gt;06 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4161,7 +4845,7 @@
         <v>283</v>
       </c>
       <c r="G180" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-cracksabbath-themix-20130920.mp3\"&gt;07 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4176,7 +4860,7 @@
         <v>283</v>
       </c>
       <c r="G181" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-cracksabbath-themix-20130920.mp3\"&gt;08 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4191,7 +4875,7 @@
         <v>283</v>
       </c>
       <c r="G182" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-cracksabbath-themix-20130920.mp3\"&gt;09 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4206,7 +4890,7 @@
         <v>283</v>
       </c>
       <c r="G183" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-cracksabbath-themix-20130920.mp3\"&gt;10Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4221,7 +4905,7 @@
         <v>283</v>
       </c>
       <c r="G184" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-cracksabbath-themix-20130920.mp3\"&gt;11Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4236,7 +4920,7 @@
         <v>283</v>
       </c>
       <c r="G185" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-cracksabbath-themix-20130920.mp3\"&gt;12Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4251,7 +4935,7 @@
         <v>283</v>
       </c>
       <c r="G186" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-cracksabbath-themix-20130920.mp3\"&gt;13Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4266,7 +4950,7 @@
         <v>284</v>
       </c>
       <c r="G187" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-cracksabbath-owlandthistle-20140917.mp3\"&gt;01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4281,7 +4965,7 @@
         <v>284</v>
       </c>
       <c r="G188" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-cracksabbath-owlandthistle-20140917.mp3\"&gt;02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4296,7 +4980,7 @@
         <v>284</v>
       </c>
       <c r="G189" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-cracksabbath-owlandthistle-20140917.mp3\"&gt;03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4311,7 +4995,7 @@
         <v>284</v>
       </c>
       <c r="G190" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-cracksabbath-owlandthistle-20140917.mp3\"&gt;04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4326,7 +5010,7 @@
         <v>284</v>
       </c>
       <c r="G191" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-cracksabbath-owlandthistle-20140917.mp3\"&gt;05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4341,7 +5025,7 @@
         <v>284</v>
       </c>
       <c r="G192" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-cracksabbath-owlandthistle-20140917.mp3\"&gt;01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4356,7 +5040,7 @@
         <v>284</v>
       </c>
       <c r="G193" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-cracksabbath-owlandthistle-20140917.mp3\"&gt;02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4371,7 +5055,7 @@
         <v>284</v>
       </c>
       <c r="G194" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-cracksabbath-owlandthistle-20140917.mp3\"&gt;03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4386,7 +5070,7 @@
         <v>284</v>
       </c>
       <c r="G195" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-cracksabbath-owlandthistle-20140917.mp3\"&gt;04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4401,7 +5085,7 @@
         <v>284</v>
       </c>
       <c r="G196" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-cracksabbath-owlandthistle-20140917.mp3\"&gt;05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4416,7 +5100,7 @@
         <v>284</v>
       </c>
       <c r="G197" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-cracksabbath-owlandthistle-20140917.mp3\"&gt;06 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4431,7 +5115,7 @@
         <v>284</v>
       </c>
       <c r="G198" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-cracksabbath-owlandthistle-20140917.mp3\"&gt;07 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4446,7 +5130,7 @@
         <v>284</v>
       </c>
       <c r="G199" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-cracksabbath-owlandthistle-20140917.mp3\"&gt;08 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4461,7 +5145,7 @@
         <v>284</v>
       </c>
       <c r="G200" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-cracksabbath-owlandthistle-20140917.mp3\"&gt;09 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4476,7 +5160,7 @@
         <v>284</v>
       </c>
       <c r="G201" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-cracksabbath-owlandthistle-20140917.mp3\"&gt;10Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4491,7 +5175,7 @@
         <v>284</v>
       </c>
       <c r="G202" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-cracksabbath-owlandthistle-20140917.mp3\"&gt;11Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4506,7 +5190,7 @@
         <v>284</v>
       </c>
       <c r="G203" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-cracksabbath-owlandthistle-20140917.mp3\"&gt;12Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4521,7 +5205,7 @@
         <v>284</v>
       </c>
       <c r="G204" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-cracksabbath-owlandthistle-20140917.mp3\"&gt;13Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4536,7 +5220,7 @@
         <v>284</v>
       </c>
       <c r="G205" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-cracksabbath-owlandthistle-20140917.mp3\"&gt;14Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4551,7 +5235,7 @@
         <v>284</v>
       </c>
       <c r="G206" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0021-cracksabbath-owlandthistle-20140917.mp3\"&gt;15Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4566,7 +5250,7 @@
         <v>284</v>
       </c>
       <c r="G207" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0022-cracksabbath-owlandthistle-20140917.mp3\"&gt;16Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4581,7 +5265,7 @@
         <v>284</v>
       </c>
       <c r="G208" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0023-cracksabbath-owlandthistle-20140917.mp3\"&gt;17Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4596,7 +5280,7 @@
         <v>308</v>
       </c>
       <c r="G209" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;01 Crack Sabbath - Royal Room - June 22nd, 2013&lt;/option&gt;</v>
       </c>
       <c r="I209" s="4"/>
@@ -4612,7 +5296,7 @@
         <v>309</v>
       </c>
       <c r="G210" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;02 Crack Sabbath - Royal Room - June 22nd, 2014&lt;/option&gt;</v>
       </c>
       <c r="I210" s="4"/>
@@ -4628,7 +5312,7 @@
         <v>310</v>
       </c>
       <c r="G211" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;03 Crack Sabbath - Royal Room - June 22nd, 2015&lt;/option&gt;</v>
       </c>
       <c r="I211" s="4"/>
@@ -4644,7 +5328,7 @@
         <v>311</v>
       </c>
       <c r="G212" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;04 Crack Sabbath - Royal Room - June 22nd, 2016&lt;/option&gt;</v>
       </c>
       <c r="I212" s="4"/>
@@ -4660,7 +5344,7 @@
         <v>312</v>
       </c>
       <c r="G213" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;05 Crack Sabbath - Royal Room - June 22nd, 2017&lt;/option&gt;</v>
       </c>
       <c r="I213" s="4"/>
@@ -4676,7 +5360,7 @@
         <v>313</v>
       </c>
       <c r="G214" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;01 Crack Sabbath - Royal Room - June 22nd, 2018&lt;/option&gt;</v>
       </c>
       <c r="I214" s="4"/>
@@ -4692,7 +5376,7 @@
         <v>314</v>
       </c>
       <c r="G215" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;02 Crack Sabbath - Royal Room - June 22nd, 2019&lt;/option&gt;</v>
       </c>
       <c r="I215" s="4"/>
@@ -4708,7 +5392,7 @@
         <v>315</v>
       </c>
       <c r="G216" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;03 Crack Sabbath - Royal Room - June 22nd, 2020&lt;/option&gt;</v>
       </c>
       <c r="I216" s="4"/>
@@ -4724,7 +5408,7 @@
         <v>316</v>
       </c>
       <c r="G217" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;04 Crack Sabbath - Royal Room - June 22nd, 2021&lt;/option&gt;</v>
       </c>
       <c r="I217" s="4"/>
@@ -4740,7 +5424,7 @@
         <v>317</v>
       </c>
       <c r="G218" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;05 Crack Sabbath - Royal Room - June 22nd, 2022&lt;/option&gt;</v>
       </c>
       <c r="I218" s="4"/>
@@ -4756,7 +5440,7 @@
         <v>318</v>
       </c>
       <c r="G219" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;06 Crack Sabbath - Royal Room - June 22nd, 2023&lt;/option&gt;</v>
       </c>
       <c r="I219" s="4"/>
@@ -4772,7 +5456,7 @@
         <v>319</v>
       </c>
       <c r="G220" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;07 Crack Sabbath - Royal Room - June 22nd, 2024&lt;/option&gt;</v>
       </c>
       <c r="I220" s="4"/>
@@ -4932,20 +5616,1002 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A52:A248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D22"/>
+      <selection activeCell="A51" sqref="A1:M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <sortState ref="A1:A65">
-    <sortCondition ref="A1"/>
+  <sheetData>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:P396">
+    <sortCondition ref="A79"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4955,4 +6621,1174 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I1" t="str">
+        <f>A1&amp;"%20"&amp;B1&amp;"%20"&amp;C1&amp;"%20"&amp;D1&amp;"%20"&amp;E1&amp;"%20"&amp;F1&amp;"%20"&amp;G1&amp;"%20"&amp;H1</f>
+        <v>01goingagainstyourmind-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I58" si="0">A2&amp;"%20"&amp;B2&amp;"%20"&amp;C2&amp;"%20"&amp;D2&amp;"%20"&amp;E2&amp;"%20"&amp;F2&amp;"%20"&amp;G2&amp;"%20"&amp;H2</f>
+        <v>1%20Going%20Against%20Your%20Mind-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>380</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>1%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>321</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>02inthemorning-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" t="s">
+        <v>383</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>2%20In%20The%20Morning-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" t="s">
+        <v>384</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>2%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" t="s">
+        <v>387</v>
+      </c>
+      <c r="E7" t="s">
+        <v>388</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>3%20Center%20of%20the%20Universe-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>3%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>322</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>03theplan-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>323</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>04strange-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" t="s">
+        <v>390</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>4%20The%20Plan-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>391</v>
+      </c>
+      <c r="C12" t="s">
+        <v>392</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>5%20Planting%20Seeds-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>393</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>5%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>324</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>05untrustable-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>325</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>06else-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>394</v>
+      </c>
+      <c r="C16" t="s">
+        <v>395</v>
+      </c>
+      <c r="D16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E16" t="s">
+        <v>387</v>
+      </c>
+      <c r="F16" t="s">
+        <v>396</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>6%20Kicked%20It%20In%20the%20Sun-BuiltToSpill-LiveatNeumos20131227.mp3%20%20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>397</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>6%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>398</v>
+      </c>
+      <c r="C18" t="s">
+        <v>399</v>
+      </c>
+      <c r="D18" t="s">
+        <v>400</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>7%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>398</v>
+      </c>
+      <c r="C19" t="s">
+        <v>399</v>
+      </c>
+      <c r="D19" t="s">
+        <v>401</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>7%20Get%20a%20Life-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>326</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>07messwithtime-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>327</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>08iwouldhurtafly-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>402</v>
+      </c>
+      <c r="C22" t="s">
+        <v>403</v>
+      </c>
+      <c r="D22" t="s">
+        <v>404</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>8%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>405</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>8%20Sidewalk-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>406</v>
+      </c>
+      <c r="C24" t="s">
+        <v>407</v>
+      </c>
+      <c r="D24" t="s">
+        <v>387</v>
+      </c>
+      <c r="E24" t="s">
+        <v>408</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>9%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>328</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>09getalife-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>409</v>
+      </c>
+      <c r="C26" t="s">
+        <v>410</v>
+      </c>
+      <c r="D26" t="s">
+        <v>411</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>9%20Here%20-%20Pavement-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>412</v>
+      </c>
+      <c r="C27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E27" t="s">
+        <v>413</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>10%20Goin%20Against%20Your%20Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>329</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>10joyride-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>414</v>
+      </c>
+      <c r="C29" t="s">
+        <v>415</v>
+      </c>
+      <c r="D29" t="s">
+        <v>416</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>10%20You%20were%20right-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C30" t="s">
+        <v>418</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>11%20Conventional%20Wisdom-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>394</v>
+      </c>
+      <c r="C31" t="s">
+        <v>395</v>
+      </c>
+      <c r="D31" t="s">
+        <v>381</v>
+      </c>
+      <c r="E31" t="s">
+        <v>382</v>
+      </c>
+      <c r="F31" t="s">
+        <v>419</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>11%20Kicked%20It%20In%20The%20Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3%20%20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>330</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>11stab-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>331</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>12carrythezero-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>385</v>
+      </c>
+      <c r="C34" t="s">
+        <v>420</v>
+      </c>
+      <c r="D34" t="s">
+        <v>382</v>
+      </c>
+      <c r="E34" t="s">
+        <v>421</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>12%20Center%20Of%20The%20Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>422</v>
+      </c>
+      <c r="C35" t="s">
+        <v>410</v>
+      </c>
+      <c r="D35" t="s">
+        <v>423</v>
+      </c>
+      <c r="E35" t="s">
+        <v>424</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>12%20Heart%20-%20Doug%20Martsch-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>425</v>
+      </c>
+      <c r="C36" t="s">
+        <v>387</v>
+      </c>
+      <c r="D36" t="s">
+        <v>426</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>13%20Carry%20the%20Zero-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>427</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>13%20Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>13youwereright-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>333</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>14bigdipper-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>428</v>
+      </c>
+      <c r="C40" t="s">
+        <v>410</v>
+      </c>
+      <c r="D40" t="s">
+        <v>429</v>
+      </c>
+      <c r="E40" t="s">
+        <v>430</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>14%20Instrumental%20-%20dont%20know-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>431</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>14%20Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>334</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>15dontfearthereaper-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>432</v>
+      </c>
+      <c r="C43" t="s">
+        <v>433</v>
+      </c>
+      <c r="D43" t="s">
+        <v>434</v>
+      </c>
+      <c r="E43" t="s">
+        <v>435</v>
+      </c>
+      <c r="F43" t="s">
+        <v>410</v>
+      </c>
+      <c r="G43" t="s">
+        <v>436</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>15%20How%20Soon%20Is%20Now%20-%20Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3%20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>437</v>
+      </c>
+      <c r="C44" t="s">
+        <v>438</v>
+      </c>
+      <c r="D44" t="s">
+        <v>439</v>
+      </c>
+      <c r="E44" t="s">
+        <v>399</v>
+      </c>
+      <c r="F44" t="s">
+        <v>440</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>15%20I%20would%20hurt%20a%20fly-BuiltToSpill-LiveatNeumos20131227.mp3%20%20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>441</v>
+      </c>
+      <c r="C45" t="s">
+        <v>386</v>
+      </c>
+      <c r="D45" t="s">
+        <v>442</v>
+      </c>
+      <c r="E45" t="s">
+        <v>410</v>
+      </c>
+      <c r="F45" t="s">
+        <v>443</v>
+      </c>
+      <c r="G45" t="s">
+        <v>444</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>16%20Age%20of%20Consent%20-%20New%20Order-BuiltToSpill-LiveatNeumos20131227.mp3%20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>335</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>16conventionalwisdom-BuiltToSpill-Freemont-20140620.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>432</v>
+      </c>
+      <c r="C47" t="s">
+        <v>433</v>
+      </c>
+      <c r="D47" t="s">
+        <v>445</v>
+      </c>
+      <c r="E47" t="s">
+        <v>435</v>
+      </c>
+      <c r="F47" t="s">
+        <v>410</v>
+      </c>
+      <c r="G47" t="s">
+        <v>382</v>
+      </c>
+      <c r="H47" t="s">
+        <v>446</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>17%20How%20Soon%20is%20Now%20-%20The%20Smiths-BuiltToSpill-LiveatNeumos20131227.mp3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>447</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>18%20Car-BuiltToSpill-LiveatNeumos20131227.mp3%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>336</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-center-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>337</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-fly-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>338</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-goingagainst-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>339</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-inthemorning-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>340</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-madeupdreams-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>341</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-sidewalk-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>342</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-soundcheck-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>343</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-theplan-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>344</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-untitled-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>345</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="0"/>
+        <v>bts-youwereright-BuiltToSpill-Geogetown-20130713.mp3%20%20%20%20%20%20%20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="I59" t="str">
+        <f t="shared" ref="I2:I59" si="1">A59&amp;" "&amp;B59&amp;" "&amp;C59&amp;" "&amp;D59&amp;" "&amp;E59&amp;" "&amp;F59&amp;" "&amp;G59&amp;" "&amp;H59</f>
+        <v xml:space="preserve">       </v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="106" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>539</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding video player and making sure it works with some options
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="OPTION" sheetId="1" r:id="rId1"/>
-    <sheet name="IMG" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="OPTIONaudio" sheetId="1" r:id="rId1"/>
+    <sheet name="OPTIONvideo" sheetId="7" r:id="rId2"/>
+    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId3"/>
+    <sheet name="IMG" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
+    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId6"/>
+    <sheet name="built to spill" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="550">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -1565,6 +1567,114 @@
   </si>
   <si>
     <t>16%20Age%20of%20Consent%20-%20New%20Order-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>Sk8creteordie over the light at Marginal</t>
+  </si>
+  <si>
+    <t>WXPFL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02</t>
+  </si>
+  <si>
+    <t>Kayla Cheering</t>
+  </si>
+  <si>
+    <t>&lt;option value=\"http://seattlerules.com/media/</t>
+  </si>
+  <si>
+    <t>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/</t>
+  </si>
+  <si>
+    <t>sk8crete201408131923451.mp4</t>
+  </si>
+  <si>
+    <t>sk8crete201408131950341.mp4</t>
+  </si>
+  <si>
+    <t>sk8crete201408131952541.mp4</t>
+  </si>
+  <si>
+    <t>sk8crete201408131956261.mp4</t>
+  </si>
+  <si>
+    <t>sk8crete201408132002401.mp4</t>
+  </si>
+  <si>
+    <t>sk8crete201408132012071.mp4</t>
+  </si>
+  <si>
+    <t>sk8crete201408142156021.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0098.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0101.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0103.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0106.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0109.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0113.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0116.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0117.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0119.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0120.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/IMG_0127.mp4</t>
+  </si>
+  <si>
+    <t>wxpfl/wxpfl-greenwood-201411.mp4</t>
+  </si>
+  <si>
+    <t>kaylacheering/kayla_cheerleading_20150215.mp4</t>
+  </si>
+  <si>
+    <t>kaylacheering/kayla_cheerleading_20150215b.mp4</t>
+  </si>
+  <si>
+    <t>marginal/jim-marginal-overthelight-march2015.mp4</t>
+  </si>
+  <si>
+    <t>Sk8creteordie cellphoto</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1730,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1699,6 +1809,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1776,7 +1899,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="160">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1884,6 +2007,19 @@
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2252,14 +2388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I220"/>
+  <dimension ref="A1:I235"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221:B278"/>
+    <sheetView topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="B221" sqref="B221:F235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
     <col min="2" max="2" width="53.1640625" customWidth="1"/>
     <col min="3" max="3" width="2.5" customWidth="1"/>
     <col min="4" max="4" width="3.1640625" customWidth="1"/>
@@ -4557,7 +4694,7 @@
         <v>282</v>
       </c>
       <c r="G166" t="str">
-        <f t="shared" ref="G166:G220" si="5">$A$1&amp;B166&amp;$C$1&amp;D166&amp;E166&amp;$F$1</f>
+        <f>$A$1&amp;B166&amp;$C$1&amp;D166&amp;E166&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-23.mp3\"&gt;18Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4572,7 +4709,7 @@
         <v>282</v>
       </c>
       <c r="G167" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B167&amp;$C$1&amp;D167&amp;E167&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-24.mp3\"&gt;19Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4587,7 +4724,7 @@
         <v>282</v>
       </c>
       <c r="G168" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B168&amp;$C$1&amp;D168&amp;E168&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-25.mp3\"&gt;20Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4602,7 +4739,7 @@
         <v>283</v>
       </c>
       <c r="G169" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B169&amp;$C$1&amp;D169&amp;E169&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-cracksabbath-themix-20130920.mp3\"&gt;01 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4617,7 +4754,7 @@
         <v>283</v>
       </c>
       <c r="G170" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B170&amp;$C$1&amp;D170&amp;E170&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-cracksabbath-themix-20130920.mp3\"&gt;02 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4632,7 +4769,7 @@
         <v>283</v>
       </c>
       <c r="G171" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B171&amp;$C$1&amp;D171&amp;E171&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-cracksabbath-themix-20130920.mp3\"&gt;03 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4647,7 +4784,7 @@
         <v>283</v>
       </c>
       <c r="G172" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B172&amp;$C$1&amp;D172&amp;E172&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-cracksabbath-themix-20130920.mp3\"&gt;04 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4662,7 +4799,7 @@
         <v>283</v>
       </c>
       <c r="G173" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B173&amp;$C$1&amp;D173&amp;E173&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-cracksabbath-themix-20130920.mp3\"&gt;05 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4677,7 +4814,7 @@
         <v>283</v>
       </c>
       <c r="G174" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B174&amp;$C$1&amp;D174&amp;E174&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-cracksabbath-themix-20130920.mp3\"&gt;01 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4692,7 +4829,7 @@
         <v>283</v>
       </c>
       <c r="G175" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B175&amp;$C$1&amp;D175&amp;E175&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-cracksabbath-themix-20130920.mp3\"&gt;02 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4707,7 +4844,7 @@
         <v>283</v>
       </c>
       <c r="G176" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B176&amp;$C$1&amp;D176&amp;E176&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-cracksabbath-themix-20130920.mp3\"&gt;03 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4722,7 +4859,7 @@
         <v>283</v>
       </c>
       <c r="G177" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B177&amp;$C$1&amp;D177&amp;E177&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-cracksabbath-themix-20130920.mp3\"&gt;04 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4737,7 +4874,7 @@
         <v>283</v>
       </c>
       <c r="G178" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B178&amp;$C$1&amp;D178&amp;E178&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-cracksabbath-themix-20130920.mp3\"&gt;05 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4752,7 +4889,7 @@
         <v>283</v>
       </c>
       <c r="G179" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B179&amp;$C$1&amp;D179&amp;E179&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-cracksabbath-themix-20130920.mp3\"&gt;06 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4767,7 +4904,7 @@
         <v>283</v>
       </c>
       <c r="G180" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B180&amp;$C$1&amp;D180&amp;E180&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-cracksabbath-themix-20130920.mp3\"&gt;07 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4782,7 +4919,7 @@
         <v>283</v>
       </c>
       <c r="G181" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B181&amp;$C$1&amp;D181&amp;E181&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-cracksabbath-themix-20130920.mp3\"&gt;08 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4797,7 +4934,7 @@
         <v>283</v>
       </c>
       <c r="G182" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B182&amp;$C$1&amp;D182&amp;E182&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-cracksabbath-themix-20130920.mp3\"&gt;09 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4812,7 +4949,7 @@
         <v>283</v>
       </c>
       <c r="G183" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B183&amp;$C$1&amp;D183&amp;E183&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-cracksabbath-themix-20130920.mp3\"&gt;10Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4827,7 +4964,7 @@
         <v>283</v>
       </c>
       <c r="G184" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B184&amp;$C$1&amp;D184&amp;E184&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-cracksabbath-themix-20130920.mp3\"&gt;11Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4842,7 +4979,7 @@
         <v>283</v>
       </c>
       <c r="G185" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B185&amp;$C$1&amp;D185&amp;E185&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-cracksabbath-themix-20130920.mp3\"&gt;12Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4857,7 +4994,7 @@
         <v>283</v>
       </c>
       <c r="G186" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B186&amp;$C$1&amp;D186&amp;E186&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-cracksabbath-themix-20130920.mp3\"&gt;13Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4872,7 +5009,7 @@
         <v>284</v>
       </c>
       <c r="G187" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B187&amp;$C$1&amp;D187&amp;E187&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-cracksabbath-owlandthistle-20140917.mp3\"&gt;01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4887,7 +5024,7 @@
         <v>284</v>
       </c>
       <c r="G188" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B188&amp;$C$1&amp;D188&amp;E188&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-cracksabbath-owlandthistle-20140917.mp3\"&gt;02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4902,7 +5039,7 @@
         <v>284</v>
       </c>
       <c r="G189" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B189&amp;$C$1&amp;D189&amp;E189&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-cracksabbath-owlandthistle-20140917.mp3\"&gt;03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4917,7 +5054,7 @@
         <v>284</v>
       </c>
       <c r="G190" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B190&amp;$C$1&amp;D190&amp;E190&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-cracksabbath-owlandthistle-20140917.mp3\"&gt;04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4932,7 +5069,7 @@
         <v>284</v>
       </c>
       <c r="G191" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B191&amp;$C$1&amp;D191&amp;E191&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-cracksabbath-owlandthistle-20140917.mp3\"&gt;05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4947,7 +5084,7 @@
         <v>284</v>
       </c>
       <c r="G192" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B192&amp;$C$1&amp;D192&amp;E192&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-cracksabbath-owlandthistle-20140917.mp3\"&gt;01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4962,7 +5099,7 @@
         <v>284</v>
       </c>
       <c r="G193" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B193&amp;$C$1&amp;D193&amp;E193&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-cracksabbath-owlandthistle-20140917.mp3\"&gt;02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4977,7 +5114,7 @@
         <v>284</v>
       </c>
       <c r="G194" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B194&amp;$C$1&amp;D194&amp;E194&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-cracksabbath-owlandthistle-20140917.mp3\"&gt;03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4992,7 +5129,7 @@
         <v>284</v>
       </c>
       <c r="G195" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B195&amp;$C$1&amp;D195&amp;E195&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-cracksabbath-owlandthistle-20140917.mp3\"&gt;04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5007,7 +5144,7 @@
         <v>284</v>
       </c>
       <c r="G196" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B196&amp;$C$1&amp;D196&amp;E196&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-cracksabbath-owlandthistle-20140917.mp3\"&gt;05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5022,7 +5159,7 @@
         <v>284</v>
       </c>
       <c r="G197" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B197&amp;$C$1&amp;D197&amp;E197&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-cracksabbath-owlandthistle-20140917.mp3\"&gt;06 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5037,7 +5174,7 @@
         <v>284</v>
       </c>
       <c r="G198" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B198&amp;$C$1&amp;D198&amp;E198&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-cracksabbath-owlandthistle-20140917.mp3\"&gt;07 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5052,7 +5189,7 @@
         <v>284</v>
       </c>
       <c r="G199" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B199&amp;$C$1&amp;D199&amp;E199&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-cracksabbath-owlandthistle-20140917.mp3\"&gt;08 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5067,7 +5204,7 @@
         <v>284</v>
       </c>
       <c r="G200" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B200&amp;$C$1&amp;D200&amp;E200&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-cracksabbath-owlandthistle-20140917.mp3\"&gt;09 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5082,7 +5219,7 @@
         <v>284</v>
       </c>
       <c r="G201" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B201&amp;$C$1&amp;D201&amp;E201&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-cracksabbath-owlandthistle-20140917.mp3\"&gt;10Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5097,7 +5234,7 @@
         <v>284</v>
       </c>
       <c r="G202" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B202&amp;$C$1&amp;D202&amp;E202&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-cracksabbath-owlandthistle-20140917.mp3\"&gt;11Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5112,7 +5249,7 @@
         <v>284</v>
       </c>
       <c r="G203" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B203&amp;$C$1&amp;D203&amp;E203&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-cracksabbath-owlandthistle-20140917.mp3\"&gt;12Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5127,7 +5264,7 @@
         <v>284</v>
       </c>
       <c r="G204" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B204&amp;$C$1&amp;D204&amp;E204&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-cracksabbath-owlandthistle-20140917.mp3\"&gt;13Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5142,7 +5279,7 @@
         <v>284</v>
       </c>
       <c r="G205" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B205&amp;$C$1&amp;D205&amp;E205&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-cracksabbath-owlandthistle-20140917.mp3\"&gt;14Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5157,7 +5294,7 @@
         <v>284</v>
       </c>
       <c r="G206" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B206&amp;$C$1&amp;D206&amp;E206&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0021-cracksabbath-owlandthistle-20140917.mp3\"&gt;15Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5172,7 +5309,7 @@
         <v>284</v>
       </c>
       <c r="G207" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B207&amp;$C$1&amp;D207&amp;E207&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0022-cracksabbath-owlandthistle-20140917.mp3\"&gt;16Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5187,7 +5324,7 @@
         <v>284</v>
       </c>
       <c r="G208" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B208&amp;$C$1&amp;D208&amp;E208&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0023-cracksabbath-owlandthistle-20140917.mp3\"&gt;17Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5202,7 +5339,7 @@
         <v>308</v>
       </c>
       <c r="G209" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B209&amp;$C$1&amp;D209&amp;E209&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;01 Crack Sabbath - Royal Room - June 22nd, 2013&lt;/option&gt;</v>
       </c>
       <c r="I209" s="4"/>
@@ -5218,7 +5355,7 @@
         <v>309</v>
       </c>
       <c r="G210" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B210&amp;$C$1&amp;D210&amp;E210&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;02 Crack Sabbath - Royal Room - June 22nd, 2014&lt;/option&gt;</v>
       </c>
       <c r="I210" s="4"/>
@@ -5234,7 +5371,7 @@
         <v>310</v>
       </c>
       <c r="G211" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B211&amp;$C$1&amp;D211&amp;E211&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;03 Crack Sabbath - Royal Room - June 22nd, 2015&lt;/option&gt;</v>
       </c>
       <c r="I211" s="4"/>
@@ -5250,7 +5387,7 @@
         <v>311</v>
       </c>
       <c r="G212" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B212&amp;$C$1&amp;D212&amp;E212&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;04 Crack Sabbath - Royal Room - June 22nd, 2016&lt;/option&gt;</v>
       </c>
       <c r="I212" s="4"/>
@@ -5266,7 +5403,7 @@
         <v>312</v>
       </c>
       <c r="G213" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B213&amp;$C$1&amp;D213&amp;E213&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;05 Crack Sabbath - Royal Room - June 22nd, 2017&lt;/option&gt;</v>
       </c>
       <c r="I213" s="4"/>
@@ -5282,7 +5419,7 @@
         <v>313</v>
       </c>
       <c r="G214" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B214&amp;$C$1&amp;D214&amp;E214&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;01 Crack Sabbath - Royal Room - June 22nd, 2018&lt;/option&gt;</v>
       </c>
       <c r="I214" s="4"/>
@@ -5298,7 +5435,7 @@
         <v>314</v>
       </c>
       <c r="G215" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B215&amp;$C$1&amp;D215&amp;E215&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;02 Crack Sabbath - Royal Room - June 22nd, 2019&lt;/option&gt;</v>
       </c>
       <c r="I215" s="4"/>
@@ -5314,7 +5451,7 @@
         <v>315</v>
       </c>
       <c r="G216" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B216&amp;$C$1&amp;D216&amp;E216&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;03 Crack Sabbath - Royal Room - June 22nd, 2020&lt;/option&gt;</v>
       </c>
       <c r="I216" s="4"/>
@@ -5330,7 +5467,7 @@
         <v>316</v>
       </c>
       <c r="G217" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B217&amp;$C$1&amp;D217&amp;E217&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;04 Crack Sabbath - Royal Room - June 22nd, 2021&lt;/option&gt;</v>
       </c>
       <c r="I217" s="4"/>
@@ -5346,7 +5483,7 @@
         <v>317</v>
       </c>
       <c r="G218" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B218&amp;$C$1&amp;D218&amp;E218&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;05 Crack Sabbath - Royal Room - June 22nd, 2022&lt;/option&gt;</v>
       </c>
       <c r="I218" s="4"/>
@@ -5362,7 +5499,7 @@
         <v>318</v>
       </c>
       <c r="G219" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B219&amp;$C$1&amp;D219&amp;E219&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;06 Crack Sabbath - Royal Room - June 22nd, 2023&lt;/option&gt;</v>
       </c>
       <c r="I219" s="4"/>
@@ -5378,10 +5515,100 @@
         <v>319</v>
       </c>
       <c r="G220" t="str">
-        <f t="shared" si="5"/>
+        <f>$A$1&amp;B220&amp;$C$1&amp;D220&amp;E220&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;07 Crack Sabbath - Royal Room - June 22nd, 2024&lt;/option&gt;</v>
       </c>
       <c r="I220" s="4"/>
+    </row>
+    <row r="221" spans="2:9">
+      <c r="G221" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B2&amp;$C$1&amp;'OPTIONvideo (2)'!D2&amp;'OPTIONvideo (2)'!E2&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/marginal/jim-marginal-overthelight-march2015.mp4\"&gt;Sk8creteordie over the light at Marginal&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="222" spans="2:9">
+      <c r="G222" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B3&amp;$C$1&amp;'OPTIONvideo (2)'!D3&amp;'OPTIONvideo (2)'!E3&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0098.mp4\"&gt;01 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9">
+      <c r="G223" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B4&amp;$C$1&amp;'OPTIONvideo (2)'!D4&amp;'OPTIONvideo (2)'!E4&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0101.mp4\"&gt;02 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="224" spans="2:9">
+      <c r="G224" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B5&amp;$C$1&amp;'OPTIONvideo (2)'!D5&amp;'OPTIONvideo (2)'!E5&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0103.mp4\"&gt;03 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="225" spans="7:7">
+      <c r="G225" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B6&amp;$C$1&amp;'OPTIONvideo (2)'!D6&amp;'OPTIONvideo (2)'!E6&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0106.mp4\"&gt;04 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7">
+      <c r="G226" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B7&amp;$C$1&amp;'OPTIONvideo (2)'!D7&amp;'OPTIONvideo (2)'!E7&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0109.mp4\"&gt;05 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="227" spans="7:7">
+      <c r="G227" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B8&amp;$C$1&amp;'OPTIONvideo (2)'!D8&amp;'OPTIONvideo (2)'!E8&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0113.mp4\"&gt;01 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7">
+      <c r="G228" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B9&amp;$C$1&amp;'OPTIONvideo (2)'!D9&amp;'OPTIONvideo (2)'!E9&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0116.mp4\"&gt;02 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="229" spans="7:7">
+      <c r="G229" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B10&amp;$C$1&amp;'OPTIONvideo (2)'!D10&amp;'OPTIONvideo (2)'!E10&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0117.mp4\"&gt;03 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7">
+      <c r="G230" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B11&amp;$C$1&amp;'OPTIONvideo (2)'!D11&amp;'OPTIONvideo (2)'!E11&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0119.mp4\"&gt;04 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="231" spans="7:7">
+      <c r="G231" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B12&amp;$C$1&amp;'OPTIONvideo (2)'!D12&amp;'OPTIONvideo (2)'!E12&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0120.mp4\"&gt;05 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7">
+      <c r="G232" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B13&amp;$C$1&amp;'OPTIONvideo (2)'!D13&amp;'OPTIONvideo (2)'!E13&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0127.mp4\"&gt;06 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="233" spans="7:7">
+      <c r="G233" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B14&amp;$C$1&amp;'OPTIONvideo (2)'!D14&amp;'OPTIONvideo (2)'!E14&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/wxpfl-greenwood-201411.mp4\"&gt;07 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7">
+      <c r="G234" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B15&amp;$C$1&amp;'OPTIONvideo (2)'!D15&amp;'OPTIONvideo (2)'!E15&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/kaylacheering/kayla_cheerleading_20150215.mp4\"&gt;01 Kayla Cheering&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="235" spans="7:7">
+      <c r="G235" t="str">
+        <f>$A$1&amp;'OPTIONvideo (2)'!B16&amp;$C$1&amp;'OPTIONvideo (2)'!D16&amp;'OPTIONvideo (2)'!E16&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/kaylacheering/kayla_cheerleading_20150215b.mp4\"&gt; 02Kayla Cheering&lt;/option&gt;</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A70:G120">
@@ -5392,6 +5619,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="D71:D120" numberStoredAsText="1"/>
+    <ignoredError sqref="G221" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5402,6 +5630,417 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="str">
+        <f>$A$1&amp;B1&amp;$C$1&amp;D1&amp;E1&amp;$F$1</f>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/ZOOM0001roxhillsessions20150827.mp3\"&gt;&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E2" t="s">
+        <v>542</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G8" si="0">$A$1&amp;B2&amp;$C$1&amp;D2&amp;E2&amp;$F$1</f>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131923451.mp4\"&gt;01Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>521</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E3" t="s">
+        <v>542</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131950341.mp4\"&gt;02Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>522</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E4" t="s">
+        <v>542</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131952541.mp4\"&gt;03Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>523</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E5" t="s">
+        <v>542</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131956261.mp4\"&gt;04Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>524</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="E6" t="s">
+        <v>542</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408132002401.mp4\"&gt;05Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>525</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E7" t="s">
+        <v>542</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408132012071.mp4\"&gt;06Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>526</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E8" t="s">
+        <v>542</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408142156021.mp4\"&gt;07Sk8creteordie cellphoto&lt;/option&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="str">
+        <f>$A$1&amp;B1&amp;$C$1&amp;D1&amp;E1&amp;$F$1</f>
+        <v>&lt;option value=\"http://seattlerules.com/media/\"&gt;&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>541</v>
+      </c>
+      <c r="E2" t="s">
+        <v>514</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G16" si="0">$A$1&amp;B2&amp;$C$1&amp;D2&amp;E2&amp;$F$1</f>
+        <v>&lt;option value=\"http://seattlerules.com/media/marginal/jim-marginal-overthelight-march2015.mp4\"&gt;Sk8creteordie over the light at Marginal&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>527</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" t="s">
+        <v>515</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0098.mp4\"&gt;01 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>528</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" t="s">
+        <v>515</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0101.mp4\"&gt;02 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" t="s">
+        <v>515</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0103.mp4\"&gt;03 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>530</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" t="s">
+        <v>515</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0106.mp4\"&gt;04 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>531</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
+        <v>515</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0109.mp4\"&gt;05 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>532</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" t="s">
+        <v>515</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0113.mp4\"&gt;01 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>533</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" t="s">
+        <v>515</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0116.mp4\"&gt;02 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>534</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0117.mp4\"&gt;03 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
+        <v>535</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0119.mp4\"&gt;04 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>536</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0120.mp4\"&gt;05 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>537</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/IMG_0127.mp4\"&gt;06 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" t="s">
+        <v>538</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/wxpfl/wxpfl-greenwood-201411.mp4\"&gt;07 WXPFL&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" t="s">
+        <v>539</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/kaylacheering/kayla_cheerleading_20150215.mp4\"&gt;01 Kayla Cheering&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>540</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;option value=\"http://seattlerules.com/media/kaylacheering/kayla_cheerleading_20150215b.mp4\"&gt; 02Kayla Cheering&lt;/option&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -5536,7 +6175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A52:A248"/>
   <sheetViews>
@@ -6545,7 +7184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
@@ -7402,11 +8041,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed size of links on home page
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="544">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -1656,25 +1656,7 @@
     <t>Sk8creteordie cellphoto</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
+    <t xml:space="preserve">06  </t>
   </si>
 </sst>
 </file>
@@ -1730,7 +1712,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="160">
+  <cellStyleXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1809,6 +1791,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1899,7 +1883,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="160">
+  <cellStyles count="162">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2020,6 +2004,8 @@
     <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5634,7 +5620,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="G2" sqref="G2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5666,14 +5652,14 @@
         <v>520</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>543</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
         <v>542</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G8" si="0">$A$1&amp;B2&amp;$C$1&amp;D2&amp;E2&amp;$F$1</f>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131923451.mp4\"&gt;01Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131923451.mp4\"&gt;01 Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5681,14 +5667,14 @@
         <v>521</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>544</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
         <v>542</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131950341.mp4\"&gt;02Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131950341.mp4\"&gt;02 Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5696,14 +5682,14 @@
         <v>522</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>545</v>
+        <v>168</v>
       </c>
       <c r="E4" t="s">
         <v>542</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131952541.mp4\"&gt;03Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131952541.mp4\"&gt;03 Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5711,14 +5697,14 @@
         <v>523</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>546</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
         <v>542</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131956261.mp4\"&gt;04Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408131956261.mp4\"&gt;04 Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5726,14 +5712,14 @@
         <v>524</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>547</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s">
         <v>542</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408132002401.mp4\"&gt;05Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408132002401.mp4\"&gt;05 Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5741,14 +5727,14 @@
         <v>525</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="E7" t="s">
         <v>542</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408132012071.mp4\"&gt;06Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408132012071.mp4\"&gt;06  Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5756,14 +5742,14 @@
         <v>526</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>549</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
         <v>542</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408142156021.mp4\"&gt;07Sk8creteordie cellphoto&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://seattlerules.com/cellphoto/cellphoto/sk8crete201408142156021.mp4\"&gt;07 Sk8creteordie cellphoto&lt;/option&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added built to spill
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="760"/>
   </bookViews>
   <sheets>
     <sheet name="OPTIONaudio" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="561">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -1657,6 +1657,57 @@
   </si>
   <si>
     <t xml:space="preserve">06  </t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1763,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="162">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1791,6 +1842,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1883,7 +1939,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="162">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2006,6 +2062,11 @@
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2374,20 +2435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I235"/>
+  <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221:F235"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="G227" sqref="G227:G278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" customWidth="1"/>
-    <col min="2" max="2" width="53.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="91.5" customWidth="1"/>
     <col min="3" max="3" width="2.5" customWidth="1"/>
     <col min="4" max="4" width="3.1640625" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
     <col min="8" max="8" width="78.1640625" customWidth="1"/>
   </cols>
@@ -4680,7 +4741,7 @@
         <v>282</v>
       </c>
       <c r="G166" t="str">
-        <f>$A$1&amp;B166&amp;$C$1&amp;D166&amp;E166&amp;$F$1</f>
+        <f t="shared" ref="G166:G197" si="5">$A$1&amp;B166&amp;$C$1&amp;D166&amp;E166&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-23.mp3\"&gt;18Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4695,7 +4756,7 @@
         <v>282</v>
       </c>
       <c r="G167" t="str">
-        <f>$A$1&amp;B167&amp;$C$1&amp;D167&amp;E167&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-24.mp3\"&gt;19Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4710,7 +4771,7 @@
         <v>282</v>
       </c>
       <c r="G168" t="str">
-        <f>$A$1&amp;B168&amp;$C$1&amp;D168&amp;E168&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/cracksabbath20140509-25.mp3\"&gt;20Crack Sabbath - Darrell's - May 8th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -4725,7 +4786,7 @@
         <v>283</v>
       </c>
       <c r="G169" t="str">
-        <f>$A$1&amp;B169&amp;$C$1&amp;D169&amp;E169&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-cracksabbath-themix-20130920.mp3\"&gt;01 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4740,7 +4801,7 @@
         <v>283</v>
       </c>
       <c r="G170" t="str">
-        <f>$A$1&amp;B170&amp;$C$1&amp;D170&amp;E170&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-cracksabbath-themix-20130920.mp3\"&gt;02 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4755,7 +4816,7 @@
         <v>283</v>
       </c>
       <c r="G171" t="str">
-        <f>$A$1&amp;B171&amp;$C$1&amp;D171&amp;E171&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-cracksabbath-themix-20130920.mp3\"&gt;03 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4770,7 +4831,7 @@
         <v>283</v>
       </c>
       <c r="G172" t="str">
-        <f>$A$1&amp;B172&amp;$C$1&amp;D172&amp;E172&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-cracksabbath-themix-20130920.mp3\"&gt;04 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4785,7 +4846,7 @@
         <v>283</v>
       </c>
       <c r="G173" t="str">
-        <f>$A$1&amp;B173&amp;$C$1&amp;D173&amp;E173&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-cracksabbath-themix-20130920.mp3\"&gt;05 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4800,7 +4861,7 @@
         <v>283</v>
       </c>
       <c r="G174" t="str">
-        <f>$A$1&amp;B174&amp;$C$1&amp;D174&amp;E174&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-cracksabbath-themix-20130920.mp3\"&gt;01 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4815,7 +4876,7 @@
         <v>283</v>
       </c>
       <c r="G175" t="str">
-        <f>$A$1&amp;B175&amp;$C$1&amp;D175&amp;E175&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-cracksabbath-themix-20130920.mp3\"&gt;02 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4830,7 +4891,7 @@
         <v>283</v>
       </c>
       <c r="G176" t="str">
-        <f>$A$1&amp;B176&amp;$C$1&amp;D176&amp;E176&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-cracksabbath-themix-20130920.mp3\"&gt;03 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4845,7 +4906,7 @@
         <v>283</v>
       </c>
       <c r="G177" t="str">
-        <f>$A$1&amp;B177&amp;$C$1&amp;D177&amp;E177&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-cracksabbath-themix-20130920.mp3\"&gt;04 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4860,7 +4921,7 @@
         <v>283</v>
       </c>
       <c r="G178" t="str">
-        <f>$A$1&amp;B178&amp;$C$1&amp;D178&amp;E178&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-cracksabbath-themix-20130920.mp3\"&gt;05 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4875,7 +4936,7 @@
         <v>283</v>
       </c>
       <c r="G179" t="str">
-        <f>$A$1&amp;B179&amp;$C$1&amp;D179&amp;E179&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-cracksabbath-themix-20130920.mp3\"&gt;06 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4890,7 +4951,7 @@
         <v>283</v>
       </c>
       <c r="G180" t="str">
-        <f>$A$1&amp;B180&amp;$C$1&amp;D180&amp;E180&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-cracksabbath-themix-20130920.mp3\"&gt;07 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4905,7 +4966,7 @@
         <v>283</v>
       </c>
       <c r="G181" t="str">
-        <f>$A$1&amp;B181&amp;$C$1&amp;D181&amp;E181&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-cracksabbath-themix-20130920.mp3\"&gt;08 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4920,7 +4981,7 @@
         <v>283</v>
       </c>
       <c r="G182" t="str">
-        <f>$A$1&amp;B182&amp;$C$1&amp;D182&amp;E182&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-cracksabbath-themix-20130920.mp3\"&gt;09 Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4935,7 +4996,7 @@
         <v>283</v>
       </c>
       <c r="G183" t="str">
-        <f>$A$1&amp;B183&amp;$C$1&amp;D183&amp;E183&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-cracksabbath-themix-20130920.mp3\"&gt;10Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4950,7 +5011,7 @@
         <v>283</v>
       </c>
       <c r="G184" t="str">
-        <f>$A$1&amp;B184&amp;$C$1&amp;D184&amp;E184&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-cracksabbath-themix-20130920.mp3\"&gt;11Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4965,7 +5026,7 @@
         <v>283</v>
       </c>
       <c r="G185" t="str">
-        <f>$A$1&amp;B185&amp;$C$1&amp;D185&amp;E185&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-cracksabbath-themix-20130920.mp3\"&gt;12Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4980,7 +5041,7 @@
         <v>283</v>
       </c>
       <c r="G186" t="str">
-        <f>$A$1&amp;B186&amp;$C$1&amp;D186&amp;E186&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-cracksabbath-themix-20130920.mp3\"&gt;13Crack Sabbath - The Mix - September 20th, 2013&lt;/option&gt;</v>
       </c>
     </row>
@@ -4995,7 +5056,7 @@
         <v>284</v>
       </c>
       <c r="G187" t="str">
-        <f>$A$1&amp;B187&amp;$C$1&amp;D187&amp;E187&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-cracksabbath-owlandthistle-20140917.mp3\"&gt;01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5010,7 +5071,7 @@
         <v>284</v>
       </c>
       <c r="G188" t="str">
-        <f>$A$1&amp;B188&amp;$C$1&amp;D188&amp;E188&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-cracksabbath-owlandthistle-20140917.mp3\"&gt;02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5025,7 +5086,7 @@
         <v>284</v>
       </c>
       <c r="G189" t="str">
-        <f>$A$1&amp;B189&amp;$C$1&amp;D189&amp;E189&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-cracksabbath-owlandthistle-20140917.mp3\"&gt;03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5040,7 +5101,7 @@
         <v>284</v>
       </c>
       <c r="G190" t="str">
-        <f>$A$1&amp;B190&amp;$C$1&amp;D190&amp;E190&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-cracksabbath-owlandthistle-20140917.mp3\"&gt;04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5055,7 +5116,7 @@
         <v>284</v>
       </c>
       <c r="G191" t="str">
-        <f>$A$1&amp;B191&amp;$C$1&amp;D191&amp;E191&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0006-cracksabbath-owlandthistle-20140917.mp3\"&gt;05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5070,7 +5131,7 @@
         <v>284</v>
       </c>
       <c r="G192" t="str">
-        <f>$A$1&amp;B192&amp;$C$1&amp;D192&amp;E192&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0007-cracksabbath-owlandthistle-20140917.mp3\"&gt;01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5085,7 +5146,7 @@
         <v>284</v>
       </c>
       <c r="G193" t="str">
-        <f>$A$1&amp;B193&amp;$C$1&amp;D193&amp;E193&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-cracksabbath-owlandthistle-20140917.mp3\"&gt;02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5100,7 +5161,7 @@
         <v>284</v>
       </c>
       <c r="G194" t="str">
-        <f>$A$1&amp;B194&amp;$C$1&amp;D194&amp;E194&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-cracksabbath-owlandthistle-20140917.mp3\"&gt;03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5115,7 +5176,7 @@
         <v>284</v>
       </c>
       <c r="G195" t="str">
-        <f>$A$1&amp;B195&amp;$C$1&amp;D195&amp;E195&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-cracksabbath-owlandthistle-20140917.mp3\"&gt;04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5130,7 +5191,7 @@
         <v>284</v>
       </c>
       <c r="G196" t="str">
-        <f>$A$1&amp;B196&amp;$C$1&amp;D196&amp;E196&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-cracksabbath-owlandthistle-20140917.mp3\"&gt;05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5145,7 +5206,7 @@
         <v>284</v>
       </c>
       <c r="G197" t="str">
-        <f>$A$1&amp;B197&amp;$C$1&amp;D197&amp;E197&amp;$F$1</f>
+        <f t="shared" si="5"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-cracksabbath-owlandthistle-20140917.mp3\"&gt;06 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5160,7 +5221,7 @@
         <v>284</v>
       </c>
       <c r="G198" t="str">
-        <f>$A$1&amp;B198&amp;$C$1&amp;D198&amp;E198&amp;$F$1</f>
+        <f t="shared" ref="G198:G261" si="6">$A$1&amp;B198&amp;$C$1&amp;D198&amp;E198&amp;$F$1</f>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-cracksabbath-owlandthistle-20140917.mp3\"&gt;07 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5175,7 +5236,7 @@
         <v>284</v>
       </c>
       <c r="G199" t="str">
-        <f>$A$1&amp;B199&amp;$C$1&amp;D199&amp;E199&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-cracksabbath-owlandthistle-20140917.mp3\"&gt;08 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5190,7 +5251,7 @@
         <v>284</v>
       </c>
       <c r="G200" t="str">
-        <f>$A$1&amp;B200&amp;$C$1&amp;D200&amp;E200&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0015-cracksabbath-owlandthistle-20140917.mp3\"&gt;09 Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5205,7 +5266,7 @@
         <v>284</v>
       </c>
       <c r="G201" t="str">
-        <f>$A$1&amp;B201&amp;$C$1&amp;D201&amp;E201&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0016-cracksabbath-owlandthistle-20140917.mp3\"&gt;10Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5220,7 +5281,7 @@
         <v>284</v>
       </c>
       <c r="G202" t="str">
-        <f>$A$1&amp;B202&amp;$C$1&amp;D202&amp;E202&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0017-cracksabbath-owlandthistle-20140917.mp3\"&gt;11Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5235,7 +5296,7 @@
         <v>284</v>
       </c>
       <c r="G203" t="str">
-        <f>$A$1&amp;B203&amp;$C$1&amp;D203&amp;E203&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0018-cracksabbath-owlandthistle-20140917.mp3\"&gt;12Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5250,7 +5311,7 @@
         <v>284</v>
       </c>
       <c r="G204" t="str">
-        <f>$A$1&amp;B204&amp;$C$1&amp;D204&amp;E204&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0019-cracksabbath-owlandthistle-20140917.mp3\"&gt;13Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5265,7 +5326,7 @@
         <v>284</v>
       </c>
       <c r="G205" t="str">
-        <f>$A$1&amp;B205&amp;$C$1&amp;D205&amp;E205&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0020-cracksabbath-owlandthistle-20140917.mp3\"&gt;14Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5280,7 +5341,7 @@
         <v>284</v>
       </c>
       <c r="G206" t="str">
-        <f>$A$1&amp;B206&amp;$C$1&amp;D206&amp;E206&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0021-cracksabbath-owlandthistle-20140917.mp3\"&gt;15Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5295,7 +5356,7 @@
         <v>284</v>
       </c>
       <c r="G207" t="str">
-        <f>$A$1&amp;B207&amp;$C$1&amp;D207&amp;E207&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0022-cracksabbath-owlandthistle-20140917.mp3\"&gt;16Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5310,7 +5371,7 @@
         <v>284</v>
       </c>
       <c r="G208" t="str">
-        <f>$A$1&amp;B208&amp;$C$1&amp;D208&amp;E208&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0023-cracksabbath-owlandthistle-20140917.mp3\"&gt;17Crack Sabbath - Owl 'n Thistle - September 17th, 2014&lt;/option&gt;</v>
       </c>
     </row>
@@ -5325,7 +5386,7 @@
         <v>308</v>
       </c>
       <c r="G209" t="str">
-        <f>$A$1&amp;B209&amp;$C$1&amp;D209&amp;E209&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0001-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;01 Crack Sabbath - Royal Room - June 22nd, 2013&lt;/option&gt;</v>
       </c>
       <c r="I209" s="4"/>
@@ -5341,7 +5402,7 @@
         <v>309</v>
       </c>
       <c r="G210" t="str">
-        <f>$A$1&amp;B210&amp;$C$1&amp;D210&amp;E210&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0002-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;02 Crack Sabbath - Royal Room - June 22nd, 2014&lt;/option&gt;</v>
       </c>
       <c r="I210" s="4"/>
@@ -5357,7 +5418,7 @@
         <v>310</v>
       </c>
       <c r="G211" t="str">
-        <f>$A$1&amp;B211&amp;$C$1&amp;D211&amp;E211&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0003-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;03 Crack Sabbath - Royal Room - June 22nd, 2015&lt;/option&gt;</v>
       </c>
       <c r="I211" s="4"/>
@@ -5373,7 +5434,7 @@
         <v>311</v>
       </c>
       <c r="G212" t="str">
-        <f>$A$1&amp;B212&amp;$C$1&amp;D212&amp;E212&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0004-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;04 Crack Sabbath - Royal Room - June 22nd, 2016&lt;/option&gt;</v>
       </c>
       <c r="I212" s="4"/>
@@ -5389,7 +5450,7 @@
         <v>312</v>
       </c>
       <c r="G213" t="str">
-        <f>$A$1&amp;B213&amp;$C$1&amp;D213&amp;E213&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0005-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;05 Crack Sabbath - Royal Room - June 22nd, 2017&lt;/option&gt;</v>
       </c>
       <c r="I213" s="4"/>
@@ -5405,7 +5466,7 @@
         <v>313</v>
       </c>
       <c r="G214" t="str">
-        <f>$A$1&amp;B214&amp;$C$1&amp;D214&amp;E214&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0008-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;01 Crack Sabbath - Royal Room - June 22nd, 2018&lt;/option&gt;</v>
       </c>
       <c r="I214" s="4"/>
@@ -5421,7 +5482,7 @@
         <v>314</v>
       </c>
       <c r="G215" t="str">
-        <f>$A$1&amp;B215&amp;$C$1&amp;D215&amp;E215&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0009-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;02 Crack Sabbath - Royal Room - June 22nd, 2019&lt;/option&gt;</v>
       </c>
       <c r="I215" s="4"/>
@@ -5437,7 +5498,7 @@
         <v>315</v>
       </c>
       <c r="G216" t="str">
-        <f>$A$1&amp;B216&amp;$C$1&amp;D216&amp;E216&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0010-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;03 Crack Sabbath - Royal Room - June 22nd, 2020&lt;/option&gt;</v>
       </c>
       <c r="I216" s="4"/>
@@ -5453,7 +5514,7 @@
         <v>316</v>
       </c>
       <c r="G217" t="str">
-        <f>$A$1&amp;B217&amp;$C$1&amp;D217&amp;E217&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0011-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;04 Crack Sabbath - Royal Room - June 22nd, 2021&lt;/option&gt;</v>
       </c>
       <c r="I217" s="4"/>
@@ -5469,7 +5530,7 @@
         <v>317</v>
       </c>
       <c r="G218" t="str">
-        <f>$A$1&amp;B218&amp;$C$1&amp;D218&amp;E218&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0012-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;05 Crack Sabbath - Royal Room - June 22nd, 2022&lt;/option&gt;</v>
       </c>
       <c r="I218" s="4"/>
@@ -5485,7 +5546,7 @@
         <v>318</v>
       </c>
       <c r="G219" t="str">
-        <f>$A$1&amp;B219&amp;$C$1&amp;D219&amp;E219&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0013-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;06 Crack Sabbath - Royal Room - June 22nd, 2023&lt;/option&gt;</v>
       </c>
       <c r="I219" s="4"/>
@@ -5501,99 +5562,879 @@
         <v>319</v>
       </c>
       <c r="G220" t="str">
-        <f>$A$1&amp;B220&amp;$C$1&amp;D220&amp;E220&amp;$F$1</f>
+        <f t="shared" si="6"/>
         <v>&lt;option value=\"http://analogarchive.com/live/ZOOM0014-CrackSabbath-RoyalRoom-20130622.mp3\"&gt;07 Crack Sabbath - Royal Room - June 22nd, 2024&lt;/option&gt;</v>
       </c>
       <c r="I220" s="4"/>
     </row>
     <row r="221" spans="2:9">
+      <c r="B221" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E221" t="s">
+        <v>548</v>
+      </c>
       <c r="G221" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B2&amp;$C$1&amp;'OPTIONvideo (2)'!D2&amp;'OPTIONvideo (2)'!E2&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/marginal/jim-marginal-overthelight-march2015.mp4\"&gt;Sk8creteordie over the light at Marginal&lt;/option&gt;</v>
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/1%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3\"&gt;01Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="222" spans="2:9">
+      <c r="B222" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E222" t="s">
+        <v>548</v>
+      </c>
       <c r="G222" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B3&amp;$C$1&amp;'OPTIONvideo (2)'!D3&amp;'OPTIONvideo (2)'!E3&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0098.mp4\"&gt;01 WXPFL&lt;/option&gt;</v>
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/10%20Goin%20Against%20Your%20Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3\"&gt;10Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="223" spans="2:9">
+      <c r="B223" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E223" t="s">
+        <v>548</v>
+      </c>
       <c r="G223" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B4&amp;$C$1&amp;'OPTIONvideo (2)'!D4&amp;'OPTIONvideo (2)'!E4&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0101.mp4\"&gt;02 WXPFL&lt;/option&gt;</v>
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/11%20Kicked%20It%20In%20The%20Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3\"&gt;11Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="224" spans="2:9">
+      <c r="B224" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E224" t="s">
+        <v>548</v>
+      </c>
       <c r="G224" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B5&amp;$C$1&amp;'OPTIONvideo (2)'!D5&amp;'OPTIONvideo (2)'!E5&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0103.mp4\"&gt;03 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="225" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/12%20Center%20Of%20The%20Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3\"&gt;12Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="225" spans="2:7">
+      <c r="B225" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E225" t="s">
+        <v>548</v>
+      </c>
       <c r="G225" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B6&amp;$C$1&amp;'OPTIONvideo (2)'!D6&amp;'OPTIONvideo (2)'!E6&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0106.mp4\"&gt;04 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="226" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/13%20Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3\"&gt;13Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="226" spans="2:7">
+      <c r="B226" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D226" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E226" t="s">
+        <v>548</v>
+      </c>
       <c r="G226" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B7&amp;$C$1&amp;'OPTIONvideo (2)'!D7&amp;'OPTIONvideo (2)'!E7&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0109.mp4\"&gt;05 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="227" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/14%20Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3\"&gt;14Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="227" spans="2:7">
+      <c r="B227" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E227" t="s">
+        <v>548</v>
+      </c>
       <c r="G227" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B8&amp;$C$1&amp;'OPTIONvideo (2)'!D8&amp;'OPTIONvideo (2)'!E8&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0113.mp4\"&gt;01 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="228" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/15%20How%20Soon%20Is%20Now%20-%20Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3\"&gt;15Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="228" spans="2:7">
+      <c r="B228" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E228" t="s">
+        <v>548</v>
+      </c>
       <c r="G228" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B9&amp;$C$1&amp;'OPTIONvideo (2)'!D9&amp;'OPTIONvideo (2)'!E9&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0116.mp4\"&gt;02 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="229" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/2%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3\"&gt;02Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="229" spans="2:7">
+      <c r="B229" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E229" t="s">
+        <v>548</v>
+      </c>
       <c r="G229" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B10&amp;$C$1&amp;'OPTIONvideo (2)'!D10&amp;'OPTIONvideo (2)'!E10&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0117.mp4\"&gt;03 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="230" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/3%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3\"&gt;03Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="230" spans="2:7">
+      <c r="B230" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="E230" t="s">
+        <v>548</v>
+      </c>
       <c r="G230" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B11&amp;$C$1&amp;'OPTIONvideo (2)'!D11&amp;'OPTIONvideo (2)'!E11&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0119.mp4\"&gt;04 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="231" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/5%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3\"&gt;04Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="231" spans="2:7">
+      <c r="B231" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E231" t="s">
+        <v>548</v>
+      </c>
       <c r="G231" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B12&amp;$C$1&amp;'OPTIONvideo (2)'!D12&amp;'OPTIONvideo (2)'!E12&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0120.mp4\"&gt;05 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/6%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3\"&gt;05Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="232" spans="2:7">
+      <c r="B232" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D232" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="E232" t="s">
+        <v>548</v>
+      </c>
       <c r="G232" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B13&amp;$C$1&amp;'OPTIONvideo (2)'!D13&amp;'OPTIONvideo (2)'!E13&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/IMG_0127.mp4\"&gt;06 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="233" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/7%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3\"&gt;06Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="233" spans="2:7">
+      <c r="B233" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E233" t="s">
+        <v>548</v>
+      </c>
       <c r="G233" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B14&amp;$C$1&amp;'OPTIONvideo (2)'!D14&amp;'OPTIONvideo (2)'!E14&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/wxpfl/wxpfl-greenwood-201411.mp4\"&gt;07 WXPFL&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="234" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/8%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3\"&gt;07Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="234" spans="2:7">
+      <c r="B234" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D234" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E234" t="s">
+        <v>548</v>
+      </c>
       <c r="G234" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B15&amp;$C$1&amp;'OPTIONvideo (2)'!D15&amp;'OPTIONvideo (2)'!E15&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/kaylacheering/kayla_cheerleading_20150215.mp4\"&gt;01 Kayla Cheering&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="235" spans="7:7">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/9%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3\"&gt;08Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="235" spans="2:7">
+      <c r="B235" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E235" t="s">
+        <v>557</v>
+      </c>
       <c r="G235" t="str">
-        <f>$A$1&amp;'OPTIONvideo (2)'!B16&amp;$C$1&amp;'OPTIONvideo (2)'!D16&amp;'OPTIONvideo (2)'!E16&amp;$F$1</f>
-        <v>&lt;option value=\"http://analogarchive.com/live/kaylacheering/kayla_cheerleading_20150215b.mp4\"&gt; 02Kayla Cheering&lt;/option&gt;</v>
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/01goingagainstyourmind-BuiltToSpill-Freemont-20140620.mp3\"&gt;01 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="236" spans="2:7">
+      <c r="B236" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D236" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E236" t="s">
+        <v>557</v>
+      </c>
+      <c r="G236" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/02inthemorning-BuiltToSpill-Freemont-20140620.mp3\"&gt;02 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="237" spans="2:7">
+      <c r="B237" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E237" t="s">
+        <v>557</v>
+      </c>
+      <c r="G237" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/03theplan-BuiltToSpill-Freemont-20140620.mp3\"&gt;03 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="238" spans="2:7">
+      <c r="B238" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E238" t="s">
+        <v>557</v>
+      </c>
+      <c r="G238" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/04strange-BuiltToSpill-Freemont-20140620.mp3\"&gt;04 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="239" spans="2:7">
+      <c r="B239" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E239" t="s">
+        <v>557</v>
+      </c>
+      <c r="G239" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/05untrustable-BuiltToSpill-Freemont-20140620.mp3\"&gt;05 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="240" spans="2:7">
+      <c r="B240" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E240" t="s">
+        <v>557</v>
+      </c>
+      <c r="G240" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/06else-BuiltToSpill-Freemont-20140620.mp3\"&gt;01 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="241" spans="2:7">
+      <c r="B241" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D241" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E241" t="s">
+        <v>557</v>
+      </c>
+      <c r="G241" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/07messwithtime-BuiltToSpill-Freemont-20140620.mp3\"&gt;02 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="242" spans="2:7">
+      <c r="B242" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E242" t="s">
+        <v>557</v>
+      </c>
+      <c r="G242" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/08iwouldhurtafly-BuiltToSpill-Freemont-20140620.mp3\"&gt;03 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="243" spans="2:7">
+      <c r="B243" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E243" t="s">
+        <v>557</v>
+      </c>
+      <c r="G243" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/09getalife-BuiltToSpill-Freemont-20140620.mp3\"&gt;04 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="244" spans="2:7">
+      <c r="B244" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E244" t="s">
+        <v>557</v>
+      </c>
+      <c r="G244" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/10joyride-BuiltToSpill-Freemont-20140620.mp3\"&gt;05 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="245" spans="2:7">
+      <c r="B245" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E245" t="s">
+        <v>557</v>
+      </c>
+      <c r="G245" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/11stab-BuiltToSpill-Freemont-20140620.mp3\"&gt;06 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="246" spans="2:7">
+      <c r="B246" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E246" t="s">
+        <v>557</v>
+      </c>
+      <c r="G246" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/12carrythezero-BuiltToSpill-Freemont-20140620.mp3\"&gt;07 Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="247" spans="2:7">
+      <c r="B247" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E247" t="s">
+        <v>557</v>
+      </c>
+      <c r="G247" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/13youwereright-BuiltToSpill-Freemont-20140620.mp3\"&gt;01Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="248" spans="2:7">
+      <c r="B248" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E248" t="s">
+        <v>557</v>
+      </c>
+      <c r="G248" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/14bigdipper-BuiltToSpill-Freemont-20140620.mp3\"&gt;10Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="249" spans="2:7">
+      <c r="B249" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E249" t="s">
+        <v>557</v>
+      </c>
+      <c r="G249" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/15dontfearthereaper-BuiltToSpill-Freemont-20140620.mp3\"&gt;11Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="250" spans="2:7">
+      <c r="B250" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E250" t="s">
+        <v>557</v>
+      </c>
+      <c r="G250" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/16conventionalwisdom-BuiltToSpill-Freemont-20140620.mp3\"&gt;12Built to Spill - Fremont - June 20th, 2014&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="251" spans="2:7">
+      <c r="B251" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E251" t="s">
+        <v>559</v>
+      </c>
+      <c r="G251" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-center-BuiltToSpill-Geogetown-20130713.mp3\"&gt;01Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="252" spans="2:7">
+      <c r="B252" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E252" t="s">
+        <v>559</v>
+      </c>
+      <c r="G252" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-fly-BuiltToSpill-Geogetown-20130713.mp3\"&gt;02Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="253" spans="2:7">
+      <c r="B253" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E253" t="s">
+        <v>559</v>
+      </c>
+      <c r="G253" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-goingagainst-BuiltToSpill-Geogetown-20130713.mp3\"&gt;03Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="254" spans="2:7">
+      <c r="B254" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="E254" t="s">
+        <v>559</v>
+      </c>
+      <c r="G254" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-inthemorning-BuiltToSpill-Geogetown-20130713.mp3\"&gt;04Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="255" spans="2:7">
+      <c r="B255" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E255" t="s">
+        <v>559</v>
+      </c>
+      <c r="G255" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-madeupdreams-BuiltToSpill-Geogetown-20130713.mp3\"&gt;05Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="256" spans="2:7">
+      <c r="B256" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="E256" t="s">
+        <v>559</v>
+      </c>
+      <c r="G256" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-sidewalk-BuiltToSpill-Geogetown-20130713.mp3\"&gt;06Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="257" spans="2:7">
+      <c r="B257" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E257" t="s">
+        <v>559</v>
+      </c>
+      <c r="G257" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-soundcheck-BuiltToSpill-Geogetown-20130713.mp3\"&gt;07Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="258" spans="2:7">
+      <c r="B258" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D258" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E258" t="s">
+        <v>559</v>
+      </c>
+      <c r="G258" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-theplan-BuiltToSpill-Geogetown-20130713.mp3\"&gt;08Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="259" spans="2:7">
+      <c r="B259" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="E259" t="s">
+        <v>559</v>
+      </c>
+      <c r="G259" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-untitled-BuiltToSpill-Geogetown-20130713.mp3\"&gt;09Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="260" spans="2:7">
+      <c r="B260" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D260" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E260" t="s">
+        <v>559</v>
+      </c>
+      <c r="G260" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/bts-youwereright-BuiltToSpill-Geogetown-20130713.mp3\"&gt;10Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="261" spans="2:7">
+      <c r="B261" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D261" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E261" t="s">
+        <v>558</v>
+      </c>
+      <c r="G261" t="str">
+        <f t="shared" si="6"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/1%20Going%20Against%20Your%20Mind-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;01Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="262" spans="2:7">
+      <c r="B262" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E262" t="s">
+        <v>558</v>
+      </c>
+      <c r="G262" t="str">
+        <f t="shared" ref="G262:G278" si="7">$A$1&amp;B262&amp;$C$1&amp;D262&amp;E262&amp;$F$1</f>
+        <v>&lt;option value=\"http://analogarchive.com/live/10%20You%20were%20right-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;02Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="263" spans="2:7">
+      <c r="B263" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D263" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E263" t="s">
+        <v>558</v>
+      </c>
+      <c r="G263" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/11%20Conventional%20Wisdom-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;03Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="264" spans="2:7">
+      <c r="B264" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="E264" t="s">
+        <v>558</v>
+      </c>
+      <c r="G264" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/12%20Heart%20-%20Doug%20Martsch-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;04Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="265" spans="2:7">
+      <c r="B265" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E265" t="s">
+        <v>558</v>
+      </c>
+      <c r="G265" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/13%20Carry%20the%20Zero-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;05Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="266" spans="2:7">
+      <c r="B266" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="E266" t="s">
+        <v>558</v>
+      </c>
+      <c r="G266" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/14%20Instrumental%20-%20dont%20know-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;06Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="267" spans="2:7">
+      <c r="B267" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E267" t="s">
+        <v>558</v>
+      </c>
+      <c r="G267" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/15%20I%20would%20hurt%20a%20fly-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;07Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="268" spans="2:7">
+      <c r="B268" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E268" t="s">
+        <v>558</v>
+      </c>
+      <c r="G268" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/16%20Age%20of%20Consent%20-%20New%20Order-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;08Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="269" spans="2:7">
+      <c r="B269" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="E269" t="s">
+        <v>558</v>
+      </c>
+      <c r="G269" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/17%20How%20Soon%20is%20Now%20-%20The%20Smiths-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;09Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="270" spans="2:7">
+      <c r="B270" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E270" t="s">
+        <v>558</v>
+      </c>
+      <c r="G270" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/18%20Car-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;10Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="271" spans="2:7">
+      <c r="B271" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E271" t="s">
+        <v>558</v>
+      </c>
+      <c r="G271" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/2%20In%20The%20Morning-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;11Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="272" spans="2:7">
+      <c r="B272" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E272" t="s">
+        <v>558</v>
+      </c>
+      <c r="G272" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/3%20Center%20of%20the%20Universe-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;12Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="273" spans="2:7">
+      <c r="B273" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E273" t="s">
+        <v>558</v>
+      </c>
+      <c r="G273" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/4%20The%20Plan-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;13Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="274" spans="2:7">
+      <c r="B274" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D274" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E274" t="s">
+        <v>558</v>
+      </c>
+      <c r="G274" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/5%20Planting%20Seeds-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;14Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="275" spans="2:7">
+      <c r="B275" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D275" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E275" t="s">
+        <v>558</v>
+      </c>
+      <c r="G275" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/6%20Kicked%20It%20In%20the%20Sun-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;15Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="276" spans="2:7">
+      <c r="B276" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D276" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E276" t="s">
+        <v>558</v>
+      </c>
+      <c r="G276" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/7%20Get%20a%20Life-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;16Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="277" spans="2:7">
+      <c r="B277" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="D277" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E277" t="s">
+        <v>558</v>
+      </c>
+      <c r="G277" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/8%20Sidewalk-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;17Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="278" spans="2:7">
+      <c r="B278" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E278" t="s">
+        <v>558</v>
+      </c>
+      <c r="G278" t="str">
+        <f t="shared" si="7"/>
+        <v>&lt;option value=\"http://analogarchive.com/live/9%20Here%20-%20Pavement-BuiltToSpill-LiveatNeumos20131227.mp3\"&gt;18Built to Spill - Neumos, Seattle - December 27th, 2013&lt;/option&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -5605,7 +6446,6 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="D71:D120" numberStoredAsText="1"/>
-    <ignoredError sqref="G221" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5619,7 +6459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G8"/>
     </sheetView>
   </sheetViews>
@@ -8029,309 +8869,488 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="106" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>498</v>
+      </c>
+      <c r="B6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>512</v>
+      </c>
+      <c r="B7" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>502</v>
+      </c>
+      <c r="B8" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>486</v>
+      </c>
+      <c r="B10" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>488</v>
+      </c>
+      <c r="B11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>489</v>
+      </c>
+      <c r="B12" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>491</v>
+      </c>
+      <c r="B13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>506</v>
+      </c>
+      <c r="B14" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B15" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>322</v>
+      </c>
+      <c r="B17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>323</v>
+      </c>
+      <c r="B18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>325</v>
+      </c>
+      <c r="B20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>326</v>
+      </c>
+      <c r="B21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>327</v>
+      </c>
+      <c r="B22" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>328</v>
+      </c>
+      <c r="B23" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>329</v>
+      </c>
+      <c r="B24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>332</v>
+      </c>
+      <c r="B27" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>333</v>
+      </c>
+      <c r="B28" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>334</v>
+      </c>
+      <c r="B29" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>335</v>
+      </c>
+      <c r="B30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>338</v>
+      </c>
+      <c r="B33" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B34" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>340</v>
+      </c>
+      <c r="B35" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>341</v>
+      </c>
+      <c r="B36" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>342</v>
+      </c>
+      <c r="B37" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>343</v>
+      </c>
+      <c r="B38" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>345</v>
+      </c>
+      <c r="B40" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="B41" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>494</v>
+      </c>
+      <c r="B42" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>508</v>
+      </c>
+      <c r="B43" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>510</v>
+      </c>
+      <c r="B44" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>496</v>
+      </c>
+      <c r="B45" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>511</v>
+      </c>
+      <c r="B46" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>499</v>
+      </c>
+      <c r="B47" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>513</v>
+      </c>
+      <c r="B48" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>482</v>
+      </c>
+      <c r="B49" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>500</v>
+      </c>
+      <c r="B50" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="B51" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+      <c r="B52" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="B53" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+      <c r="B54" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="B55" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+      <c r="B56" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="B57" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>345</v>
+      <c r="B58" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B58">
+    <sortCondition ref="B1:B58"/>
+    <sortCondition ref="A1:A58"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated built to spill links
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="597">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -1708,6 +1708,114 @@
   </si>
   <si>
     <t>02</t>
+  </si>
+  <si>
+    <t>08 bts-center-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>08 bts-fly-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>08 bts-goingagainst-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>08 bts-inthemorning-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>09 bts-madeupdreams-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>09 bts-sidewalk-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>09 bts-soundcheck-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>09 bts-theplan-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>09 bts-untitled-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>09 bts-youwereright-BuiltToSpill-Geogetown-20130713.mp3</t>
+  </si>
+  <si>
+    <t>02 In The Morning-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>03 Center of the Universe-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>04 The Plan-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>01 Going Against Your Mind-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>05 Planting Seeds-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>06 Kicked It In the Sun-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>07 Get a Life-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>08 Sidewalk-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>09 Here - Pavement-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>10 You were right-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>11 Conventional Wisdom-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>12 Heart - Doug Martsch-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>13 Carry the Zero-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>14 Instrumental - dont know-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>15 I would hurt a fly-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>16 Age of Consent - New Order-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>17 How Soon is Now - The Smiths-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>18 Car-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>01%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>02%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>03%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>05%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>06%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>07%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>08%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3</t>
+  </si>
+  <si>
+    <t>09%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1871,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1842,6 +1950,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1939,7 +2050,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="170">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2067,6 +2178,9 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2437,8 +2551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="G227" sqref="G227:G278"/>
+    <sheetView tabSelected="1" topLeftCell="C213" workbookViewId="0">
+      <selection activeCell="D234" sqref="D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5569,7 +5683,7 @@
     </row>
     <row r="221" spans="2:9">
       <c r="B221" s="1" t="s">
-        <v>483</v>
+        <v>589</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>549</v>
@@ -5579,12 +5693,12 @@
       </c>
       <c r="G221" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/1%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3\"&gt;01Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/01%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3\"&gt;01Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="222" spans="2:9">
       <c r="B222" s="1" t="s">
-        <v>507</v>
+        <v>590</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>285</v>
@@ -5594,12 +5708,12 @@
       </c>
       <c r="G222" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/10%20Goin%20Against%20Your%20Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3\"&gt;10Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/02%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3\"&gt;10Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="223" spans="2:9">
       <c r="B223" s="1" t="s">
-        <v>495</v>
+        <v>591</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>286</v>
@@ -5609,12 +5723,12 @@
       </c>
       <c r="G223" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/11%20Kicked%20It%20In%20The%20Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3\"&gt;11Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/03%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3\"&gt;11Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="224" spans="2:9">
       <c r="B224" s="1" t="s">
-        <v>509</v>
+        <v>592</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>287</v>
@@ -5624,12 +5738,12 @@
       </c>
       <c r="G224" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/12%20Center%20Of%20The%20Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3\"&gt;12Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/05%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3\"&gt;12Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="225" spans="2:7">
       <c r="B225" s="1" t="s">
-        <v>497</v>
+        <v>593</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>288</v>
@@ -5639,12 +5753,12 @@
       </c>
       <c r="G225" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/13%20Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3\"&gt;13Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/06%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3\"&gt;13Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="226" spans="2:7">
       <c r="B226" s="1" t="s">
-        <v>498</v>
+        <v>594</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>289</v>
@@ -5654,12 +5768,12 @@
       </c>
       <c r="G226" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/14%20Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3\"&gt;14Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/07%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3\"&gt;14Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="227" spans="2:7">
       <c r="B227" s="1" t="s">
-        <v>512</v>
+        <v>595</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>290</v>
@@ -5669,12 +5783,12 @@
       </c>
       <c r="G227" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/15%20How%20Soon%20Is%20Now%20-%20Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3\"&gt;15Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/08%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3\"&gt;15Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="228" spans="2:7">
       <c r="B228" s="1" t="s">
-        <v>502</v>
+        <v>596</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>560</v>
@@ -5684,12 +5798,12 @@
       </c>
       <c r="G228" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/2%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3\"&gt;02Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/09%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3\"&gt;02Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="229" spans="2:7">
       <c r="B229" s="1" t="s">
-        <v>485</v>
+        <v>507</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>550</v>
@@ -5699,12 +5813,12 @@
       </c>
       <c r="G229" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/3%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3\"&gt;03Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/10%20Goin%20Against%20Your%20Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3\"&gt;03Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="230" spans="2:7">
       <c r="B230" s="1" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>551</v>
@@ -5714,12 +5828,12 @@
       </c>
       <c r="G230" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/5%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3\"&gt;04Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/11%20Kicked%20It%20In%20The%20Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3\"&gt;04Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="231" spans="2:7">
       <c r="B231" s="1" t="s">
-        <v>488</v>
+        <v>509</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>552</v>
@@ -5729,12 +5843,12 @@
       </c>
       <c r="G231" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/6%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3\"&gt;05Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/12%20Center%20Of%20The%20Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3\"&gt;05Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="232" spans="2:7">
       <c r="B232" s="1" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>553</v>
@@ -5744,12 +5858,12 @@
       </c>
       <c r="G232" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/7%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3\"&gt;06Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/13%20Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3\"&gt;06Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="233" spans="2:7">
       <c r="B233" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>554</v>
@@ -5759,12 +5873,12 @@
       </c>
       <c r="G233" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/8%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3\"&gt;07Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/14%20Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3\"&gt;07Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="234" spans="2:7">
       <c r="B234" s="1" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>555</v>
@@ -5774,7 +5888,7 @@
       </c>
       <c r="G234" t="str">
         <f t="shared" si="6"/>
-        <v>&lt;option value=\"http://analogarchive.com/live/9%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3\"&gt;08Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
+        <v>&lt;option value=\"http://analogarchive.com/live/15%20How%20Soon%20Is%20Now%20-%20Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3\"&gt;08Built to Spill - Bellingham - February 2nd, 2013&lt;/option&gt;</v>
       </c>
     </row>
     <row r="235" spans="2:7">
@@ -8869,485 +8983,834 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A58"/>
+      <selection activeCell="C1" sqref="C1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="79.33203125" customWidth="1"/>
+    <col min="3" max="3" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>483</v>
       </c>
       <c r="B1" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>589</v>
+      </c>
+      <c r="D1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>507</v>
       </c>
       <c r="B2" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>590</v>
+      </c>
+      <c r="D2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>495</v>
       </c>
       <c r="B3" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>591</v>
+      </c>
+      <c r="D3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>509</v>
       </c>
       <c r="B4" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>592</v>
+      </c>
+      <c r="D4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>497</v>
       </c>
       <c r="B5" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>593</v>
+      </c>
+      <c r="D5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>498</v>
       </c>
       <c r="B6" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>594</v>
+      </c>
+      <c r="D6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>512</v>
       </c>
       <c r="B7" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>595</v>
+      </c>
+      <c r="D7" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>502</v>
       </c>
       <c r="B8" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>596</v>
+      </c>
+      <c r="D8" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>485</v>
       </c>
       <c r="B9" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>507</v>
+      </c>
+      <c r="D9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>486</v>
       </c>
       <c r="B10" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>495</v>
+      </c>
+      <c r="D10" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>488</v>
       </c>
       <c r="B11" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>509</v>
+      </c>
+      <c r="D11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>489</v>
       </c>
       <c r="B12" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>497</v>
+      </c>
+      <c r="D12" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>491</v>
       </c>
       <c r="B13" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>498</v>
+      </c>
+      <c r="D13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>506</v>
       </c>
       <c r="B14" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>512</v>
+      </c>
+      <c r="D14" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>320</v>
       </c>
       <c r="B15" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>320</v>
+      </c>
+      <c r="D15" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>321</v>
       </c>
       <c r="B16" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>321</v>
+      </c>
+      <c r="D16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>322</v>
       </c>
       <c r="B17" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>323</v>
       </c>
       <c r="B18" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>323</v>
+      </c>
+      <c r="D18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>324</v>
       </c>
       <c r="B19" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>324</v>
+      </c>
+      <c r="D19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>325</v>
       </c>
       <c r="B20" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>325</v>
+      </c>
+      <c r="D20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>326</v>
       </c>
       <c r="B21" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>326</v>
+      </c>
+      <c r="D21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>327</v>
       </c>
       <c r="B22" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>328</v>
       </c>
       <c r="B23" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>328</v>
+      </c>
+      <c r="D23" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>329</v>
       </c>
       <c r="B24" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>329</v>
+      </c>
+      <c r="D24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>330</v>
       </c>
       <c r="B25" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>330</v>
+      </c>
+      <c r="D25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>331</v>
       </c>
       <c r="B26" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>331</v>
+      </c>
+      <c r="D26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>332</v>
       </c>
       <c r="B27" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
+      <c r="D27" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>333</v>
       </c>
       <c r="B28" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D28" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>334</v>
       </c>
       <c r="B29" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>334</v>
+      </c>
+      <c r="D29" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>335</v>
       </c>
       <c r="B30" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>335</v>
+      </c>
+      <c r="D30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>336</v>
       </c>
       <c r="B31" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>561</v>
+      </c>
+      <c r="D31" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>337</v>
       </c>
       <c r="B32" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>562</v>
+      </c>
+      <c r="D32" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>338</v>
       </c>
       <c r="B33" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>563</v>
+      </c>
+      <c r="D33" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>339</v>
       </c>
       <c r="B34" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>564</v>
+      </c>
+      <c r="D34" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>340</v>
       </c>
       <c r="B35" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>565</v>
+      </c>
+      <c r="D35" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>341</v>
       </c>
       <c r="B36" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>566</v>
+      </c>
+      <c r="D36" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>342</v>
       </c>
       <c r="B37" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>567</v>
+      </c>
+      <c r="D37" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>343</v>
       </c>
       <c r="B38" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>568</v>
+      </c>
+      <c r="D38" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>344</v>
       </c>
       <c r="B39" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>569</v>
+      </c>
+      <c r="D39" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>345</v>
       </c>
       <c r="B40" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>570</v>
+      </c>
+      <c r="D40" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>501</v>
       </c>
       <c r="B41" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>574</v>
+      </c>
+      <c r="D41" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>494</v>
       </c>
       <c r="B42" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>571</v>
+      </c>
+      <c r="D42" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>508</v>
       </c>
       <c r="B43" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>572</v>
+      </c>
+      <c r="D43" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>510</v>
       </c>
       <c r="B44" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>573</v>
+      </c>
+      <c r="D44" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>496</v>
       </c>
       <c r="B45" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>575</v>
+      </c>
+      <c r="D45" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>511</v>
       </c>
       <c r="B46" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>576</v>
+      </c>
+      <c r="D46" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>499</v>
       </c>
       <c r="B47" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>577</v>
+      </c>
+      <c r="D47" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>513</v>
       </c>
       <c r="B48" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>578</v>
+      </c>
+      <c r="D48" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>482</v>
       </c>
       <c r="B49" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>579</v>
+      </c>
+      <c r="D49" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>500</v>
       </c>
       <c r="B50" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>580</v>
+      </c>
+      <c r="D50" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>484</v>
       </c>
       <c r="B51" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>581</v>
+      </c>
+      <c r="D51" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>503</v>
       </c>
       <c r="B52" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>582</v>
+      </c>
+      <c r="D52" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>504</v>
       </c>
       <c r="B53" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>583</v>
+      </c>
+      <c r="D53" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>505</v>
       </c>
       <c r="B54" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>584</v>
+      </c>
+      <c r="D54" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>487</v>
       </c>
       <c r="B55" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>585</v>
+      </c>
+      <c r="D55" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>490</v>
       </c>
       <c r="B56" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>586</v>
+      </c>
+      <c r="D56" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>492</v>
       </c>
       <c r="B57" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>587</v>
+      </c>
+      <c r="D57" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>493</v>
       </c>
       <c r="B58" t="s">
         <v>545</v>
       </c>
+      <c r="C58" t="s">
+        <v>588</v>
+      </c>
+      <c r="D58" t="s">
+        <v>545</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B58">
-    <sortCondition ref="B1:B58"/>
-    <sortCondition ref="A1:A58"/>
+  <sortState ref="C1:D58">
+    <sortCondition ref="D1:D58"/>
+    <sortCondition ref="C1:C58"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
made it easier to add songs
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="OPTIONaudio" sheetId="1" r:id="rId1"/>
-    <sheet name="OPTIONvideo" sheetId="7" r:id="rId2"/>
-    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId3"/>
-    <sheet name="IMG" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
-    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId6"/>
-    <sheet name="built to spill" sheetId="6" r:id="rId7"/>
+    <sheet name="json array" sheetId="10" r:id="rId1"/>
+    <sheet name="OPTIONaudio" sheetId="1" r:id="rId2"/>
+    <sheet name="OPTIONvideo" sheetId="7" r:id="rId3"/>
+    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId4"/>
+    <sheet name="IMG" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
+    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId7"/>
+    <sheet name="built to spill" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -2580,9 +2581,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
       <selection activeCell="B261" sqref="B261:B278"/>
     </sheetView>
   </sheetViews>
@@ -2592,7 +2610,7 @@
     <col min="2" max="2" width="91.5" customWidth="1"/>
     <col min="3" max="3" width="2.5" customWidth="1"/>
     <col min="4" max="4" width="3.1640625" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
     <col min="8" max="8" width="78.1640625" customWidth="1"/>
@@ -6600,7 +6618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -6748,7 +6766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -7011,7 +7029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -7146,7 +7164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A52:A248"/>
   <sheetViews>
@@ -8155,7 +8173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
@@ -9012,7 +9030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>

</xml_diff>

<commit_message>
added built to spill through the new way
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="44600" windowHeight="25040" tabRatio="760"/>
   </bookViews>
   <sheets>
-    <sheet name="json array" sheetId="10" r:id="rId1"/>
-    <sheet name="OPTIONaudio" sheetId="1" r:id="rId2"/>
-    <sheet name="OPTIONvideo" sheetId="7" r:id="rId3"/>
-    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId4"/>
-    <sheet name="IMG" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
-    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId7"/>
-    <sheet name="built to spill" sheetId="6" r:id="rId8"/>
+    <sheet name="builttospilljson" sheetId="11" r:id="rId1"/>
+    <sheet name="json array" sheetId="10" r:id="rId2"/>
+    <sheet name="OPTIONaudio" sheetId="1" r:id="rId3"/>
+    <sheet name="OPTIONvideo" sheetId="7" r:id="rId4"/>
+    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId5"/>
+    <sheet name="IMG" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId7"/>
+    <sheet name="SONGS WITH SPACES" sheetId="5" r:id="rId8"/>
+    <sheet name="built to spill" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="659">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -1844,6 +1845,165 @@
   </si>
   <si>
     <t>09%20Here%20-%20Pavement-BuiltToSpill-LiveatNeumos20131227.mp3</t>
+  </si>
+  <si>
+    <t>01 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>02 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>03 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>04 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>05 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>06 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>07 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>08 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>10 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>11 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>12 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>13 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>14 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>15 Built to Spill - Bellingham - February 2nd, 2013</t>
+  </si>
+  <si>
+    <t>01 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>02 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>03 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>04 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>05 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>06 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>07 Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>01Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>10Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>11Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>12Built to Spill - Fremont - June 20th, 2014</t>
+  </si>
+  <si>
+    <t>01Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>02Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>03Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>04Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>05Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>06Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>07Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>08Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>09Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>10Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013</t>
+  </si>
+  <si>
+    <t>01Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>02Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>03Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>04Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>05Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>06Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>07Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>08Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>09Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>10Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>11Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>12Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>13Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>14Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>15Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>16Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>17Built to Spill - Neumos, Seattle - December 27th, 2013</t>
+  </si>
+  <si>
+    <t>18Built to Spill - Neumos, Seattle - December 27th, 2013</t>
   </si>
 </sst>
 </file>
@@ -2581,6 +2741,726 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C60" sqref="C59:C67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="74" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"{'file':'"&amp;A1&amp;"','title','"&amp;B1&amp;"'},"</f>
+        <v>{'file':'01%20Hazy2013-02-03-15-02-09-0679196-BuiltToSpill-Bellingham-20130202.mp3','title','01 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">"{'file':'"&amp;A2&amp;"','title','"&amp;B2&amp;"'},"</f>
+        <v>{'file':'09%20Dont%20Fear%20the%20Reaper2013-02-03-15-17-23-8247012-BuiltToSpill-Bellingham-20130202.mp3','title','02 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'10%20Goin%20Against%20Your%20Mind2013-02-03-15-17-25-1663528-BuiltToSpill-Bellingham-20130202.mp3','title','03 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B4" t="s">
+        <v>609</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'11%20Kicked%20It%20In%20The%20Sun2013-02-03-15-17-25-9151816-BuiltToSpill-Bellingham-20130202.mp3','title','04 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B5" t="s">
+        <v>610</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'12%20Center%20Of%20The%20Universe2013-02-03-15-17-27-2100314-BuiltToSpill-Bellingham-20130202.mp3','title','05 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B6" t="s">
+        <v>611</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'13%20Heart2013-02-03-15-17-27-3192356-BuiltToSpill-Bellingham-20130202.mp3','title','06 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>498</v>
+      </c>
+      <c r="B7" t="s">
+        <v>612</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'14%20Pat2013-02-03-15-17-28-4736800-BuiltToSpill-Bellingham-20130202.mp3','title','07 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>512</v>
+      </c>
+      <c r="B8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'15%20How%20Soon%20Is%20Now%20-%20Unknown2013-02-03-15-17-29-5657220-BuiltToSpill-Bellingham-20130202.mp3','title','08 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>590</v>
+      </c>
+      <c r="B9" t="s">
+        <v>614</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'02%20The%20Source2013-02-03-15-02-10-4095712-BuiltToSpill-Bellingham-20130202.mp3','title','10 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>591</v>
+      </c>
+      <c r="B10" t="s">
+        <v>615</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'03%20Reasons2013-02-03-15-02-11-6108174-BuiltToSpill-Bellingham-20130202.mp3','title','11 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>592</v>
+      </c>
+      <c r="B11" t="s">
+        <v>616</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'05%20Stab2013-02-03-15-02-13-9977092-BuiltToSpill-Bellingham-20130202.mp3','title','12 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>593</v>
+      </c>
+      <c r="B12" t="s">
+        <v>617</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'06%20Strange2013-02-03-15-02-15-2301566-BuiltToSpill-Bellingham-20130202.mp3','title','13 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>594</v>
+      </c>
+      <c r="B13" t="s">
+        <v>618</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'07%20Get%20a%20Life2013-02-03-15-02-15-5421686-BuiltToSpill-Bellingham-20130202.mp3','title','14 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>595</v>
+      </c>
+      <c r="B14" t="s">
+        <v>619</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'08%20Made%20Up%20Dreams2013-02-03-15-02-16-8214178-BuiltToSpill-Bellingham-20130202.mp3','title','15 Built to Spill - Bellingham - February 2nd, 2013'},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B15" t="s">
+        <v>620</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'01goingagainstyourmind-BuiltToSpill-Freemont-20140620.mp3','title','01 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>621</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'02inthemorning-BuiltToSpill-Freemont-20140620.mp3','title','02 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>322</v>
+      </c>
+      <c r="B17" t="s">
+        <v>622</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'03theplan-BuiltToSpill-Freemont-20140620.mp3','title','03 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>323</v>
+      </c>
+      <c r="B18" t="s">
+        <v>623</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'04strange-BuiltToSpill-Freemont-20140620.mp3','title','04 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B19" t="s">
+        <v>624</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'05untrustable-BuiltToSpill-Freemont-20140620.mp3','title','05 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>325</v>
+      </c>
+      <c r="B20" t="s">
+        <v>620</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'06else-BuiltToSpill-Freemont-20140620.mp3','title','01 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>326</v>
+      </c>
+      <c r="B21" t="s">
+        <v>621</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'07messwithtime-BuiltToSpill-Freemont-20140620.mp3','title','02 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>327</v>
+      </c>
+      <c r="B22" t="s">
+        <v>622</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'08iwouldhurtafly-BuiltToSpill-Freemont-20140620.mp3','title','03 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>328</v>
+      </c>
+      <c r="B23" t="s">
+        <v>623</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'09getalife-BuiltToSpill-Freemont-20140620.mp3','title','04 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>329</v>
+      </c>
+      <c r="B24" t="s">
+        <v>624</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'10joyride-BuiltToSpill-Freemont-20140620.mp3','title','05 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" t="s">
+        <v>625</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'11stab-BuiltToSpill-Freemont-20140620.mp3','title','06 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" t="s">
+        <v>626</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'12carrythezero-BuiltToSpill-Freemont-20140620.mp3','title','07 Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>332</v>
+      </c>
+      <c r="B27" t="s">
+        <v>627</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'13youwereright-BuiltToSpill-Freemont-20140620.mp3','title','01Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>333</v>
+      </c>
+      <c r="B28" t="s">
+        <v>628</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'14bigdipper-BuiltToSpill-Freemont-20140620.mp3','title','10Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>334</v>
+      </c>
+      <c r="B29" t="s">
+        <v>629</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'15dontfearthereaper-BuiltToSpill-Freemont-20140620.mp3','title','11Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>335</v>
+      </c>
+      <c r="B30" t="s">
+        <v>630</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'16conventionalwisdom-BuiltToSpill-Freemont-20140620.mp3','title','12Built to Spill - Fremont - June 20th, 2014'},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" t="s">
+        <v>631</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-center-BuiltToSpill-Geogetown-20130713.mp3','title','01Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32" t="s">
+        <v>632</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-fly-BuiltToSpill-Geogetown-20130713.mp3','title','02Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>338</v>
+      </c>
+      <c r="B33" t="s">
+        <v>633</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-goingagainst-BuiltToSpill-Geogetown-20130713.mp3','title','03Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B34" t="s">
+        <v>634</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-inthemorning-BuiltToSpill-Geogetown-20130713.mp3','title','04Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>340</v>
+      </c>
+      <c r="B35" t="s">
+        <v>635</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-madeupdreams-BuiltToSpill-Geogetown-20130713.mp3','title','05Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>341</v>
+      </c>
+      <c r="B36" t="s">
+        <v>636</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-sidewalk-BuiltToSpill-Geogetown-20130713.mp3','title','06Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>342</v>
+      </c>
+      <c r="B37" t="s">
+        <v>637</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-soundcheck-BuiltToSpill-Geogetown-20130713.mp3','title','07Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>343</v>
+      </c>
+      <c r="B38" t="s">
+        <v>638</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-theplan-BuiltToSpill-Geogetown-20130713.mp3','title','08Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" t="s">
+        <v>639</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-untitled-BuiltToSpill-Geogetown-20130713.mp3','title','09Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>345</v>
+      </c>
+      <c r="B40" t="s">
+        <v>640</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'bts-youwereright-BuiltToSpill-Geogetown-20130713.mp3','title','10Built to Spill - Sub Pop 25th, Georgetown - July 13th, 2013'},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>597</v>
+      </c>
+      <c r="B41" t="s">
+        <v>641</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'01%20Going%20Against%20Your%20Mind-BuiltToSpill-LiveatNeumos20131227.mp3','title','01Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>598</v>
+      </c>
+      <c r="B42" t="s">
+        <v>642</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'02%20In%20The%20Morning-BuiltToSpill-LiveatNeumos20131227.mp3','title','02Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>599</v>
+      </c>
+      <c r="B43" t="s">
+        <v>643</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'03%20Center%20of%20the%20Universe-BuiltToSpill-LiveatNeumos20131227.mp3','title','03Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>600</v>
+      </c>
+      <c r="B44" t="s">
+        <v>644</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'04%20The%20Plan-BuiltToSpill-LiveatNeumos20131227.mp3','title','04Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>601</v>
+      </c>
+      <c r="B45" t="s">
+        <v>645</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'05%20Planting%20Seeds-BuiltToSpill-LiveatNeumos20131227.mp3','title','05Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>602</v>
+      </c>
+      <c r="B46" t="s">
+        <v>646</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'06%20Kicked%20It%20In%20the%20Sun-BuiltToSpill-LiveatNeumos20131227.mp3','title','06Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>603</v>
+      </c>
+      <c r="B47" t="s">
+        <v>647</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'07%20Get%20a%20Life-BuiltToSpill-LiveatNeumos20131227.mp3','title','07Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>604</v>
+      </c>
+      <c r="B48" t="s">
+        <v>648</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'08%20Sidewalk-BuiltToSpill-LiveatNeumos20131227.mp3','title','08Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>605</v>
+      </c>
+      <c r="B49" t="s">
+        <v>649</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'09%20Here%20-%20Pavement-BuiltToSpill-LiveatNeumos20131227.mp3','title','09Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>494</v>
+      </c>
+      <c r="B50" t="s">
+        <v>650</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'10%20You%20were%20right-BuiltToSpill-LiveatNeumos20131227.mp3','title','10Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>508</v>
+      </c>
+      <c r="B51" t="s">
+        <v>651</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'11%20Conventional%20Wisdom-BuiltToSpill-LiveatNeumos20131227.mp3','title','11Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>510</v>
+      </c>
+      <c r="B52" t="s">
+        <v>652</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'12%20Heart%20-%20Doug%20Martsch-BuiltToSpill-LiveatNeumos20131227.mp3','title','12Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>496</v>
+      </c>
+      <c r="B53" t="s">
+        <v>653</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'13%20Carry%20the%20Zero-BuiltToSpill-LiveatNeumos20131227.mp3','title','13Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>511</v>
+      </c>
+      <c r="B54" t="s">
+        <v>654</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'14%20Instrumental%20-%20dont%20know-BuiltToSpill-LiveatNeumos20131227.mp3','title','14Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>499</v>
+      </c>
+      <c r="B55" t="s">
+        <v>655</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'15%20I%20would%20hurt%20a%20fly-BuiltToSpill-LiveatNeumos20131227.mp3','title','15Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>513</v>
+      </c>
+      <c r="B56" t="s">
+        <v>656</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'16%20Age%20of%20Consent%20-%20New%20Order-BuiltToSpill-LiveatNeumos20131227.mp3','title','16Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>482</v>
+      </c>
+      <c r="B57" t="s">
+        <v>657</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'17%20How%20Soon%20is%20Now%20-%20The%20Smiths-BuiltToSpill-LiveatNeumos20131227.mp3','title','17Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>500</v>
+      </c>
+      <c r="B58" t="s">
+        <v>658</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'18%20Car-BuiltToSpill-LiveatNeumos20131227.mp3','title','18Built to Spill - Neumos, Seattle - December 27th, 2013'},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2596,11 +3476,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+    <sheetView topLeftCell="A237" workbookViewId="0">
       <selection activeCell="B261" sqref="B261:B278"/>
     </sheetView>
   </sheetViews>
@@ -6618,7 +7498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -6766,7 +7646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -7029,7 +7909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -7164,7 +8044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A52:A248"/>
   <sheetViews>
@@ -8173,7 +9053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
@@ -9030,11 +9910,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added roxhill session and did some more formatting changes to page
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="865" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="865"/>
   </bookViews>
   <sheets>
-    <sheet name="zekeJSON" sheetId="4" r:id="rId1"/>
-    <sheet name="lastgaspJSON" sheetId="16" r:id="rId2"/>
-    <sheet name="marklaneganJSON" sheetId="17" r:id="rId3"/>
-    <sheet name="bigbusinessJSON" sheetId="18" r:id="rId4"/>
-    <sheet name="cracksabbathJSON" sheetId="12" r:id="rId5"/>
-    <sheet name="melvinsJSON" sheetId="14" r:id="rId6"/>
-    <sheet name="sufferingfuckheadsJSON" sheetId="15" r:id="rId7"/>
-    <sheet name="builttospillJSON" sheetId="11" r:id="rId8"/>
-    <sheet name="json array" sheetId="10" r:id="rId9"/>
-    <sheet name="OPTIONaudio" sheetId="1" r:id="rId10"/>
-    <sheet name="OPTIONvideo" sheetId="7" r:id="rId11"/>
-    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId12"/>
-    <sheet name="IMG" sheetId="3" r:id="rId13"/>
+    <sheet name="roxhillJSON" sheetId="19" r:id="rId1"/>
+    <sheet name="zekeJSON" sheetId="4" r:id="rId2"/>
+    <sheet name="lastgaspJSON" sheetId="16" r:id="rId3"/>
+    <sheet name="marklaneganJSON" sheetId="17" r:id="rId4"/>
+    <sheet name="bigbusinessJSON" sheetId="18" r:id="rId5"/>
+    <sheet name="cracksabbathJSON" sheetId="12" r:id="rId6"/>
+    <sheet name="melvinsJSON" sheetId="14" r:id="rId7"/>
+    <sheet name="sufferingfuckheadsJSON" sheetId="15" r:id="rId8"/>
+    <sheet name="builttospillJSON" sheetId="11" r:id="rId9"/>
+    <sheet name="json array" sheetId="10" r:id="rId10"/>
+    <sheet name="OPTIONaudio" sheetId="1" r:id="rId11"/>
+    <sheet name="OPTIONvideo" sheetId="7" r:id="rId12"/>
+    <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId13"/>
+    <sheet name="IMG" sheetId="3" r:id="rId14"/>
+    <sheet name="Sheet2" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="896">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -2566,6 +2568,159 @@
   </si>
   <si>
     <t>19%20marklanegan-showbox-20140703-19.mp3</t>
+  </si>
+  <si>
+    <t>ZOOM0001roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>4506KB</t>
+  </si>
+  <si>
+    <t>2.2MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0002roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>2620KB</t>
+  </si>
+  <si>
+    <t>2.6MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0003roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>1174KB</t>
+  </si>
+  <si>
+    <t>1.2MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0004roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>839KB</t>
+  </si>
+  <si>
+    <t>838.9KB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0005roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>2399KB</t>
+  </si>
+  <si>
+    <t>2.3MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0006roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>808KB</t>
+  </si>
+  <si>
+    <t>808.0KB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0007roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>1041KB</t>
+  </si>
+  <si>
+    <t>1.0MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0008roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>1562KB</t>
+  </si>
+  <si>
+    <t>1.5MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0009roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>3317KB</t>
+  </si>
+  <si>
+    <t>3.2MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0010roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>2032KB</t>
+  </si>
+  <si>
+    <t>2.0MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0011roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>3583KB</t>
+  </si>
+  <si>
+    <t>3.5MB/s</t>
+  </si>
+  <si>
+    <t>ZOOM0012roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>3985KB</t>
+  </si>
+  <si>
+    <t>ZOOM0013roxhillsessions20150930.mp3</t>
+  </si>
+  <si>
+    <t>3720KB</t>
+  </si>
+  <si>
+    <t>1.8MB/s</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 1</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 2</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 3</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 4</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 5</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 6</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 7</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 8</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 9</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 10</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 11</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 12</t>
+  </si>
+  <si>
+    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 13</t>
   </si>
 </sst>
 </file>
@@ -2621,7 +2776,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="226">
+  <cellStyleXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2848,15 +3003,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="226">
+  <cellStyles count="229">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3043,6 +3202,9 @@
     <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3411,440 +3573,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>365</v>
+        <v>845</v>
       </c>
       <c r="B1" t="s">
-        <v>744</v>
+        <v>883</v>
       </c>
       <c r="C1" t="str">
-        <f>"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
-        <v>{'file':'Vinyl-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 1'},</v>
+        <f t="shared" ref="C1:C13" si="0">"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
+        <v>{'file':'ZOOM0001roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 1'},</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>356</v>
+        <v>848</v>
       </c>
       <c r="B2" t="s">
-        <v>745</v>
+        <v>884</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C10" si="0">"{'file':'"&amp;A2&amp;"','title':'"&amp;B2&amp;"'},"</f>
-        <v>{'file':'Vinyl_1-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 2'},</v>
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0002roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 2'},</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>357</v>
+        <v>851</v>
       </c>
       <c r="B3" t="s">
-        <v>746</v>
+        <v>885</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_2-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 3'},</v>
+        <v>{'file':'ZOOM0003roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 3'},</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>854</v>
       </c>
       <c r="B4" t="s">
-        <v>747</v>
+        <v>886</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_3-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 4'},</v>
+        <v>{'file':'ZOOM0004roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 4'},</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>359</v>
+        <v>857</v>
       </c>
       <c r="B5" t="s">
-        <v>748</v>
+        <v>887</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_4-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 5'},</v>
+        <v>{'file':'ZOOM0005roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 5'},</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>360</v>
+        <v>860</v>
       </c>
       <c r="B6" t="s">
-        <v>749</v>
+        <v>888</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_5-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 6'},</v>
+        <v>{'file':'ZOOM0006roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 6'},</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>361</v>
+        <v>863</v>
       </c>
       <c r="B7" t="s">
-        <v>750</v>
+        <v>889</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_6-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 7'},</v>
+        <v>{'file':'ZOOM0007roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 7'},</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>362</v>
+        <v>866</v>
       </c>
       <c r="B8" t="s">
-        <v>751</v>
+        <v>890</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_7-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 8'},</v>
+        <v>{'file':'ZOOM0008roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 8'},</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>363</v>
+        <v>869</v>
       </c>
       <c r="B9" t="s">
-        <v>752</v>
+        <v>891</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_8-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 9'},</v>
+        <v>{'file':'ZOOM0009roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 9'},</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>364</v>
+        <v>872</v>
       </c>
       <c r="B10" t="s">
-        <v>753</v>
+        <v>892</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>{'file':'Vinyl_9-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 10'},</v>
+        <v>{'file':'ZOOM0010roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 10'},</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>346</v>
+        <v>875</v>
       </c>
       <c r="B11" t="s">
-        <v>754</v>
+        <v>893</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ref="C11:C20" si="1">"{'file':'"&amp;A11&amp;"','title':'"&amp;B11&amp;"'},"</f>
-        <v>{'file':'Vinyl_10-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 11'},</v>
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0011roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 11'},</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>347</v>
+        <v>878</v>
       </c>
       <c r="B12" t="s">
-        <v>755</v>
+        <v>894</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_11-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 12'},</v>
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0012roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 12'},</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>348</v>
+        <v>880</v>
       </c>
       <c r="B13" t="s">
-        <v>756</v>
+        <v>895</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_12-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 13'},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>349</v>
-      </c>
-      <c r="B14" t="s">
-        <v>757</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_13-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 14'},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>350</v>
-      </c>
-      <c r="B15" t="s">
-        <v>758</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_14-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 15'},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>351</v>
-      </c>
-      <c r="B16" t="s">
-        <v>759</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_15-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 16'},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17" t="s">
-        <v>760</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_16-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 17'},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>353</v>
-      </c>
-      <c r="B18" t="s">
-        <v>761</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_17-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 18'},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>354</v>
-      </c>
-      <c r="B19" t="s">
-        <v>762</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_18-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 19'},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>355</v>
-      </c>
-      <c r="B20" t="s">
-        <v>763</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'Vinyl_19-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 20'},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>367</v>
-      </c>
-      <c r="B21" t="s">
-        <v>764</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" ref="C21" si="2">"{'file':'"&amp;A21&amp;"','title':'"&amp;B21&amp;"'},"</f>
-        <v>{'file':'ZOOM0001-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 1'},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>369</v>
-      </c>
-      <c r="B22" t="s">
-        <v>765</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" ref="C22:C35" si="3">"{'file':'"&amp;A22&amp;"','title':'"&amp;B22&amp;"'},"</f>
-        <v>{'file':'ZOOM0002-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 2'},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>371</v>
-      </c>
-      <c r="B23" t="s">
-        <v>766</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0003-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 3'},</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>373</v>
-      </c>
-      <c r="B24" t="s">
-        <v>767</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0004-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 4'},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>375</v>
-      </c>
-      <c r="B25" t="s">
-        <v>768</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0005-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 5'},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>376</v>
-      </c>
-      <c r="B26" t="s">
-        <v>769</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0006-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 6'},</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>377</v>
-      </c>
-      <c r="B27" t="s">
-        <v>770</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0007-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 7'},</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>378</v>
-      </c>
-      <c r="B28" t="s">
-        <v>771</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0008-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 8'},</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>379</v>
-      </c>
-      <c r="B29" t="s">
-        <v>772</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0009-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 9'},</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>380</v>
-      </c>
-      <c r="B30" t="s">
-        <v>773</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0010-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 10'},</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>381</v>
-      </c>
-      <c r="B31" t="s">
-        <v>774</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0011-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 11'},</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>382</v>
-      </c>
-      <c r="B32" t="s">
-        <v>775</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0012-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 12'},</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>383</v>
-      </c>
-      <c r="B33" t="s">
-        <v>776</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0013-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 13'},</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>384</v>
-      </c>
-      <c r="B34" t="s">
-        <v>777</v>
-      </c>
-      <c r="C34" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0014-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 14'},</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>385</v>
-      </c>
-      <c r="B35" t="s">
-        <v>778</v>
-      </c>
-      <c r="C35" t="str">
-        <f t="shared" si="3"/>
-        <v>{'file':'ZOOM0015-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 15'},</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>703</v>
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0013roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 13'},</v>
       </c>
     </row>
   </sheetData>
@@ -3859,6 +3753,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I278"/>
   <sheetViews>
@@ -7880,7 +7791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -8028,7 +7939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -8291,7 +8202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -8426,7 +8337,698 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>845</v>
+      </c>
+      <c r="B1" s="5">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D1" t="s">
+        <v>847</v>
+      </c>
+      <c r="E1" s="4">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>849</v>
+      </c>
+      <c r="D2" t="s">
+        <v>850</v>
+      </c>
+      <c r="E2" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>851</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>852</v>
+      </c>
+      <c r="D3" t="s">
+        <v>853</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>854</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>855</v>
+      </c>
+      <c r="D4" t="s">
+        <v>856</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>857</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>858</v>
+      </c>
+      <c r="D5" t="s">
+        <v>859</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>860</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>861</v>
+      </c>
+      <c r="D6" t="s">
+        <v>862</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>863</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>864</v>
+      </c>
+      <c r="D7" t="s">
+        <v>865</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>866</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>867</v>
+      </c>
+      <c r="D8" t="s">
+        <v>868</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>869</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>870</v>
+      </c>
+      <c r="D9" t="s">
+        <v>871</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>872</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>873</v>
+      </c>
+      <c r="D10" t="s">
+        <v>874</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>875</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>876</v>
+      </c>
+      <c r="D11" t="s">
+        <v>877</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>878</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>879</v>
+      </c>
+      <c r="D12" t="s">
+        <v>874</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>880</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>881</v>
+      </c>
+      <c r="D13" t="s">
+        <v>882</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
+        <v>{'file':'Vinyl-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 1'},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C10" si="0">"{'file':'"&amp;A2&amp;"','title':'"&amp;B2&amp;"'},"</f>
+        <v>{'file':'Vinyl_1-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 2'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_2-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 3'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B4" t="s">
+        <v>747</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_3-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 4'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5" t="s">
+        <v>748</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_4-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 5'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_5-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 6'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7" t="s">
+        <v>750</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_6-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 7'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_7-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 8'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" t="s">
+        <v>752</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_8-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 9'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" t="s">
+        <v>753</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'Vinyl_9-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 10'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>346</v>
+      </c>
+      <c r="B11" t="s">
+        <v>754</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" ref="C11:C20" si="1">"{'file':'"&amp;A11&amp;"','title':'"&amp;B11&amp;"'},"</f>
+        <v>{'file':'Vinyl_10-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 11'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>347</v>
+      </c>
+      <c r="B12" t="s">
+        <v>755</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_11-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 12'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" t="s">
+        <v>756</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_12-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 13'},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>349</v>
+      </c>
+      <c r="B14" t="s">
+        <v>757</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_13-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 14'},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>350</v>
+      </c>
+      <c r="B15" t="s">
+        <v>758</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_14-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 15'},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>351</v>
+      </c>
+      <c r="B16" t="s">
+        <v>759</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_15-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 16'},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" t="s">
+        <v>760</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_16-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 17'},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B18" t="s">
+        <v>761</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_17-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 18'},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19" t="s">
+        <v>762</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_18-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 19'},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B20" t="s">
+        <v>763</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'Vinyl_19-zeke-elcorazon-2013.mp3','title':'Zeke - El Corazon - 2013 - 20'},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>367</v>
+      </c>
+      <c r="B21" t="s">
+        <v>764</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" ref="C21" si="2">"{'file':'"&amp;A21&amp;"','title':'"&amp;B21&amp;"'},"</f>
+        <v>{'file':'ZOOM0001-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 1'},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>369</v>
+      </c>
+      <c r="B22" t="s">
+        <v>765</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" ref="C22:C35" si="3">"{'file':'"&amp;A22&amp;"','title':'"&amp;B22&amp;"'},"</f>
+        <v>{'file':'ZOOM0002-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 2'},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23" t="s">
+        <v>766</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0003-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 3'},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>373</v>
+      </c>
+      <c r="B24" t="s">
+        <v>767</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0004-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 4'},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>375</v>
+      </c>
+      <c r="B25" t="s">
+        <v>768</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0005-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 5'},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>376</v>
+      </c>
+      <c r="B26" t="s">
+        <v>769</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0006-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 6'},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>377</v>
+      </c>
+      <c r="B27" t="s">
+        <v>770</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0007-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 7'},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>378</v>
+      </c>
+      <c r="B28" t="s">
+        <v>771</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0008-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 8'},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>379</v>
+      </c>
+      <c r="B29" t="s">
+        <v>772</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0009-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 9'},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>380</v>
+      </c>
+      <c r="B30" t="s">
+        <v>773</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0010-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 10'},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>381</v>
+      </c>
+      <c r="B31" t="s">
+        <v>774</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0011-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 11'},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>382</v>
+      </c>
+      <c r="B32" t="s">
+        <v>775</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0012-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 12'},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>383</v>
+      </c>
+      <c r="B33" t="s">
+        <v>776</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0013-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 13'},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>384</v>
+      </c>
+      <c r="B34" t="s">
+        <v>777</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0014-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 14'},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>385</v>
+      </c>
+      <c r="B35" t="s">
+        <v>778</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="3"/>
+        <v>{'file':'ZOOM0015-zeke-highline-20140822.mp3','title':'Zeke - Highline - August 22nd, 2014 - 15'},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>703</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -8786,11 +9388,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C19"/>
     </sheetView>
   </sheetViews>
@@ -8807,7 +9409,7 @@
         <v>719</v>
       </c>
       <c r="C1" t="str">
-        <f>"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
+        <f t="shared" ref="C1:C19" si="0">"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
         <v>{'file':'01%20marklanegan-showbox-20140703-01.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 1'},</v>
       </c>
     </row>
@@ -8819,7 +9421,7 @@
         <v>720</v>
       </c>
       <c r="C2" t="str">
-        <f>"{'file':'"&amp;A2&amp;"','title':'"&amp;B2&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'02%20marklanegan-showbox-20140703-02.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 2'},</v>
       </c>
     </row>
@@ -8831,7 +9433,7 @@
         <v>721</v>
       </c>
       <c r="C3" t="str">
-        <f>"{'file':'"&amp;A3&amp;"','title':'"&amp;B3&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'03%20marklanegan-showbox-20140703-03.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 3'},</v>
       </c>
     </row>
@@ -8843,7 +9445,7 @@
         <v>722</v>
       </c>
       <c r="C4" t="str">
-        <f>"{'file':'"&amp;A4&amp;"','title':'"&amp;B4&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'04%20marklanegan-showbox-20140703-04.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 4'},</v>
       </c>
     </row>
@@ -8855,7 +9457,7 @@
         <v>723</v>
       </c>
       <c r="C5" t="str">
-        <f>"{'file':'"&amp;A5&amp;"','title':'"&amp;B5&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'05%20marklanegan-showbox-20140703-05.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 5'},</v>
       </c>
     </row>
@@ -8867,7 +9469,7 @@
         <v>724</v>
       </c>
       <c r="C6" t="str">
-        <f>"{'file':'"&amp;A6&amp;"','title':'"&amp;B6&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'06%20marklanegan-showbox-20140703-06.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 6'},</v>
       </c>
     </row>
@@ -8879,7 +9481,7 @@
         <v>725</v>
       </c>
       <c r="C7" t="str">
-        <f>"{'file':'"&amp;A7&amp;"','title':'"&amp;B7&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'07%20marklanegan-showbox-20140703-07.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 7'},</v>
       </c>
     </row>
@@ -8891,7 +9493,7 @@
         <v>726</v>
       </c>
       <c r="C8" t="str">
-        <f>"{'file':'"&amp;A8&amp;"','title':'"&amp;B8&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'08%20marklanegan-showbox-20140703-08.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 8'},</v>
       </c>
     </row>
@@ -8903,7 +9505,7 @@
         <v>727</v>
       </c>
       <c r="C9" t="str">
-        <f>"{'file':'"&amp;A9&amp;"','title':'"&amp;B9&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'09%20marklanegan-showbox-20140703-09.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 9'},</v>
       </c>
     </row>
@@ -8915,7 +9517,7 @@
         <v>728</v>
       </c>
       <c r="C10" t="str">
-        <f>"{'file':'"&amp;A10&amp;"','title':'"&amp;B10&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'10%20marklanegan-showbox-20140703-10.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 10'},</v>
       </c>
     </row>
@@ -8927,7 +9529,7 @@
         <v>729</v>
       </c>
       <c r="C11" t="str">
-        <f>"{'file':'"&amp;A11&amp;"','title':'"&amp;B11&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'11%20marklanegan-showbox-20140703-11.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 11'},</v>
       </c>
     </row>
@@ -8939,7 +9541,7 @@
         <v>730</v>
       </c>
       <c r="C12" t="str">
-        <f>"{'file':'"&amp;A12&amp;"','title':'"&amp;B12&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'12%20marklanegan-showbox-20140703-12.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 12'},</v>
       </c>
     </row>
@@ -8951,7 +9553,7 @@
         <v>731</v>
       </c>
       <c r="C13" t="str">
-        <f>"{'file':'"&amp;A13&amp;"','title':'"&amp;B13&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'13%20marklanegan-showbox-20140703-13.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 13'},</v>
       </c>
     </row>
@@ -8963,7 +9565,7 @@
         <v>732</v>
       </c>
       <c r="C14" t="str">
-        <f>"{'file':'"&amp;A14&amp;"','title':'"&amp;B14&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'14%20marklanegan-showbox-20140703-14.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 14'},</v>
       </c>
     </row>
@@ -8975,7 +9577,7 @@
         <v>733</v>
       </c>
       <c r="C15" t="str">
-        <f>"{'file':'"&amp;A15&amp;"','title':'"&amp;B15&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'15%20marklanegan-showbox-20140703-15.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 15'},</v>
       </c>
     </row>
@@ -8987,7 +9589,7 @@
         <v>734</v>
       </c>
       <c r="C16" t="str">
-        <f>"{'file':'"&amp;A16&amp;"','title':'"&amp;B16&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'16%20marklanegan-showbox-20140703-16.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 16'},</v>
       </c>
     </row>
@@ -8999,7 +9601,7 @@
         <v>735</v>
       </c>
       <c r="C17" t="str">
-        <f>"{'file':'"&amp;A17&amp;"','title':'"&amp;B17&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'17%20marklanegan-showbox-20140703-17.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 17'},</v>
       </c>
     </row>
@@ -9011,7 +9613,7 @@
         <v>736</v>
       </c>
       <c r="C18" t="str">
-        <f>"{'file':'"&amp;A18&amp;"','title':'"&amp;B18&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'18%20marklanegan-showbox-20140703-18.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 18'},</v>
       </c>
     </row>
@@ -9023,7 +9625,7 @@
         <v>737</v>
       </c>
       <c r="C19" t="str">
-        <f>"{'file':'"&amp;A19&amp;"','title':'"&amp;B19&amp;"'},"</f>
+        <f t="shared" si="0"/>
         <v>{'file':'19%20marklanegan-showbox-20140703-19.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 19'},</v>
       </c>
     </row>
@@ -9035,7 +9637,7 @@
         <v>738</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" ref="C20:C22" si="0">"{'file':'"&amp;A20&amp;"','title':'"&amp;B20&amp;"'},"</f>
+        <f t="shared" ref="C20:C22" si="1">"{'file':'"&amp;A20&amp;"','title':'"&amp;B20&amp;"'},"</f>
         <v>{'file':'IMG_0763-1024x768.jpg','title':'Mark Lanegan 1'},</v>
       </c>
     </row>
@@ -9047,7 +9649,7 @@
         <v>739</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{'file':'IMG_0764-1024x768.jpg','title':'Mark Lanegan 2'},</v>
       </c>
     </row>
@@ -9059,7 +9661,7 @@
         <v>740</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>{'file':'IMG_0768-1024x768.jpg','title':'Mark Lanegan 3'},</v>
       </c>
     </row>
@@ -9226,7 +9828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -9370,7 +9972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H87"/>
   <sheetViews>
@@ -10450,7 +11052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -10750,7 +11352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
@@ -11507,7 +12109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
@@ -12227,21 +12829,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated scratch spreadsheet with one song name for roxhill session 2
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="865"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="865"/>
   </bookViews>
   <sheets>
     <sheet name="roxhillJSON" sheetId="19" r:id="rId1"/>
@@ -2684,9 +2684,6 @@
     <t>1.8MB/s</t>
   </si>
   <si>
-    <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 1</t>
-  </si>
-  <si>
     <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 2</t>
   </si>
   <si>
@@ -2721,6 +2718,9 @@
   </si>
   <si>
     <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 13</t>
+  </si>
+  <si>
+    <t>Are We Really Gonna Spit at This?</t>
   </si>
 </sst>
 </file>
@@ -3576,13 +3576,13 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3590,11 +3590,11 @@
         <v>845</v>
       </c>
       <c r="B1" t="s">
-        <v>883</v>
+        <v>895</v>
       </c>
       <c r="C1" t="str">
         <f t="shared" ref="C1:C13" si="0">"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
-        <v>{'file':'ZOOM0001roxhillsessions20150930.mp3','title':'Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 1'},</v>
+        <v>{'file':'ZOOM0001roxhillsessions20150930.mp3','title':'Are We Really Gonna Spit at This?'},</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3602,7 +3602,7 @@
         <v>848</v>
       </c>
       <c r="B2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="0"/>
@@ -3614,7 +3614,7 @@
         <v>851</v>
       </c>
       <c r="B3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -3626,7 +3626,7 @@
         <v>854</v>
       </c>
       <c r="B4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -3638,7 +3638,7 @@
         <v>857</v>
       </c>
       <c r="B5" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -3650,7 +3650,7 @@
         <v>860</v>
       </c>
       <c r="B6" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -3662,7 +3662,7 @@
         <v>863</v>
       </c>
       <c r="B7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3674,7 +3674,7 @@
         <v>866</v>
       </c>
       <c r="B8" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3686,7 +3686,7 @@
         <v>869</v>
       </c>
       <c r="B9" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3698,7 +3698,7 @@
         <v>872</v>
       </c>
       <c r="B10" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3710,7 +3710,7 @@
         <v>875</v>
       </c>
       <c r="B11" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -3722,7 +3722,7 @@
         <v>878</v>
       </c>
       <c r="B12" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -3734,7 +3734,7 @@
         <v>880</v>
       </c>
       <c r="B13" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
added a sheet for method signatures
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="865"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="865" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="roxhillJSON" sheetId="19" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="OPTIONvideo" sheetId="7" r:id="rId12"/>
     <sheet name="OPTIONvideo (2)" sheetId="9" r:id="rId13"/>
     <sheet name="IMG" sheetId="3" r:id="rId14"/>
-    <sheet name="Sheet2" sheetId="20" r:id="rId15"/>
+    <sheet name="Functions" sheetId="20" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="894">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -2573,117 +2573,42 @@
     <t>ZOOM0001roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>4506KB</t>
-  </si>
-  <si>
-    <t>2.2MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0002roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>2620KB</t>
-  </si>
-  <si>
-    <t>2.6MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0003roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>1174KB</t>
-  </si>
-  <si>
-    <t>1.2MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0004roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>839KB</t>
-  </si>
-  <si>
-    <t>838.9KB/s</t>
-  </si>
-  <si>
     <t>ZOOM0005roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>2399KB</t>
-  </si>
-  <si>
-    <t>2.3MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0006roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>808KB</t>
-  </si>
-  <si>
-    <t>808.0KB/s</t>
-  </si>
-  <si>
     <t>ZOOM0007roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>1041KB</t>
-  </si>
-  <si>
-    <t>1.0MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0008roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>1562KB</t>
-  </si>
-  <si>
-    <t>1.5MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0009roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>3317KB</t>
-  </si>
-  <si>
-    <t>3.2MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0010roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>2032KB</t>
-  </si>
-  <si>
-    <t>2.0MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0011roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>3583KB</t>
-  </si>
-  <si>
-    <t>3.5MB/s</t>
-  </si>
-  <si>
     <t>ZOOM0012roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>3985KB</t>
-  </si>
-  <si>
     <t>ZOOM0013roxhillsessions20150930.mp3</t>
   </si>
   <si>
-    <t>3720KB</t>
-  </si>
-  <si>
-    <t>1.8MB/s</t>
-  </si>
-  <si>
     <t>Roxhill Sessions - Roxhill Bridge, Seattle - September 30th, 2015 - 2</t>
   </si>
   <si>
@@ -2721,6 +2646,75 @@
   </si>
   <si>
     <t>Are We Really Gonna Spit at This?</t>
+  </si>
+  <si>
+    <t>function onBaseTapSocketEventDots(tapMsgObject){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            objectTimerId = startShapeObjectTimerUp(circleId,"cx","cy",shapeInterval);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            objectTimerId = startShapeObjectTimerDown(circleId,"cx","cy",shapeInterval);</t>
+  </si>
+  <si>
+    <t>function onBaseTapSocketEventLines(tapMsgObject){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            objectTimerId = startShapeObjectTimerUp(lineId,"x1","y1",shapeInterval);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            objectTimerId = startShapeObjectTimerDown(lineId,"x1","y1",shapeInterval);</t>
+  </si>
+  <si>
+    <t>function onBaseTapSocketEventCustom(tapMsgObject){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                onBaseTapSocketEventImages(tapMsgObject,tapMsgObject.customimage);</t>
+  </si>
+  <si>
+    <t>function onBaseTapSocketEventImages(tapMsgObject,imagePath){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            objectTimerId = startAnimalObjectTimerUp(animalId,"x","y",animalInterval);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            objectTimerId = startAnimalObjectTimerDown(animalId,"x","y",animalInterval);</t>
+  </si>
+  <si>
+    <t>function startAnimalObjectTimerUp(objectId,xAxisAttr,yAxisAttr,animalInterval){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    var timerId=window.setInterval(moveAnimalObjectUp,animalInterval,objectId,xAxisAttr,yAxisAttr);</t>
+  </si>
+  <si>
+    <t>function startShapeObjectTimerUp(objectId,xAxisAttr,yAxisAttr,shapeInterval){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    var timerId = window.setInterval(moveShapeObjectUp,shapeInterval,objectId,xAxisAttr,yAxisAttr);</t>
+  </si>
+  <si>
+    <t>function startAnimalObjectTimerDown(objectId,xAxisAttr,yAxisAttr,animalInterval){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    var timerId = window.setInterval(moveAnimalObjectDown,animalInterval,objectId,xAxisAttr,yAxisAttr);</t>
+  </si>
+  <si>
+    <t>function startShapeObjectTimerDown(objectId,xAxisAttr,yAxisAttr,shapeInterval){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    var timerId = window.setInterval(moveShapeObjectDown,shapeInterval,objectId,xAxisAttr,yAxisAttr);</t>
+  </si>
+  <si>
+    <t>function moveShapeObjectDown(objectId,xAxisAttr,yAxisAttr) {</t>
+  </si>
+  <si>
+    <t>function moveAnimalObjectUp(objectId,xAxisAttr,yAxisAttr) {</t>
+  </si>
+  <si>
+    <t>function moveAnimalObjectDown(objectId,xAxisAttr,yAxisAttr) {</t>
+  </si>
+  <si>
+    <t>function moveShapeObjectUp(objectId,xAxisAttr,yAxisAttr) {</t>
   </si>
 </sst>
 </file>
@@ -3007,13 +3001,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="229">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3575,7 +3568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3590,7 +3583,7 @@
         <v>845</v>
       </c>
       <c r="B1" t="s">
-        <v>895</v>
+        <v>870</v>
       </c>
       <c r="C1" t="str">
         <f t="shared" ref="C1:C13" si="0">"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
@@ -3599,10 +3592,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B2" t="s">
-        <v>883</v>
+        <v>858</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="0"/>
@@ -3611,10 +3604,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="B3" t="s">
-        <v>884</v>
+        <v>859</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -3623,10 +3616,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="B4" t="s">
-        <v>885</v>
+        <v>860</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -3635,10 +3628,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="B5" t="s">
-        <v>886</v>
+        <v>861</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -3647,10 +3640,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="B6" t="s">
-        <v>887</v>
+        <v>862</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -3659,10 +3652,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>851</v>
+      </c>
+      <c r="B7" t="s">
         <v>863</v>
-      </c>
-      <c r="B7" t="s">
-        <v>888</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3671,10 +3664,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>866</v>
+        <v>852</v>
       </c>
       <c r="B8" t="s">
-        <v>889</v>
+        <v>864</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3683,10 +3676,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>869</v>
+        <v>853</v>
       </c>
       <c r="B9" t="s">
-        <v>890</v>
+        <v>865</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3695,10 +3688,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>872</v>
+        <v>854</v>
       </c>
       <c r="B10" t="s">
-        <v>891</v>
+        <v>866</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3707,10 +3700,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>875</v>
+        <v>855</v>
       </c>
       <c r="B11" t="s">
-        <v>892</v>
+        <v>867</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -3719,10 +3712,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>878</v>
+        <v>856</v>
       </c>
       <c r="B12" t="s">
-        <v>893</v>
+        <v>868</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -3731,10 +3724,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>880</v>
+        <v>857</v>
       </c>
       <c r="B13" t="s">
-        <v>894</v>
+        <v>869</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -8339,234 +8332,159 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="69.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>845</v>
-      </c>
-      <c r="B1" s="5">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>846</v>
-      </c>
-      <c r="D1" t="s">
-        <v>847</v>
-      </c>
-      <c r="E1" s="4">
-        <v>1.3888888888888889E-3</v>
-      </c>
+      <c r="A1" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>848</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>849</v>
-      </c>
-      <c r="D2" t="s">
-        <v>850</v>
-      </c>
-      <c r="E2" s="4">
-        <v>6.9444444444444447E-4</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>851</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>852</v>
-      </c>
-      <c r="D3" t="s">
-        <v>853</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>854</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>855</v>
-      </c>
-      <c r="D4" t="s">
-        <v>856</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>857</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>858</v>
-      </c>
-      <c r="D5" t="s">
-        <v>859</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
+      <c r="A5" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>860</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>861</v>
-      </c>
-      <c r="D6" t="s">
-        <v>862</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
+      <c r="A6" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>863</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>864</v>
-      </c>
-      <c r="D7" t="s">
-        <v>865</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>866</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>867</v>
-      </c>
-      <c r="D8" t="s">
-        <v>868</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
+      <c r="A8" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>869</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>870</v>
-      </c>
-      <c r="D9" t="s">
-        <v>871</v>
-      </c>
-      <c r="E9" s="4">
-        <v>6.9444444444444447E-4</v>
-      </c>
+      <c r="A9" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>872</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>873</v>
-      </c>
-      <c r="D10" t="s">
-        <v>874</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
+      <c r="A10" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>875</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>876</v>
-      </c>
-      <c r="D11" t="s">
-        <v>877</v>
-      </c>
-      <c r="E11" s="4">
-        <v>6.9444444444444447E-4</v>
-      </c>
+      <c r="A11" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>878</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>879</v>
-      </c>
-      <c r="D12" t="s">
-        <v>874</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1.3888888888888889E-3</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>880</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>881</v>
-      </c>
-      <c r="D13" t="s">
-        <v>882</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1.3888888888888889E-3</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
more work to the hit test. getting close
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14520" tabRatio="865" firstSheet="5" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="865" firstSheet="5" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="roxhillJSON" sheetId="19" r:id="rId1"/>
@@ -8335,7 +8335,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added more roxhill songs
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="45120" windowHeight="26320" tabRatio="865"/>
+    <workbookView xWindow="60" yWindow="40" windowWidth="25040" windowHeight="15040" tabRatio="865"/>
   </bookViews>
   <sheets>
     <sheet name="roxhillJSON" sheetId="19" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="1117">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -3366,6 +3366,24 @@
   </si>
   <si>
     <t>06 Eventhough She Got No Bush</t>
+  </si>
+  <si>
+    <t>01roxhillsessions20151101.mp3</t>
+  </si>
+  <si>
+    <t>01roxhillsessions20151102.mp3</t>
+  </si>
+  <si>
+    <t>01roxhillsessions20151103.mp3</t>
+  </si>
+  <si>
+    <t>01 This is Called Roshay</t>
+  </si>
+  <si>
+    <t>02 Rabid Beauboon</t>
+  </si>
+  <si>
+    <t>03 Harry Potters My Bitch</t>
   </si>
 </sst>
 </file>
@@ -3421,7 +3439,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="250">
+  <cellStyleXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3500,6 +3518,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3680,7 +3700,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="77"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="250">
+  <cellStyles count="252">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3891,6 +3911,8 @@
     <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4259,10 +4281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD13"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4279,7 +4301,7 @@
         <v>1105</v>
       </c>
       <c r="C1" t="str">
-        <f t="shared" ref="C1:C6" si="0">"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
+        <f t="shared" ref="C1:C9" si="0">"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
         <v>{'file':'01roxhillsessionssquidwerdthisword20151014.mp3','title':'01 Squidwerd This Word'},</v>
       </c>
     </row>
@@ -4344,7 +4366,40 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'01roxhillsessions20151101.mp3','title':'01 This is Called Roshay'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'01roxhillsessions20151102.mp3','title':'02 Rabid Beauboon'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'01roxhillsessions20151103.mp3','title':'03 Harry Potters My Bitch'},</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
first attempt at star wars stuffed animal war with external background and local images
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="40" windowWidth="25040" windowHeight="15040" tabRatio="865"/>
   </bookViews>
   <sheets>
-    <sheet name="skycriesmaryJSON" sheetId="24" r:id="rId1"/>
+    <sheet name="file title JSON" sheetId="24" r:id="rId1"/>
     <sheet name="image anchors" sheetId="21" r:id="rId2"/>
     <sheet name="roxhillJSON" sheetId="19" r:id="rId3"/>
     <sheet name="zekeJSON" sheetId="4" r:id="rId4"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1104">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -3267,6 +3267,84 @@
   </si>
   <si>
     <t>Sky Cries Mary - Neumos - 2015 - Second Set 08</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Crocodile</t>
+  </si>
+  <si>
+    <t>Darth Vader</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>R2D2</t>
+  </si>
+  <si>
+    <t>I'm tired of these motherfuckin' snakes on this motherfuckin' plane!</t>
+  </si>
+  <si>
+    <t>Storm Trooper</t>
+  </si>
+  <si>
+    <t>You were the chosen one!</t>
+  </si>
+  <si>
+    <t>Yoda</t>
+  </si>
+  <si>
+    <t>gamemedia/cats.png</t>
+  </si>
+  <si>
+    <t>gamemedia/chickens.png</t>
+  </si>
+  <si>
+    <t>gamemedia/crocodiles.png</t>
+  </si>
+  <si>
+    <t>gamemedia/darthvader.png</t>
+  </si>
+  <si>
+    <t>gamemedia/dogs.png</t>
+  </si>
+  <si>
+    <t>gamemedia/lamblambs.png</t>
+  </si>
+  <si>
+    <t>gamemedia/lions.png</t>
+  </si>
+  <si>
+    <t>gamemedia/queen.png</t>
+  </si>
+  <si>
+    <t>gamemedia/r2d2.png</t>
+  </si>
+  <si>
+    <t>gamemedia/snakesonaplane.png</t>
+  </si>
+  <si>
+    <t>gamemedia/stormtrooper.png</t>
+  </si>
+  <si>
+    <t>gamemedia/thechosenone.png</t>
+  </si>
+  <si>
+    <t>gamemedia/yoda.png</t>
   </si>
 </sst>
 </file>
@@ -3322,7 +3400,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="273">
+  <cellStyleXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3401,6 +3479,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3605,7 +3687,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="273">
+  <cellStyles count="277">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3839,6 +3921,10 @@
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4207,10 +4293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62:C69"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4731,7 +4817,7 @@
         <v>790</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" ref="C44:C69" si="1">"{'file':'"&amp;A44&amp;"','title':'"&amp;B44&amp;"'},"</f>
+        <f t="shared" ref="C44:C83" si="1">"{'file':'"&amp;A44&amp;"','title':'"&amp;B44&amp;"'},"</f>
         <v>{'file':'ZOOM0038.jpg','title':'Last Gasp 1'},</v>
       </c>
     </row>
@@ -4955,7 +5041,7 @@
       </c>
       <c r="E64" s="4"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>1066</v>
       </c>
@@ -4968,7 +5054,7 @@
       </c>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>1067</v>
       </c>
@@ -4981,7 +5067,7 @@
       </c>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>1068</v>
       </c>
@@ -4994,7 +5080,7 @@
       </c>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>1069</v>
       </c>
@@ -5007,7 +5093,7 @@
       </c>
       <c r="E68" s="4"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>1062</v>
       </c>
@@ -5018,6 +5104,174 @@
         <f t="shared" si="1"/>
         <v>{'file':'skycriesmaryneumos201508.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 08'},</v>
       </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/cats.png','title':'Cat'},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/chickens.png','title':'Chicken'},</v>
+      </c>
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/crocodiles.png','title':'Crocodile'},</v>
+      </c>
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/darthvader.png','title':'Darth Vader'},</v>
+      </c>
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/dogs.png','title':'Dog'},</v>
+      </c>
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/lamblambs.png','title':'Lamb'},</v>
+      </c>
+      <c r="H76" s="4"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/lions.png','title':'Lion'},</v>
+      </c>
+      <c r="H77" s="4"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/queen.png','title':'Queen'},</v>
+      </c>
+      <c r="H78" s="4"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/r2d2.png','title':'R2D2'},</v>
+      </c>
+      <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/snakesonaplane.png','title':'I'm tired of these motherfuckin' snakes on this motherfuckin' plane!'},</v>
+      </c>
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/stormtrooper.png','title':'Storm Trooper'},</v>
+      </c>
+      <c r="H81" s="4"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/thechosenone.png','title':'You were the chosen one!'},</v>
+      </c>
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'gamemedia/yoda.png','title':'Yoda'},</v>
+      </c>
+      <c r="H83" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
more changes to make sure sky cries mary still works
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -3296,9 +3296,6 @@
     <t>R2D2</t>
   </si>
   <si>
-    <t>I'm tired of these motherfuckin' snakes on this motherfuckin' plane!</t>
-  </si>
-  <si>
     <t>Storm Trooper</t>
   </si>
   <si>
@@ -3345,6 +3342,9 @@
   </si>
   <si>
     <t>gamemedia/yoda.png</t>
+  </si>
+  <si>
+    <t>Im tired of these motherfuckin stuffed animals on this motherfuckin game!</t>
   </si>
 </sst>
 </file>
@@ -3400,7 +3400,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="277">
+  <cellStyleXfs count="282">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3479,6 +3479,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3687,7 +3692,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="277">
+  <cellStyles count="282">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3925,6 +3930,11 @@
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4293,10 +4303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4809,469 +4819,469 @@
         <v>{'file':'IMG_4558.JPG','title':'Sky Cries Mary - Neumos - 2015 - 042'},</v>
       </c>
     </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>666</v>
+      </c>
+      <c r="B43" t="s">
+        <v>790</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" ref="C43:C73" si="1">"{'file':'"&amp;A43&amp;"','title':'"&amp;B43&amp;"'},"</f>
+        <v>{'file':'ZOOM0038.jpg','title':'Last Gasp 1'},</v>
+      </c>
+    </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B44" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" ref="C44:C83" si="1">"{'file':'"&amp;A44&amp;"','title':'"&amp;B44&amp;"'},"</f>
-        <v>{'file':'ZOOM0038.jpg','title':'Last Gasp 1'},</v>
+        <f t="shared" si="1"/>
+        <v>{'file':'ZOOM0039.jpg','title':'Last Gasp 2'},</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B45" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0039.jpg','title':'Last Gasp 2'},</v>
+        <v>{'file':'ZOOM0040.jpg','title':'Last Gasp 3'},</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B46" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0040.jpg','title':'Last Gasp 3'},</v>
+        <v>{'file':'ZOOM0041.jpg','title':'Last Gasp 4'},</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B47" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0041.jpg','title':'Last Gasp 4'},</v>
+        <v>{'file':'ZOOM0042.jpg','title':'Last Gasp 5'},</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B48" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0042.jpg','title':'Last Gasp 5'},</v>
+        <v>{'file':'ZOOM0043.jpg','title':'Last Gasp 6'},</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B49" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0043.jpg','title':'Last Gasp 6'},</v>
+        <v>{'file':'ZOOM0044.jpg','title':'Last Gasp 7'},</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B50" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0044.jpg','title':'Last Gasp 7'},</v>
+        <v>{'file':'ZOOM0045.jpg','title':'Last Gasp 8'},</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B51" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0045.jpg','title':'Last Gasp 8'},</v>
+        <v>{'file':'ZOOM0046.jpg','title':'Last Gasp 9'},</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B52" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0046.jpg','title':'Last Gasp 9'},</v>
+        <v>{'file':'ZOOM0047.jpg','title':'Last Gasp 10'},</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B53" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0047.jpg','title':'Last Gasp 10'},</v>
+        <v>{'file':'ZOOM0048.jpg','title':'Last Gasp 11'},</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B54" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0048.jpg','title':'Last Gasp 11'},</v>
+        <v>{'file':'ZOOM0049.jpg','title':'Last Gasp 12'},</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B55" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0049.jpg','title':'Last Gasp 12'},</v>
+        <v>{'file':'ZOOM0050.jpg','title':'Last Gasp 13'},</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B56" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0050.jpg','title':'Last Gasp 13'},</v>
+        <v>{'file':'ZOOM0051.jpg','title':'Last Gasp 14'},</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>679</v>
-      </c>
-      <c r="B57" t="s">
-        <v>803</v>
+        <v>1058</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>1060</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'ZOOM0051.jpg','title':'Last Gasp 14'},</v>
+        <v>{'file':'IMG_4516.mp4','title':'Sky Cries Mary - Neumos - 2015 - Video01'},</v>
+      </c>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'IMG_4519.mp4','title':'Sky Cries Mary - Neumos - 2015 - Video02'},</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>1058</v>
+        <v>1063</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>1060</v>
+        <v>1070</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'IMG_4516.mp4','title':'Sky Cries Mary - Neumos - 2015 - Video01'},</v>
+        <v>{'file':'skycriesmaryneumos201501.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 01'},</v>
       </c>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>1059</v>
+        <v>1064</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>1061</v>
+        <v>1071</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'IMG_4519.mp4','title':'Sky Cries Mary - Neumos - 2015 - Video02'},</v>
-      </c>
+        <v>{'file':'skycriesmaryneumos201502.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 02'},</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="1"/>
+        <v>{'file':'skycriesmaryneumos201503.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 03'},</v>
+      </c>
+      <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201501.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 01'},</v>
+        <v>{'file':'skycriesmaryneumos201504.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 04'},</v>
       </c>
       <c r="E62" s="4"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>1064</v>
+        <v>1067</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201502.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 02'},</v>
+        <v>{'file':'skycriesmaryneumos201505.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 05'},</v>
       </c>
       <c r="E63" s="4"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>1065</v>
+        <v>1068</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201503.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 03'},</v>
+        <v>{'file':'skycriesmaryneumos201506.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 06'},</v>
       </c>
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>1073</v>
+        <v>1076</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201504.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 04'},</v>
+        <v>{'file':'skycriesmaryneumos201507.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 07'},</v>
       </c>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>1067</v>
+        <v>1062</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201505.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 05'},</v>
-      </c>
-      <c r="E66" s="4"/>
+        <v>{'file':'skycriesmaryneumos201508.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 08'},</v>
+      </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>1068</v>
+        <v>1093</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>1075</v>
+        <v>1081</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201506.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 06'},</v>
-      </c>
-      <c r="E67" s="4"/>
+        <f>"{'file':'"&amp;A67&amp;"','title':'"&amp;B67&amp;"'},"</f>
+        <v>{'file':'gamemedia/darthvader.png','title':'Darth Vader'},</v>
+      </c>
+      <c r="H67" s="4"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>1069</v>
+        <v>1097</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>1076</v>
+        <v>1085</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201507.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 07'},</v>
-      </c>
-      <c r="E68" s="4"/>
+        <v>{'file':'gamemedia/queen.png','title':'Queen'},</v>
+      </c>
+      <c r="H68" s="4"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>1062</v>
+        <v>1099</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>1077</v>
+        <v>1103</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'skycriesmaryneumos201508.mp3','title':'Sky Cries Mary - Neumos - 2015 - Second Set 08'},</v>
-      </c>
+        <v>{'file':'gamemedia/snakesonaplane.png','title':'Im tired of these motherfuckin stuffed animals on this motherfuckin game!'},</v>
+      </c>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C70" t="str">
+        <f>"{'file':'"&amp;A70&amp;"','title':'"&amp;B70&amp;"'},"</f>
+        <v>{'file':'gamemedia/r2d2.png','title':'R2D2'},</v>
+      </c>
+      <c r="H70" s="4"/>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>1091</v>
+        <v>1100</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>1078</v>
+        <v>1087</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/cats.png','title':'Cat'},</v>
-      </c>
+        <v>{'file':'gamemedia/stormtrooper.png','title':'Storm Trooper'},</v>
+      </c>
+      <c r="H71" s="4"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>1092</v>
+        <v>1101</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>1079</v>
+        <v>1088</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/chickens.png','title':'Chicken'},</v>
+        <v>{'file':'gamemedia/thechosenone.png','title':'You were the chosen one!'},</v>
       </c>
       <c r="H72" s="4"/>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>1093</v>
+        <v>1102</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>1080</v>
+        <v>1089</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/crocodiles.png','title':'Crocodile'},</v>
+        <v>{'file':'gamemedia/yoda.png','title':'Yoda'},</v>
       </c>
       <c r="H73" s="4"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/darthvader.png','title':'Darth Vader'},</v>
-      </c>
-      <c r="H74" s="4"/>
+        <f>"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
+        <v>{'file':'gamemedia/cats.png','title':'Cat'},</v>
+      </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/dogs.png','title':'Dog'},</v>
+        <f>"{'file':'"&amp;A75&amp;"','title':'"&amp;B75&amp;"'},"</f>
+        <v>{'file':'gamemedia/chickens.png','title':'Chicken'},</v>
       </c>
       <c r="H75" s="4"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/lamblambs.png','title':'Lamb'},</v>
+        <f>"{'file':'"&amp;A76&amp;"','title':'"&amp;B76&amp;"'},"</f>
+        <v>{'file':'gamemedia/crocodiles.png','title':'Crocodile'},</v>
       </c>
       <c r="H76" s="4"/>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/lions.png','title':'Lion'},</v>
+        <f>"{'file':'"&amp;A77&amp;"','title':'"&amp;B77&amp;"'},"</f>
+        <v>{'file':'gamemedia/dogs.png','title':'Dog'},</v>
       </c>
       <c r="H77" s="4"/>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/queen.png','title':'Queen'},</v>
+        <f>"{'file':'"&amp;A78&amp;"','title':'"&amp;B78&amp;"'},"</f>
+        <v>{'file':'gamemedia/lamblambs.png','title':'Lamb'},</v>
       </c>
       <c r="H78" s="4"/>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/r2d2.png','title':'R2D2'},</v>
+        <f>"{'file':'"&amp;A79&amp;"','title':'"&amp;B79&amp;"'},"</f>
+        <v>{'file':'gamemedia/lions.png','title':'Lion'},</v>
       </c>
       <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>1087</v>
-      </c>
-      <c r="C80" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/snakesonaplane.png','title':'I'm tired of these motherfuckin' snakes on this motherfuckin' plane!'},</v>
-      </c>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>1088</v>
-      </c>
-      <c r="C81" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/stormtrooper.png','title':'Storm Trooper'},</v>
-      </c>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>1089</v>
-      </c>
-      <c r="C82" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/thechosenone.png','title':'You were the chosen one!'},</v>
-      </c>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C83" t="str">
-        <f t="shared" si="1"/>
-        <v>{'file':'gamemedia/yoda.png','title':'Yoda'},</v>
-      </c>
-      <c r="H83" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added roxhill local songs
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="40" windowWidth="25040" windowHeight="15040" tabRatio="865"/>
+    <workbookView xWindow="25700" yWindow="160" windowWidth="37980" windowHeight="20440" tabRatio="865"/>
   </bookViews>
   <sheets>
     <sheet name="file title JSON" sheetId="24" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="1118">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -3345,6 +3345,48 @@
   </si>
   <si>
     <t>Im tired of these motherfuckin stuffed animals on this motherfuckin game!</t>
+  </si>
+  <si>
+    <t>Bats Do It.mp3</t>
+  </si>
+  <si>
+    <t>Cannabalistic Attack.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delirious.mp3    </t>
+  </si>
+  <si>
+    <t>God Knowledge.mp3</t>
+  </si>
+  <si>
+    <t>Hella Buckarooni.mp3</t>
+  </si>
+  <si>
+    <t>Hop Off This Beat.mp3</t>
+  </si>
+  <si>
+    <t>Just Beau By Himself.mp3</t>
+  </si>
+  <si>
+    <t>Bats Do It</t>
+  </si>
+  <si>
+    <t>Cannibalistic Attack</t>
+  </si>
+  <si>
+    <t>Delirious</t>
+  </si>
+  <si>
+    <t>God Knowledge</t>
+  </si>
+  <si>
+    <t>Hella Buckarooni</t>
+  </si>
+  <si>
+    <t>Hop Off This Beat</t>
+  </si>
+  <si>
+    <t>Just Beau By Himself</t>
   </si>
 </sst>
 </file>
@@ -3400,7 +3442,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="282">
+  <cellStyleXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3479,6 +3521,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3692,7 +3736,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="282">
+  <cellStyles count="284">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3935,6 +3979,8 @@
     <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4303,10 +4349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5214,7 +5260,7 @@
         <v>1078</v>
       </c>
       <c r="C74" t="str">
-        <f>"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
+        <f t="shared" ref="C74:C86" si="2">"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
         <v>{'file':'gamemedia/cats.png','title':'Cat'},</v>
       </c>
     </row>
@@ -5226,7 +5272,7 @@
         <v>1079</v>
       </c>
       <c r="C75" t="str">
-        <f>"{'file':'"&amp;A75&amp;"','title':'"&amp;B75&amp;"'},"</f>
+        <f t="shared" si="2"/>
         <v>{'file':'gamemedia/chickens.png','title':'Chicken'},</v>
       </c>
       <c r="H75" s="4"/>
@@ -5239,7 +5285,7 @@
         <v>1080</v>
       </c>
       <c r="C76" t="str">
-        <f>"{'file':'"&amp;A76&amp;"','title':'"&amp;B76&amp;"'},"</f>
+        <f t="shared" si="2"/>
         <v>{'file':'gamemedia/crocodiles.png','title':'Crocodile'},</v>
       </c>
       <c r="H76" s="4"/>
@@ -5252,7 +5298,7 @@
         <v>1082</v>
       </c>
       <c r="C77" t="str">
-        <f>"{'file':'"&amp;A77&amp;"','title':'"&amp;B77&amp;"'},"</f>
+        <f t="shared" si="2"/>
         <v>{'file':'gamemedia/dogs.png','title':'Dog'},</v>
       </c>
       <c r="H77" s="4"/>
@@ -5265,7 +5311,7 @@
         <v>1083</v>
       </c>
       <c r="C78" t="str">
-        <f>"{'file':'"&amp;A78&amp;"','title':'"&amp;B78&amp;"'},"</f>
+        <f t="shared" si="2"/>
         <v>{'file':'gamemedia/lamblambs.png','title':'Lamb'},</v>
       </c>
       <c r="H78" s="4"/>
@@ -5278,10 +5324,94 @@
         <v>1084</v>
       </c>
       <c r="C79" t="str">
-        <f>"{'file':'"&amp;A79&amp;"','title':'"&amp;B79&amp;"'},"</f>
+        <f t="shared" si="2"/>
         <v>{'file':'gamemedia/lions.png','title':'Lion'},</v>
       </c>
       <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'Bats Do It.mp3','title':'Bats Do It'},</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'Cannabalistic Attack.mp3','title':'Cannibalistic Attack'},</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'Delirious.mp3    ','title':'Delirious'},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'God Knowledge.mp3','title':'God Knowledge'},</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'Hella Buckarooni.mp3','title':'Hella Buckarooni'},</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'Hop Off This Beat.mp3','title':'Hop Off This Beat'},</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'Just Beau By Himself.mp3','title':'Just Beau By Himself'},</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
mix page for helena
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1156">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -3387,6 +3387,120 @@
   </si>
   <si>
     <t>Just Beau By Himself</t>
+  </si>
+  <si>
+    <t>airplanejivetalkersfoodsickwithjunecleaver.mp4</t>
+  </si>
+  <si>
+    <t>airplanejivetalkers.mp4</t>
+  </si>
+  <si>
+    <t>Airplane Movie -Jive Talkers</t>
+  </si>
+  <si>
+    <t>Airplane Movie -Jive Talkers Order Food</t>
+  </si>
+  <si>
+    <t>Airplane Movie -Jive Talkers Sick with June Cleaver</t>
+  </si>
+  <si>
+    <t>airplanejivetalkersorderfood.mp4</t>
+  </si>
+  <si>
+    <t>01 Here To Fall.mp3</t>
+  </si>
+  <si>
+    <t>03 By Twos.mp3</t>
+  </si>
+  <si>
+    <t>04 Nothing To Hide.mp3</t>
+  </si>
+  <si>
+    <t>02 Avalon Or Someone Very Similar.mp3</t>
+  </si>
+  <si>
+    <t>05 Periodically Triple Or Double.mp3</t>
+  </si>
+  <si>
+    <t>07 Im On My Way.mp3</t>
+  </si>
+  <si>
+    <t>08 When Its Dark.mp3</t>
+  </si>
+  <si>
+    <t>09 All Your Secrets.mp3</t>
+  </si>
+  <si>
+    <t>10 More Stars Than There Are In Heaven.mp3</t>
+  </si>
+  <si>
+    <t>11 The Fireside.mp3</t>
+  </si>
+  <si>
+    <t>IMG_4599.JPG</t>
+  </si>
+  <si>
+    <t>IMG_4659.JPG</t>
+  </si>
+  <si>
+    <t>IMG_4675.JPG</t>
+  </si>
+  <si>
+    <t>IMG_4575.JPG</t>
+  </si>
+  <si>
+    <t>IMG_4691.JPG</t>
+  </si>
+  <si>
+    <t>Here to Fall</t>
+  </si>
+  <si>
+    <t>Avalon Or Someone Very Similar</t>
+  </si>
+  <si>
+    <t>By Twos</t>
+  </si>
+  <si>
+    <t>Nothing to Hide</t>
+  </si>
+  <si>
+    <t>Periodically Triple Or Double</t>
+  </si>
+  <si>
+    <t>If Its True</t>
+  </si>
+  <si>
+    <t>Im On My Way</t>
+  </si>
+  <si>
+    <t>When Its Dark</t>
+  </si>
+  <si>
+    <t>All Your Secrets</t>
+  </si>
+  <si>
+    <t>More Stars Than There Are In Heaven</t>
+  </si>
+  <si>
+    <t>The Fireside</t>
+  </si>
+  <si>
+    <t>Leaf Blower</t>
+  </si>
+  <si>
+    <t>Good Luck Kitteh!</t>
+  </si>
+  <si>
+    <t>Good Boy!</t>
+  </si>
+  <si>
+    <t>Kitteh Mehowh</t>
+  </si>
+  <si>
+    <t>Daffodil</t>
+  </si>
+  <si>
+    <t>06 If Its True.mp3</t>
   </si>
 </sst>
 </file>
@@ -3442,7 +3556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="284">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3521,6 +3635,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3736,7 +3867,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="284">
+  <cellStyles count="301">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3981,6 +4112,23 @@
     <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4349,15 +4497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101:C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="58.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5260,7 +5408,7 @@
         <v>1078</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" ref="C74:C86" si="2">"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
+        <f t="shared" ref="C74:C105" si="2">"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
         <v>{'file':'gamemedia/cats.png','title':'Cat'},</v>
       </c>
     </row>
@@ -5411,6 +5559,234 @@
       <c r="C86" t="str">
         <f t="shared" si="2"/>
         <v>{'file':'Just Beau By Himself.mp3','title':'Just Beau By Himself'},</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'airplanejivetalkersfoodsickwithjunecleaver.mp4','title':'Airplane Movie -Jive Talkers Sick with June Cleaver'},</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'airplanejivetalkers.mp4','title':'Airplane Movie -Jive Talkers'},</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'airplanejivetalkersorderfood.mp4','title':'Airplane Movie -Jive Talkers Order Food'},</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'01 Here To Fall.mp3','title':'Here to Fall'},</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'02 Avalon Or Someone Very Similar.mp3','title':'Avalon Or Someone Very Similar'},</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'03 By Twos.mp3','title':'By Twos'},</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'04 Nothing To Hide.mp3','title':'Nothing to Hide'},</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'05 Periodically Triple Or Double.mp3','title':'Periodically Triple Or Double'},</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'06 If Its True.mp3','title':'If Its True'},</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'07 Im On My Way.mp3','title':'Im On My Way'},</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'08 When Its Dark.mp3','title':'When Its Dark'},</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'09 All Your Secrets.mp3','title':'All Your Secrets'},</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'10 More Stars Than There Are In Heaven.mp3','title':'More Stars Than There Are In Heaven'},</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'11 The Fireside.mp3','title':'The Fireside'},</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_4599.JPG','title':'Kitteh Mehowh'},</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_4659.JPG','title':'Daffodil'},</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_4675.JPG','title':'Good Luck Kitteh!'},</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_4575.JPG','title':'Good Boy!'},</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_4691.JPG','title':'Leaf Blower'},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed background to last gasp
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25700" yWindow="160" windowWidth="37980" windowHeight="20440" tabRatio="865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="865"/>
   </bookViews>
   <sheets>
     <sheet name="file title JSON" sheetId="24" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1164">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -3501,6 +3501,30 @@
   </si>
   <si>
     <t>06 If Its True.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IMG_0054rotated.m4v</t>
+  </si>
+  <si>
+    <t>IMG_0055.m4v</t>
+  </si>
+  <si>
+    <t>IMG_0056.m4v</t>
+  </si>
+  <si>
+    <t>IMG_0059.m4v</t>
+  </si>
+  <si>
+    <t>IMG_0069rotated.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jim-marginal-overthelight-march2015.mp4</t>
+  </si>
+  <si>
+    <t>Marginal - Jim over the light</t>
+  </si>
+  <si>
+    <t>Marginal?</t>
   </si>
 </sst>
 </file>
@@ -3556,7 +3580,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="301">
+  <cellStyleXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3635,6 +3659,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3867,7 +3892,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="301">
+  <cellStyles count="302">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4129,6 +4154,7 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4497,10 +4523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101:C105"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105:C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5408,7 +5434,7 @@
         <v>1078</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" ref="C74:C105" si="2">"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
+        <f t="shared" ref="C74:C111" si="2">"{'file':'"&amp;A74&amp;"','title':'"&amp;B74&amp;"'},"</f>
         <v>{'file':'gamemedia/cats.png','title':'Cat'},</v>
       </c>
     </row>
@@ -5787,6 +5813,78 @@
       <c r="C105" t="str">
         <f t="shared" si="2"/>
         <v>{'file':'IMG_4691.JPG','title':'Leaf Blower'},</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':' IMG_0054rotated.m4v','title':'Marginal?'},</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_0055.m4v','title':'Marginal?'},</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_0056.m4v','title':'Marginal?'},</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_0059.m4v','title':'Marginal?'},</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':'IMG_0069rotated.m4v','title':'Marginal?'},</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="2"/>
+        <v>{'file':' jim-marginal-overthelight-march2015.mp4','title':'Marginal - Jim over the light'},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue of no dj worky
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3144" uniqueCount="1506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="1542">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -4517,40 +4517,148 @@
     <t>14ride2015.mp3</t>
   </si>
   <si>
-    <t>IMG_4733.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4734.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4743.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4748.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4757.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4758.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4759.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4763.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4766.jpg</t>
-  </si>
-  <si>
-    <t>IMG_4767.jpg</t>
-  </si>
-  <si>
     <t>Leave Them All Behind</t>
   </si>
   <si>
     <t>Twisterella</t>
+  </si>
+  <si>
+    <t>03 YYZ.mp3</t>
+  </si>
+  <si>
+    <t>blondie-callme-7inch.mp3</t>
+  </si>
+  <si>
+    <t>03%20YYZ.mp3</t>
+  </si>
+  <si>
+    <t>ride01</t>
+  </si>
+  <si>
+    <t>ride02</t>
+  </si>
+  <si>
+    <t>rush xyz</t>
+  </si>
+  <si>
+    <t>ride03</t>
+  </si>
+  <si>
+    <t>ride04</t>
+  </si>
+  <si>
+    <t>ride05</t>
+  </si>
+  <si>
+    <t>ride06</t>
+  </si>
+  <si>
+    <t>ride07</t>
+  </si>
+  <si>
+    <t>ride08</t>
+  </si>
+  <si>
+    <t>ride09</t>
+  </si>
+  <si>
+    <t>ride10</t>
+  </si>
+  <si>
+    <t>ride11</t>
+  </si>
+  <si>
+    <t>ride12</t>
+  </si>
+  <si>
+    <t>ride13</t>
+  </si>
+  <si>
+    <t>ride14</t>
+  </si>
+  <si>
+    <t>Ride01</t>
+  </si>
+  <si>
+    <t>Ride02</t>
+  </si>
+  <si>
+    <t>Rush YYZ</t>
+  </si>
+  <si>
+    <t>Ride03</t>
+  </si>
+  <si>
+    <t>Ride04</t>
+  </si>
+  <si>
+    <t>Ride05</t>
+  </si>
+  <si>
+    <t>Ride 06</t>
+  </si>
+  <si>
+    <t>Ride07</t>
+  </si>
+  <si>
+    <t>Ride08</t>
+  </si>
+  <si>
+    <t>Ride09</t>
+  </si>
+  <si>
+    <t>Ride10</t>
+  </si>
+  <si>
+    <t>Ride11</t>
+  </si>
+  <si>
+    <t>Ride12</t>
+  </si>
+  <si>
+    <t>Ride13</t>
+  </si>
+  <si>
+    <t>Ride14</t>
+  </si>
+  <si>
+    <t>Blondie-Call Me</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-Here To Fall</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-Avalon Or Someone Very Similar</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-By Twos</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-Nothing To Hide</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-Periodically Triple Or Double</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-If Its True</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-Im On My Way</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-When Its Dark</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-All Your Secrets</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-More Stars Than There Are In Heaven</t>
+  </si>
+  <si>
+    <t>Yo La Tengo-The Fireside</t>
+  </si>
+  <si>
+    <t>Skerik Trio-Owl n Thistle</t>
   </si>
 </sst>
 </file>
@@ -4630,7 +4738,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="317">
+  <cellStyleXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4709,6 +4817,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4960,7 +5074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="317">
+  <cellStyles count="323">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5238,6 +5352,12 @@
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5606,10 +5726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H687"/>
+  <dimension ref="A1:H720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A653" workbookViewId="0">
-      <selection activeCell="B666" sqref="B666"/>
+    <sheetView tabSelected="1" topLeftCell="A693" workbookViewId="0">
+      <selection activeCell="C693" sqref="C693:C720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7950,7 +8070,7 @@
         <v>1177</v>
       </c>
       <c r="C193" t="str">
-        <f t="shared" ref="C193:C256" si="3">"{'file':'"&amp;A193&amp;"','title':'"&amp;B193&amp;"'},"</f>
+        <f t="shared" ref="C193:C255" si="3">"{'file':'"&amp;A193&amp;"','title':'"&amp;B193&amp;"'},"</f>
         <v>{'file':'cincodemargo/IMG_0566.m4v','title':'./cincodemargo/IMG_0566.m4v'},</v>
       </c>
     </row>
@@ -13314,7 +13434,7 @@
         <v>383</v>
       </c>
       <c r="C640" s="7" t="str">
-        <f t="shared" ref="C640:C677" si="10">"{'file':'"&amp;A640&amp;"','title':'"&amp;B640&amp;"'},"</f>
+        <f t="shared" ref="C640:C720" si="10">"{'file':'"&amp;A640&amp;"','title':'"&amp;B640&amp;"'},"</f>
         <v>{'file':'ZOOM0038-lastgasp-highline-2014.mp3','title':'ZOOM0038-lastgasp-highline-2014.mp3'},</v>
       </c>
     </row>
@@ -13599,7 +13719,7 @@
         <v>1480</v>
       </c>
       <c r="B664" t="s">
-        <v>1504</v>
+        <v>1494</v>
       </c>
       <c r="C664" s="8" t="str">
         <f t="shared" si="10"/>
@@ -13611,7 +13731,7 @@
         <v>1481</v>
       </c>
       <c r="B665" t="s">
-        <v>1505</v>
+        <v>1495</v>
       </c>
       <c r="C665" s="8" t="str">
         <f t="shared" si="10"/>
@@ -13764,52 +13884,518 @@
     </row>
     <row r="678" spans="1:3">
       <c r="A678" t="s">
-        <v>1494</v>
+        <v>1480</v>
+      </c>
+      <c r="B678" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C678" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'01ride2015.mp3','title':'ride01'},</v>
       </c>
     </row>
     <row r="679" spans="1:3">
       <c r="A679" t="s">
-        <v>1495</v>
+        <v>1481</v>
+      </c>
+      <c r="B679" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C679" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'02ride2015.mp3','title':'ride02'},</v>
       </c>
     </row>
     <row r="680" spans="1:3">
       <c r="A680" t="s">
-        <v>1496</v>
+        <v>1498</v>
+      </c>
+      <c r="B680" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C680" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'03%20YYZ.mp3','title':'rush xyz'},</v>
       </c>
     </row>
     <row r="681" spans="1:3">
       <c r="A681" t="s">
-        <v>1497</v>
+        <v>1482</v>
+      </c>
+      <c r="B681" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C681" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'03ride2015.mp3','title':'ride03'},</v>
       </c>
     </row>
     <row r="682" spans="1:3">
       <c r="A682" t="s">
-        <v>1498</v>
+        <v>1483</v>
+      </c>
+      <c r="B682" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C682" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'04ride2015.mp3','title':'ride04'},</v>
       </c>
     </row>
     <row r="683" spans="1:3">
       <c r="A683" t="s">
-        <v>1499</v>
+        <v>1484</v>
+      </c>
+      <c r="B683" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C683" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'05ride2015.mp3','title':'ride05'},</v>
       </c>
     </row>
     <row r="684" spans="1:3">
       <c r="A684" t="s">
-        <v>1500</v>
+        <v>1485</v>
+      </c>
+      <c r="B684" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C684" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'06ride2015.mp3','title':'ride06'},</v>
       </c>
     </row>
     <row r="685" spans="1:3">
       <c r="A685" t="s">
-        <v>1501</v>
+        <v>1486</v>
+      </c>
+      <c r="B685" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C685" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'07ride2015.mp3','title':'ride07'},</v>
       </c>
     </row>
     <row r="686" spans="1:3">
       <c r="A686" t="s">
-        <v>1502</v>
+        <v>1487</v>
+      </c>
+      <c r="B686" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C686" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'08ride2015.mp3','title':'ride08'},</v>
       </c>
     </row>
     <row r="687" spans="1:3">
       <c r="A687" t="s">
-        <v>1503</v>
+        <v>1488</v>
+      </c>
+      <c r="B687" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C687" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'09ride2015.mp3','title':'ride09'},</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3">
+      <c r="A688" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B688" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C688" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'10ride2015.mp3','title':'ride10'},</v>
+      </c>
+    </row>
+    <row r="689" spans="1:3">
+      <c r="A689" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B689" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C689" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'11ride2015.mp3','title':'ride11'},</v>
+      </c>
+    </row>
+    <row r="690" spans="1:3">
+      <c r="A690" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B690" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C690" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'12ride2015.mp3','title':'ride12'},</v>
+      </c>
+    </row>
+    <row r="691" spans="1:3">
+      <c r="A691" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B691" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C691" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'13ride2015.mp3','title':'ride13'},</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3">
+      <c r="A692" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B692" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C692" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'14ride2015.mp3','title':'ride14'},</v>
+      </c>
+    </row>
+    <row r="693" spans="1:3">
+      <c r="A693" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B693" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C693" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'ZOOM0012-SkerikTrio-OwlnThistle-20130227.mp3','title':'Skerik Trio-Owl n Thistle'},</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3">
+      <c r="A694" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B694" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C694" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'blondie-callme-7inch.mp3','title':'Blondie-Call Me'},</v>
+      </c>
+    </row>
+    <row r="695" spans="1:3">
+      <c r="A695" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B695" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C695" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'01 Here To Fall.mp3','title':'Yo La Tengo-Here To Fall'},</v>
+      </c>
+    </row>
+    <row r="696" spans="1:3">
+      <c r="A696" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B696" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C696" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'01ride2015.mp3','title':'Ride01'},</v>
+      </c>
+    </row>
+    <row r="697" spans="1:3">
+      <c r="A697" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B697" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C697" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'02 Avalon Or Someone Very Similar.mp3','title':'Yo La Tengo-Avalon Or Someone Very Similar'},</v>
+      </c>
+    </row>
+    <row r="698" spans="1:3">
+      <c r="A698" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B698" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C698" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'02ride2015.mp3','title':'Ride02'},</v>
+      </c>
+    </row>
+    <row r="699" spans="1:3">
+      <c r="A699" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B699" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C699" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'03 By Twos.mp3','title':'Yo La Tengo-By Twos'},</v>
+      </c>
+    </row>
+    <row r="700" spans="1:3">
+      <c r="A700" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B700" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C700" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'03 YYZ.mp3','title':'Rush YYZ'},</v>
+      </c>
+    </row>
+    <row r="701" spans="1:3">
+      <c r="A701" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B701" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C701" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'03ride2015.mp3','title':'Ride03'},</v>
+      </c>
+    </row>
+    <row r="702" spans="1:3">
+      <c r="A702" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B702" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C702" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'04 Nothing To Hide.mp3','title':'Yo La Tengo-Nothing To Hide'},</v>
+      </c>
+    </row>
+    <row r="703" spans="1:3">
+      <c r="A703" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B703" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C703" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'04ride2015.mp3','title':'Ride04'},</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3">
+      <c r="A704" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B704" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C704" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'05 Periodically Triple Or Double.mp3','title':'Yo La Tengo-Periodically Triple Or Double'},</v>
+      </c>
+    </row>
+    <row r="705" spans="1:3">
+      <c r="A705" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B705" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C705" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'05ride2015.mp3','title':'Ride05'},</v>
+      </c>
+    </row>
+    <row r="706" spans="1:3">
+      <c r="A706" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B706" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C706" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'06 If Its True.mp3','title':'Yo La Tengo-If Its True'},</v>
+      </c>
+    </row>
+    <row r="707" spans="1:3">
+      <c r="A707" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B707" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C707" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'06ride2015.mp3','title':'Ride 06'},</v>
+      </c>
+    </row>
+    <row r="708" spans="1:3">
+      <c r="A708" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B708" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C708" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'07 Im On My Way.mp3','title':'Yo La Tengo-Im On My Way'},</v>
+      </c>
+    </row>
+    <row r="709" spans="1:3">
+      <c r="A709" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B709" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C709" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'07ride2015.mp3','title':'Ride07'},</v>
+      </c>
+    </row>
+    <row r="710" spans="1:3">
+      <c r="A710" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B710" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C710" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'08 When Its Dark.mp3','title':'Yo La Tengo-When Its Dark'},</v>
+      </c>
+    </row>
+    <row r="711" spans="1:3">
+      <c r="A711" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B711" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C711" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'08ride2015.mp3','title':'Ride08'},</v>
+      </c>
+    </row>
+    <row r="712" spans="1:3">
+      <c r="A712" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B712" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C712" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'09 All Your Secrets.mp3','title':'Yo La Tengo-All Your Secrets'},</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3">
+      <c r="A713" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B713" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C713" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'09ride2015.mp3','title':'Ride09'},</v>
+      </c>
+    </row>
+    <row r="714" spans="1:3">
+      <c r="A714" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B714" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C714" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'10 More Stars Than There Are In Heaven.mp3','title':'Yo La Tengo-More Stars Than There Are In Heaven'},</v>
+      </c>
+    </row>
+    <row r="715" spans="1:3">
+      <c r="A715" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B715" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C715" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'10ride2015.mp3','title':'Ride10'},</v>
+      </c>
+    </row>
+    <row r="716" spans="1:3">
+      <c r="A716" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B716" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C716" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'11 The Fireside.mp3','title':'Yo La Tengo-The Fireside'},</v>
+      </c>
+    </row>
+    <row r="717" spans="1:3">
+      <c r="A717" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B717" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C717" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'11ride2015.mp3','title':'Ride11'},</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3">
+      <c r="A718" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B718" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C718" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'12ride2015.mp3','title':'Ride12'},</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3">
+      <c r="A719" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B719" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C719" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'13ride2015.mp3','title':'Ride13'},</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3">
+      <c r="A720" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B720" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C720" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v>{'file':'14ride2015.mp3','title':'Ride14'},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first attempt at omlb page
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="865"/>
+    <workbookView xWindow="-80" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="865"/>
   </bookViews>
   <sheets>
     <sheet name="file title JSON" sheetId="24" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="1542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3240" uniqueCount="1562">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -4659,6 +4659,66 @@
   </si>
   <si>
     <t>Skerik Trio-Owl n Thistle</t>
+  </si>
+  <si>
+    <t>03 The Tide Is High.mp3</t>
+  </si>
+  <si>
+    <t>1-07%20I%20Will%20Refuse.mp3</t>
+  </si>
+  <si>
+    <t>1-14%20With%20Teeth%20(Live).mp3</t>
+  </si>
+  <si>
+    <t>Pailhead - I Will Refuse</t>
+  </si>
+  <si>
+    <t>Blondie - The Tide Is High</t>
+  </si>
+  <si>
+    <t>Melvins - With Teeth (Live)</t>
+  </si>
+  <si>
+    <t>02%20Avalon%20Or%20Someone%20Very%20Similar.mp3</t>
+  </si>
+  <si>
+    <t>Yo La Tengo - Avalon Or Someone Very Similar</t>
+  </si>
+  <si>
+    <t>03%20Pass%20The%20Mic.mp3</t>
+  </si>
+  <si>
+    <t>Beastie Boys - Pass the Mic</t>
+  </si>
+  <si>
+    <t>Beastie Boys - Car Thief</t>
+  </si>
+  <si>
+    <t>11%20Car%20Thief.mp3</t>
+  </si>
+  <si>
+    <t>Beck - Black Tambourine</t>
+  </si>
+  <si>
+    <t>12%20Black%20Tambourine%20(Film%20Version).mp3</t>
+  </si>
+  <si>
+    <t>1-01%20Supernaut.mp3</t>
+  </si>
+  <si>
+    <t>1000 Homo DJs - Supernaut</t>
+  </si>
+  <si>
+    <t>03%20In%20Your%20Face.mp3</t>
+  </si>
+  <si>
+    <t>7 Seconds - In Your Face</t>
+  </si>
+  <si>
+    <t>3-01%20Rubber%20Glove%20Seduction.mp3</t>
+  </si>
+  <si>
+    <t>PTP - Rubber Glove Seduction</t>
   </si>
 </sst>
 </file>
@@ -5726,10 +5786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H720"/>
+  <dimension ref="A1:H730"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A693" workbookViewId="0">
-      <selection activeCell="C693" sqref="C693:C720"/>
+    <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
+      <selection activeCell="A721" sqref="A721:XFD730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13434,7 +13494,7 @@
         <v>383</v>
       </c>
       <c r="C640" s="7" t="str">
-        <f t="shared" ref="C640:C720" si="10">"{'file':'"&amp;A640&amp;"','title':'"&amp;B640&amp;"'},"</f>
+        <f t="shared" ref="C640:C726" si="10">"{'file':'"&amp;A640&amp;"','title':'"&amp;B640&amp;"'},"</f>
         <v>{'file':'ZOOM0038-lastgasp-highline-2014.mp3','title':'ZOOM0038-lastgasp-highline-2014.mp3'},</v>
       </c>
     </row>
@@ -14062,7 +14122,7 @@
         <v>{'file':'14ride2015.mp3','title':'ride14'},</v>
       </c>
     </row>
-    <row r="693" spans="1:3">
+    <row r="693" spans="1:3" hidden="1">
       <c r="A693" t="s">
         <v>1438</v>
       </c>
@@ -14074,7 +14134,7 @@
         <v>{'file':'ZOOM0012-SkerikTrio-OwlnThistle-20130227.mp3','title':'Skerik Trio-Owl n Thistle'},</v>
       </c>
     </row>
-    <row r="694" spans="1:3">
+    <row r="694" spans="1:3" hidden="1">
       <c r="A694" t="s">
         <v>1497</v>
       </c>
@@ -14086,7 +14146,7 @@
         <v>{'file':'blondie-callme-7inch.mp3','title':'Blondie-Call Me'},</v>
       </c>
     </row>
-    <row r="695" spans="1:3">
+    <row r="695" spans="1:3" hidden="1">
       <c r="A695" t="s">
         <v>1044</v>
       </c>
@@ -14098,7 +14158,7 @@
         <v>{'file':'01 Here To Fall.mp3','title':'Yo La Tengo-Here To Fall'},</v>
       </c>
     </row>
-    <row r="696" spans="1:3">
+    <row r="696" spans="1:3" hidden="1">
       <c r="A696" t="s">
         <v>1480</v>
       </c>
@@ -14110,7 +14170,7 @@
         <v>{'file':'01ride2015.mp3','title':'Ride01'},</v>
       </c>
     </row>
-    <row r="697" spans="1:3">
+    <row r="697" spans="1:3" hidden="1">
       <c r="A697" t="s">
         <v>1047</v>
       </c>
@@ -14122,7 +14182,7 @@
         <v>{'file':'02 Avalon Or Someone Very Similar.mp3','title':'Yo La Tengo-Avalon Or Someone Very Similar'},</v>
       </c>
     </row>
-    <row r="698" spans="1:3">
+    <row r="698" spans="1:3" hidden="1">
       <c r="A698" t="s">
         <v>1481</v>
       </c>
@@ -14134,7 +14194,7 @@
         <v>{'file':'02ride2015.mp3','title':'Ride02'},</v>
       </c>
     </row>
-    <row r="699" spans="1:3">
+    <row r="699" spans="1:3" hidden="1">
       <c r="A699" t="s">
         <v>1045</v>
       </c>
@@ -14146,7 +14206,7 @@
         <v>{'file':'03 By Twos.mp3','title':'Yo La Tengo-By Twos'},</v>
       </c>
     </row>
-    <row r="700" spans="1:3">
+    <row r="700" spans="1:3" hidden="1">
       <c r="A700" t="s">
         <v>1496</v>
       </c>
@@ -14158,7 +14218,7 @@
         <v>{'file':'03 YYZ.mp3','title':'Rush YYZ'},</v>
       </c>
     </row>
-    <row r="701" spans="1:3">
+    <row r="701" spans="1:3" hidden="1">
       <c r="A701" t="s">
         <v>1482</v>
       </c>
@@ -14170,7 +14230,7 @@
         <v>{'file':'03ride2015.mp3','title':'Ride03'},</v>
       </c>
     </row>
-    <row r="702" spans="1:3">
+    <row r="702" spans="1:3" hidden="1">
       <c r="A702" t="s">
         <v>1046</v>
       </c>
@@ -14182,7 +14242,7 @@
         <v>{'file':'04 Nothing To Hide.mp3','title':'Yo La Tengo-Nothing To Hide'},</v>
       </c>
     </row>
-    <row r="703" spans="1:3">
+    <row r="703" spans="1:3" hidden="1">
       <c r="A703" t="s">
         <v>1483</v>
       </c>
@@ -14194,7 +14254,7 @@
         <v>{'file':'04ride2015.mp3','title':'Ride04'},</v>
       </c>
     </row>
-    <row r="704" spans="1:3">
+    <row r="704" spans="1:3" hidden="1">
       <c r="A704" t="s">
         <v>1048</v>
       </c>
@@ -14206,7 +14266,7 @@
         <v>{'file':'05 Periodically Triple Or Double.mp3','title':'Yo La Tengo-Periodically Triple Or Double'},</v>
       </c>
     </row>
-    <row r="705" spans="1:3">
+    <row r="705" spans="1:3" hidden="1">
       <c r="A705" t="s">
         <v>1484</v>
       </c>
@@ -14218,7 +14278,7 @@
         <v>{'file':'05ride2015.mp3','title':'Ride05'},</v>
       </c>
     </row>
-    <row r="706" spans="1:3">
+    <row r="706" spans="1:3" hidden="1">
       <c r="A706" t="s">
         <v>1075</v>
       </c>
@@ -14230,7 +14290,7 @@
         <v>{'file':'06 If Its True.mp3','title':'Yo La Tengo-If Its True'},</v>
       </c>
     </row>
-    <row r="707" spans="1:3">
+    <row r="707" spans="1:3" hidden="1">
       <c r="A707" t="s">
         <v>1485</v>
       </c>
@@ -14242,7 +14302,7 @@
         <v>{'file':'06ride2015.mp3','title':'Ride 06'},</v>
       </c>
     </row>
-    <row r="708" spans="1:3">
+    <row r="708" spans="1:3" hidden="1">
       <c r="A708" t="s">
         <v>1049</v>
       </c>
@@ -14254,7 +14314,7 @@
         <v>{'file':'07 Im On My Way.mp3','title':'Yo La Tengo-Im On My Way'},</v>
       </c>
     </row>
-    <row r="709" spans="1:3">
+    <row r="709" spans="1:3" hidden="1">
       <c r="A709" t="s">
         <v>1486</v>
       </c>
@@ -14266,7 +14326,7 @@
         <v>{'file':'07ride2015.mp3','title':'Ride07'},</v>
       </c>
     </row>
-    <row r="710" spans="1:3">
+    <row r="710" spans="1:3" hidden="1">
       <c r="A710" t="s">
         <v>1050</v>
       </c>
@@ -14278,7 +14338,7 @@
         <v>{'file':'08 When Its Dark.mp3','title':'Yo La Tengo-When Its Dark'},</v>
       </c>
     </row>
-    <row r="711" spans="1:3">
+    <row r="711" spans="1:3" hidden="1">
       <c r="A711" t="s">
         <v>1487</v>
       </c>
@@ -14290,7 +14350,7 @@
         <v>{'file':'08ride2015.mp3','title':'Ride08'},</v>
       </c>
     </row>
-    <row r="712" spans="1:3">
+    <row r="712" spans="1:3" hidden="1">
       <c r="A712" t="s">
         <v>1051</v>
       </c>
@@ -14302,7 +14362,7 @@
         <v>{'file':'09 All Your Secrets.mp3','title':'Yo La Tengo-All Your Secrets'},</v>
       </c>
     </row>
-    <row r="713" spans="1:3">
+    <row r="713" spans="1:3" hidden="1">
       <c r="A713" t="s">
         <v>1488</v>
       </c>
@@ -14314,7 +14374,7 @@
         <v>{'file':'09ride2015.mp3','title':'Ride09'},</v>
       </c>
     </row>
-    <row r="714" spans="1:3">
+    <row r="714" spans="1:3" hidden="1">
       <c r="A714" t="s">
         <v>1052</v>
       </c>
@@ -14326,7 +14386,7 @@
         <v>{'file':'10 More Stars Than There Are In Heaven.mp3','title':'Yo La Tengo-More Stars Than There Are In Heaven'},</v>
       </c>
     </row>
-    <row r="715" spans="1:3">
+    <row r="715" spans="1:3" hidden="1">
       <c r="A715" t="s">
         <v>1489</v>
       </c>
@@ -14338,7 +14398,7 @@
         <v>{'file':'10ride2015.mp3','title':'Ride10'},</v>
       </c>
     </row>
-    <row r="716" spans="1:3">
+    <row r="716" spans="1:3" hidden="1">
       <c r="A716" t="s">
         <v>1053</v>
       </c>
@@ -14350,7 +14410,7 @@
         <v>{'file':'11 The Fireside.mp3','title':'Yo La Tengo-The Fireside'},</v>
       </c>
     </row>
-    <row r="717" spans="1:3">
+    <row r="717" spans="1:3" hidden="1">
       <c r="A717" t="s">
         <v>1490</v>
       </c>
@@ -14362,7 +14422,7 @@
         <v>{'file':'11ride2015.mp3','title':'Ride11'},</v>
       </c>
     </row>
-    <row r="718" spans="1:3">
+    <row r="718" spans="1:3" hidden="1">
       <c r="A718" t="s">
         <v>1491</v>
       </c>
@@ -14374,7 +14434,7 @@
         <v>{'file':'12ride2015.mp3','title':'Ride12'},</v>
       </c>
     </row>
-    <row r="719" spans="1:3">
+    <row r="719" spans="1:3" hidden="1">
       <c r="A719" t="s">
         <v>1492</v>
       </c>
@@ -14386,7 +14446,7 @@
         <v>{'file':'13ride2015.mp3','title':'Ride13'},</v>
       </c>
     </row>
-    <row r="720" spans="1:3">
+    <row r="720" spans="1:3" hidden="1">
       <c r="A720" t="s">
         <v>1493</v>
       </c>
@@ -14398,10 +14458,134 @@
         <v>{'file':'14ride2015.mp3','title':'Ride14'},</v>
       </c>
     </row>
+    <row r="721" spans="1:3">
+      <c r="A721" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B721" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C721" s="8" t="str">
+        <f>"{'file':'"&amp;A721&amp;"','title':'"&amp;B721&amp;"'},"</f>
+        <v>{'file':'1-01%20Supernaut.mp3','title':'1000 Homo DJs - Supernaut'},</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3">
+      <c r="A722" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B722" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C722" s="8" t="str">
+        <f>"{'file':'"&amp;A722&amp;"','title':'"&amp;B722&amp;"'},"</f>
+        <v>{'file':'03%20In%20Your%20Face.mp3','title':'7 Seconds - In Your Face'},</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3">
+      <c r="A723" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B723" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C723" s="8" t="str">
+        <f>"{'file':'"&amp;A723&amp;"','title':'"&amp;B723&amp;"'},"</f>
+        <v>{'file':'11%20Car%20Thief.mp3','title':'Beastie Boys - Car Thief'},</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3">
+      <c r="A724" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B724" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C724" s="8" t="str">
+        <f>"{'file':'"&amp;A724&amp;"','title':'"&amp;B724&amp;"'},"</f>
+        <v>{'file':'03%20Pass%20The%20Mic.mp3','title':'Beastie Boys - Pass the Mic'},</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3">
+      <c r="A725" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C725" s="8" t="str">
+        <f>"{'file':'"&amp;A725&amp;"','title':'"&amp;B725&amp;"'},"</f>
+        <v>{'file':'12%20Black%20Tambourine%20(Film%20Version).mp3','title':'Beck - Black Tambourine'},</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3">
+      <c r="A726" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B726" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C726" s="8" t="str">
+        <f>"{'file':'"&amp;A726&amp;"','title':'"&amp;B726&amp;"'},"</f>
+        <v>{'file':'03 The Tide Is High.mp3','title':'Blondie - The Tide Is High'},</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3">
+      <c r="A727" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C727" s="8" t="str">
+        <f>"{'file':'"&amp;A727&amp;"','title':'"&amp;B727&amp;"'},"</f>
+        <v>{'file':'1-14%20With%20Teeth%20(Live).mp3','title':'Melvins - With Teeth (Live)'},</v>
+      </c>
+    </row>
+    <row r="728" spans="1:3">
+      <c r="A728" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B728" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C728" s="8" t="str">
+        <f>"{'file':'"&amp;A728&amp;"','title':'"&amp;B728&amp;"'},"</f>
+        <v>{'file':'1-07%20I%20Will%20Refuse.mp3','title':'Pailhead - I Will Refuse'},</v>
+      </c>
+    </row>
+    <row r="729" spans="1:3">
+      <c r="A729" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B729" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C729" s="8" t="str">
+        <f>"{'file':'"&amp;A729&amp;"','title':'"&amp;B729&amp;"'},"</f>
+        <v>{'file':'3-01%20Rubber%20Glove%20Seduction.mp3','title':'PTP - Rubber Glove Seduction'},</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3">
+      <c r="A730" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B730" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C730" s="8" t="str">
+        <f>"{'file':'"&amp;A730&amp;"','title':'"&amp;B730&amp;"'},"</f>
+        <v>{'file':'02%20Avalon%20Or%20Someone%20Very%20Similar.mp3','title':'Yo La Tengo - Avalon Or Someone Very Similar'},</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:C693">
-    <sortCondition ref="B131"/>
+  <sortState ref="A721:H730">
+    <sortCondition ref="B721:B730"/>
+    <sortCondition ref="A721:A730"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="A726" r:id="rId1" display="digital/03 The Tide Is High.mp3"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
put music first on music pages. and put houston photos on omlb page
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -4798,7 +4798,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="323">
+  <cellStyleXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4877,6 +4877,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5134,7 +5137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="323">
+  <cellStyles count="326">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5418,6 +5421,9 @@
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5789,7 +5795,7 @@
   <dimension ref="A1:H730"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
-      <selection activeCell="A721" sqref="A721:XFD730"/>
+      <selection activeCell="C721" sqref="C721:C730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13494,7 +13500,7 @@
         <v>383</v>
       </c>
       <c r="C640" s="7" t="str">
-        <f t="shared" ref="C640:C726" si="10">"{'file':'"&amp;A640&amp;"','title':'"&amp;B640&amp;"'},"</f>
+        <f t="shared" ref="C640:C720" si="10">"{'file':'"&amp;A640&amp;"','title':'"&amp;B640&amp;"'},"</f>
         <v>{'file':'ZOOM0038-lastgasp-highline-2014.mp3','title':'ZOOM0038-lastgasp-highline-2014.mp3'},</v>
       </c>
     </row>
@@ -14460,122 +14466,122 @@
     </row>
     <row r="721" spans="1:3">
       <c r="A721" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="B721" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="C721" s="8" t="str">
         <f>"{'file':'"&amp;A721&amp;"','title':'"&amp;B721&amp;"'},"</f>
-        <v>{'file':'1-01%20Supernaut.mp3','title':'1000 Homo DJs - Supernaut'},</v>
+        <v>{'file':'11%20Car%20Thief.mp3','title':'Beastie Boys - Car Thief'},</v>
       </c>
     </row>
     <row r="722" spans="1:3">
       <c r="A722" t="s">
-        <v>1558</v>
+        <v>1550</v>
       </c>
       <c r="B722" t="s">
-        <v>1559</v>
+        <v>1551</v>
       </c>
       <c r="C722" s="8" t="str">
         <f>"{'file':'"&amp;A722&amp;"','title':'"&amp;B722&amp;"'},"</f>
-        <v>{'file':'03%20In%20Your%20Face.mp3','title':'7 Seconds - In Your Face'},</v>
+        <v>{'file':'03%20Pass%20The%20Mic.mp3','title':'Beastie Boys - Pass the Mic'},</v>
       </c>
     </row>
     <row r="723" spans="1:3">
       <c r="A723" t="s">
-        <v>1553</v>
+        <v>1555</v>
       </c>
       <c r="B723" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
       <c r="C723" s="8" t="str">
         <f>"{'file':'"&amp;A723&amp;"','title':'"&amp;B723&amp;"'},"</f>
-        <v>{'file':'11%20Car%20Thief.mp3','title':'Beastie Boys - Car Thief'},</v>
+        <v>{'file':'12%20Black%20Tambourine%20(Film%20Version).mp3','title':'Beck - Black Tambourine'},</v>
       </c>
     </row>
     <row r="724" spans="1:3">
-      <c r="A724" t="s">
-        <v>1550</v>
+      <c r="A724" s="3" t="s">
+        <v>1542</v>
       </c>
       <c r="B724" t="s">
-        <v>1551</v>
+        <v>1546</v>
       </c>
       <c r="C724" s="8" t="str">
         <f>"{'file':'"&amp;A724&amp;"','title':'"&amp;B724&amp;"'},"</f>
-        <v>{'file':'03%20Pass%20The%20Mic.mp3','title':'Beastie Boys - Pass the Mic'},</v>
+        <v>{'file':'03 The Tide Is High.mp3','title':'Blondie - The Tide Is High'},</v>
       </c>
     </row>
     <row r="725" spans="1:3">
       <c r="A725" t="s">
-        <v>1555</v>
+        <v>1544</v>
       </c>
       <c r="B725" t="s">
-        <v>1554</v>
+        <v>1547</v>
       </c>
       <c r="C725" s="8" t="str">
         <f>"{'file':'"&amp;A725&amp;"','title':'"&amp;B725&amp;"'},"</f>
-        <v>{'file':'12%20Black%20Tambourine%20(Film%20Version).mp3','title':'Beck - Black Tambourine'},</v>
+        <v>{'file':'1-14%20With%20Teeth%20(Live).mp3','title':'Melvins - With Teeth (Live)'},</v>
       </c>
     </row>
     <row r="726" spans="1:3">
-      <c r="A726" s="3" t="s">
-        <v>1542</v>
+      <c r="A726" t="s">
+        <v>1543</v>
       </c>
       <c r="B726" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C726" s="8" t="str">
         <f>"{'file':'"&amp;A726&amp;"','title':'"&amp;B726&amp;"'},"</f>
-        <v>{'file':'03 The Tide Is High.mp3','title':'Blondie - The Tide Is High'},</v>
+        <v>{'file':'1-07%20I%20Will%20Refuse.mp3','title':'Pailhead - I Will Refuse'},</v>
       </c>
     </row>
     <row r="727" spans="1:3">
       <c r="A727" t="s">
-        <v>1544</v>
+        <v>1560</v>
       </c>
       <c r="B727" t="s">
-        <v>1547</v>
+        <v>1561</v>
       </c>
       <c r="C727" s="8" t="str">
         <f>"{'file':'"&amp;A727&amp;"','title':'"&amp;B727&amp;"'},"</f>
-        <v>{'file':'1-14%20With%20Teeth%20(Live).mp3','title':'Melvins - With Teeth (Live)'},</v>
+        <v>{'file':'3-01%20Rubber%20Glove%20Seduction.mp3','title':'PTP - Rubber Glove Seduction'},</v>
       </c>
     </row>
     <row r="728" spans="1:3">
       <c r="A728" t="s">
-        <v>1543</v>
+        <v>1548</v>
       </c>
       <c r="B728" t="s">
-        <v>1545</v>
+        <v>1549</v>
       </c>
       <c r="C728" s="8" t="str">
         <f>"{'file':'"&amp;A728&amp;"','title':'"&amp;B728&amp;"'},"</f>
-        <v>{'file':'1-07%20I%20Will%20Refuse.mp3','title':'Pailhead - I Will Refuse'},</v>
+        <v>{'file':'02%20Avalon%20Or%20Someone%20Very%20Similar.mp3','title':'Yo La Tengo - Avalon Or Someone Very Similar'},</v>
       </c>
     </row>
     <row r="729" spans="1:3">
       <c r="A729" t="s">
-        <v>1560</v>
+        <v>1556</v>
       </c>
       <c r="B729" t="s">
-        <v>1561</v>
+        <v>1557</v>
       </c>
       <c r="C729" s="8" t="str">
         <f>"{'file':'"&amp;A729&amp;"','title':'"&amp;B729&amp;"'},"</f>
-        <v>{'file':'3-01%20Rubber%20Glove%20Seduction.mp3','title':'PTP - Rubber Glove Seduction'},</v>
+        <v>{'file':'1-01%20Supernaut.mp3','title':'1000 Homo DJs - Supernaut'},</v>
       </c>
     </row>
     <row r="730" spans="1:3">
       <c r="A730" t="s">
-        <v>1548</v>
+        <v>1558</v>
       </c>
       <c r="B730" t="s">
-        <v>1549</v>
+        <v>1559</v>
       </c>
       <c r="C730" s="8" t="str">
         <f>"{'file':'"&amp;A730&amp;"','title':'"&amp;B730&amp;"'},"</f>
-        <v>{'file':'02%20Avalon%20Or%20Someone%20Very%20Similar.mp3','title':'Yo La Tengo - Avalon Or Someone Very Similar'},</v>
+        <v>{'file':'03%20In%20Your%20Face.mp3','title':'7 Seconds - In Your Face'},</v>
       </c>
     </row>
   </sheetData>
@@ -14584,7 +14590,7 @@
     <sortCondition ref="A721:A730"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A726" r:id="rId1" display="digital/03 The Tide Is High.mp3"/>
+    <hyperlink ref="A724" r:id="rId1" display="digital/03 The Tide Is High.mp3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added music and took out apostrophes
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="865" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="865" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="file title JSON" sheetId="24" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3030" uniqueCount="2154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="2260">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -6499,6 +6499,324 @@
   </si>
   <si>
     <t>{'file':'18%20Car-BuiltToSpill-LiveatNeumos20131227.mp3','title':'18Built to Spill - Neumos, Seattle - December 27th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-01.mp3','title':'01 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-02.mp3','title':'02 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-03.mp3','title':'03 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-04.mp3','title':'04 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-05.mp3','title':'05 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-06.mp3','title':'01 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-07.mp3','title':'02 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-08.mp3','title':'03 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-09.mp3','title':'04 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-10.mp3','title':'05 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-11.mp3','title':'06 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-12.mp3','title':'07 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-13.mp3','title':'08 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-14.mp3','title':'09 Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-15.mp3','title':'10Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-16.mp3','title':'11Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-17.mp3','title':'12Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-18.mp3','title':'13Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-19.mp3','title':'14Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-20.mp3','title':'15Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-21.mp3','title':'16Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-22.mp3','title':'17Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-23.mp3','title':'18Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-24.mp3','title':'19Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'cracksabbath20140509-25.mp3','title':'20Crack Sabbath - Darrell's - May 8th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0001-cracksabbath-themix-20130920.mp3','title':'01 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0002-cracksabbath-themix-20130920.mp3','title':'02 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0003-cracksabbath-themix-20130920.mp3','title':'03 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0004-cracksabbath-themix-20130920.mp3','title':'04 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0005-cracksabbath-themix-20130920.mp3','title':'05 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0007-cracksabbath-themix-20130920.mp3','title':'01 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0008-cracksabbath-themix-20130920.mp3','title':'02 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0009-cracksabbath-themix-20130920.mp3','title':'03 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0010-cracksabbath-themix-20130920.mp3','title':'04 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0011-cracksabbath-themix-20130920.mp3','title':'05 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0012-cracksabbath-themix-20130920.mp3','title':'06 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0013-cracksabbath-themix-20130920.mp3','title':'07 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0014-cracksabbath-themix-20130920.mp3','title':'08 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0015-cracksabbath-themix-20130920.mp3','title':'09 Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0016-cracksabbath-themix-20130920.mp3','title':'10Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0017-cracksabbath-themix-20130920.mp3','title':'11Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0018-cracksabbath-themix-20130920.mp3','title':'12Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0019-cracksabbath-themix-20130920.mp3','title':'13Crack Sabbath - The Mix - September 20th, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0002-cracksabbath-owlandthistle-20140917.mp3','title':'01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0003-cracksabbath-owlandthistle-20140917.mp3','title':'02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0004-cracksabbath-owlandthistle-20140917.mp3','title':'03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0005-cracksabbath-owlandthistle-20140917.mp3','title':'04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0006-cracksabbath-owlandthistle-20140917.mp3','title':'05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0007-cracksabbath-owlandthistle-20140917.mp3','title':'01 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0008-cracksabbath-owlandthistle-20140917.mp3','title':'02 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0009-cracksabbath-owlandthistle-20140917.mp3','title':'03 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0010-cracksabbath-owlandthistle-20140917.mp3','title':'04 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0011-cracksabbath-owlandthistle-20140917.mp3','title':'05 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0012-cracksabbath-owlandthistle-20140917.mp3','title':'06 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0013-cracksabbath-owlandthistle-20140917.mp3','title':'07 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0014-cracksabbath-owlandthistle-20140917.mp3','title':'08 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0015-cracksabbath-owlandthistle-20140917.mp3','title':'09 Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0016-cracksabbath-owlandthistle-20140917.mp3','title':'10Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0017-cracksabbath-owlandthistle-20140917.mp3','title':'11Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0018-cracksabbath-owlandthistle-20140917.mp3','title':'12Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0019-cracksabbath-owlandthistle-20140917.mp3','title':'13Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0020-cracksabbath-owlandthistle-20140917.mp3','title':'14Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0021-cracksabbath-owlandthistle-20140917.mp3','title':'15Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0022-cracksabbath-owlandthistle-20140917.mp3','title':'16Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0023-cracksabbath-owlandthistle-20140917.mp3','title':'17Crack Sabbath - Owl 'n Thistle - September 17th, 2014'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0001-CrackSabbath-RoyalRoom-20130622.mp3','title':'01 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0002-CrackSabbath-RoyalRoom-20130622.mp3','title':'2 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0003-CrackSabbath-RoyalRoom-20130622.mp3','title':'3 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0004-CrackSabbath-RoyalRoom-20130622.mp3','title':'4 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0005-CrackSabbath-RoyalRoom-20130622.mp3','title':'5 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0008-CrackSabbath-RoyalRoom-20130622.mp3','title':'6 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0009-CrackSabbath-RoyalRoom-20130622.mp3','title':'7 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0010-CrackSabbath-RoyalRoom-20130622.mp3','title':'8 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0011-CrackSabbath-RoyalRoom-20130622.mp3','title':'9 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0012-CrackSabbath-RoyalRoom-20130622.mp3','title':'10 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0013-CrackSabbath-RoyalRoom-20130622.mp3','title':'11 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0014-CrackSabbath-RoyalRoom-20130622.mp3','title':'12 Crack Sabbath - Royal Room - June 22nd, 2013'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0001-cracksabbath.jpg','title':'Crack Sabbath Photo 7'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0002-cracksabbath.jpg','title':'Crack Sabbath Photo 8'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0003-cracksabbath.jpg','title':'Crack Sabbath Photo 9'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0004-cracksabbath.jpg','title':'Crack Sabbath Photo 10'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0005-cracksabbath.jpg','title':'Crack Sabbath Photo 11'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0006-cracksabbath.jpg','title':'Crack Sabbath Photo 12'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0007-cracksabbath.jpg','title':'Crack Sabbath Photo 13'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0008-cracksabbath.jpg','title':'Crack Sabbath Photo 14'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0009-cracksabbath.jpg','title':'Crack Sabbath Photo 15'},</t>
+  </si>
+  <si>
+    <t>{'file':'ZOOM0010-cracksabbath.jpg','title':'Crack Sabbath Photo 16'},</t>
+  </si>
+  <si>
+    <t>{'file':'01%20marklanegan-showbox-20140703-01.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 1'},</t>
+  </si>
+  <si>
+    <t>{'file':'02%20marklanegan-showbox-20140703-02.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 2'},</t>
+  </si>
+  <si>
+    <t>{'file':'03%20marklanegan-showbox-20140703-03.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 3'},</t>
+  </si>
+  <si>
+    <t>{'file':'04%20marklanegan-showbox-20140703-04.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 4'},</t>
+  </si>
+  <si>
+    <t>{'file':'05%20marklanegan-showbox-20140703-05.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 5'},</t>
+  </si>
+  <si>
+    <t>{'file':'06%20marklanegan-showbox-20140703-06.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 6'},</t>
+  </si>
+  <si>
+    <t>{'file':'07%20marklanegan-showbox-20140703-07.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 7'},</t>
+  </si>
+  <si>
+    <t>{'file':'08%20marklanegan-showbox-20140703-08.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 8'},</t>
+  </si>
+  <si>
+    <t>{'file':'09%20marklanegan-showbox-20140703-09.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 9'},</t>
+  </si>
+  <si>
+    <t>{'file':'10%20marklanegan-showbox-20140703-10.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 10'},</t>
+  </si>
+  <si>
+    <t>{'file':'11%20marklanegan-showbox-20140703-11.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 11'},</t>
+  </si>
+  <si>
+    <t>{'file':'12%20marklanegan-showbox-20140703-12.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 12'},</t>
+  </si>
+  <si>
+    <t>{'file':'13%20marklanegan-showbox-20140703-13.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 13'},</t>
+  </si>
+  <si>
+    <t>{'file':'14%20marklanegan-showbox-20140703-14.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 14'},</t>
+  </si>
+  <si>
+    <t>{'file':'15%20marklanegan-showbox-20140703-15.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 15'},</t>
+  </si>
+  <si>
+    <t>{'file':'16%20marklanegan-showbox-20140703-16.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 16'},</t>
+  </si>
+  <si>
+    <t>{'file':'17%20marklanegan-showbox-20140703-17.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 17'},</t>
+  </si>
+  <si>
+    <t>{'file':'18%20marklanegan-showbox-20140703-18.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 18'},</t>
+  </si>
+  <si>
+    <t>{'file':'19%20marklanegan-showbox-20140703-19.mp3','title':'Mark Lanegan - Showbox Market, Seattle - July 3rd, 2014 - 19'},</t>
   </si>
 </sst>
 </file>
@@ -22398,677 +22716,1207 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A133"/>
+  <dimension ref="A1:A239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A133" sqref="A1:A133"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121:XFD139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2021</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2022</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2023</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2024</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2025</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2026</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2027</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2028</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2029</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2030</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>2031</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2032</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>2033</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2034</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>2035</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2036</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>2037</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2038</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2039</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2040</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>2041</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>2042</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2043</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>2044</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2045</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2046</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>2047</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>2048</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>2049</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>2050</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>2051</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>2052</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>2053</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>2054</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>2055</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>2056</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>2057</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>2058</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>2059</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>2060</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>2061</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>2062</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>2063</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>2064</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>2065</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>2066</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>2067</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>2068</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2069</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>2070</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>2071</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>2072</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>2073</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>2074</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>2075</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>2076</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>2077</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>2078</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>2079</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>2080</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>2081</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>2082</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>2083</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>2084</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>2085</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>2086</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>2087</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>2088</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>2089</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>2090</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>2091</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>2092</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>2093</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>2094</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>2095</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>2096</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>2097</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>2098</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>2099</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>2100</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>2101</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>2102</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>2103</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>2104</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>2105</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>2106</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>2107</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>2108</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>2109</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>2110</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>2111</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>2112</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>2113</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>2114</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>2115</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>2116</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>2117</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>2118</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>2119</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>2120</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>2121</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>2122</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>2123</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>2124</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>2125</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>2126</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>2127</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>2128</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>2129</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>2130</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>2131</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>2132</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>2133</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>2134</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>2135</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>2136</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>2137</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>2138</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>2139</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>2140</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>2141</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>2142</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>2143</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>2144</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>2145</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>2146</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>2147</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>2148</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>2149</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>2150</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>2151</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>2152</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>2153</v>
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>2055</v>
       </c>
     </row>
   </sheetData>
@@ -24454,7 +25302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A71" workbookViewId="0">
       <selection activeCell="C87" sqref="C1:C87"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added videows to skatecreteordie
</commit_message>
<xml_diff>
--- a/stuffedanimalwar.com/scratch.xlsx
+++ b/stuffedanimalwar.com/scratch.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="865"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="file title JSON" sheetId="24" r:id="rId1"/>
-    <sheet name="roxhillJSON" sheetId="19" r:id="rId2"/>
-    <sheet name="houston2015" sheetId="26" r:id="rId3"/>
-    <sheet name="zekeJSON" sheetId="4" r:id="rId4"/>
-    <sheet name="lastgaspJSON" sheetId="16" r:id="rId5"/>
-    <sheet name="marklaneganJSON" sheetId="17" r:id="rId6"/>
-    <sheet name="bigbusinessJSON" sheetId="18" r:id="rId7"/>
-    <sheet name="cracksabbathJSON" sheetId="12" r:id="rId8"/>
-    <sheet name="melvinsJSON" sheetId="14" r:id="rId9"/>
-    <sheet name="sufferingfuckheadsJSON" sheetId="15" r:id="rId10"/>
-    <sheet name="builttospillJSON" sheetId="11" r:id="rId11"/>
+    <sheet name="file title poster JSON" sheetId="27" r:id="rId2"/>
+    <sheet name="roxhillJSON" sheetId="19" r:id="rId3"/>
+    <sheet name="houston2015" sheetId="26" r:id="rId4"/>
+    <sheet name="zekeJSON" sheetId="4" r:id="rId5"/>
+    <sheet name="lastgaspJSON" sheetId="16" r:id="rId6"/>
+    <sheet name="marklaneganJSON" sheetId="17" r:id="rId7"/>
+    <sheet name="bigbusinessJSON" sheetId="18" r:id="rId8"/>
+    <sheet name="cracksabbathJSON" sheetId="12" r:id="rId9"/>
+    <sheet name="melvinsJSON" sheetId="14" r:id="rId10"/>
+    <sheet name="sufferingfuckheadsJSON" sheetId="15" r:id="rId11"/>
+    <sheet name="builttospillJSON" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3443" uniqueCount="2046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3465" uniqueCount="2068">
   <si>
     <t>ZOOM0001roxhillsessions20150827.mp3</t>
   </si>
@@ -6175,13 +6176,79 @@
   </si>
   <si>
     <t>rhodes park</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodbluntswitchtransferdisaster.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodbluntswitchtransferdisaster.mp4</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodbonelesstransfer.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodbonelesstransfer.mp4</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodfourthdimensionmarbletransfer.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodfourthdimensionmarbletransfer.mp4</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodfrigidtransfer.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodfrigidtransfer.mp4</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodintopooltransferwithalady.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodintopooltransferwithalady.mp4</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodpoolmethodtransfer.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipgodpoolmethodtransfer.mp4</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipmarbletransfer.jpg</t>
+  </si>
+  <si>
+    <t>ANDI20160601andrewflipmarbletransfer.mp4</t>
+  </si>
+  <si>
+    <t>@androflipgod BLUNT SWITCH TRANSFER DISASTER marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>@androflipgod BONELESS TRANSFER marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>@androflipgod POOL METHOD TRANSFER OUT  marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>@androflipgod FOURTH DIMENSION MARBLE TRANSFER OUT marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>@androflipgod FOURTH DIMENSION FRIGID TRANSFER OUT marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>@androflipgod LADIES NIGHT POOL TRANSFER marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>@androflipgod  MARBLE TRANSFER marginal way seattle wa</t>
+  </si>
+  <si>
+    <t>{'file':'ANDI20160601andrewflipgodbluntswitchtransferdisaster.mp4','title':'@androwflipgodflipgod bluntswitchtransferdisaster', 'poster':'ANDI20160601andrewflipgodbluntswitchtransferdisaster.jpg'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6211,6 +6278,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6598,7 +6670,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -6607,6 +6679,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="342">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7286,8 +7359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1100" workbookViewId="0">
-      <selection activeCell="C1118" sqref="C1118"/>
+    <sheetView topLeftCell="A1099" workbookViewId="0">
+      <selection activeCell="C1120" sqref="C1120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20770,6 +20843,301 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
+        <v>{'file':'ZOOM0006melvinsportlandwonderballroom20150907.mp3','title':'01  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C23" si="0">"{'file':'"&amp;A2&amp;"','title':'"&amp;B2&amp;"'},"</f>
+        <v>{'file':'ZOOM0007melvinsportlandwonderballroom20150907.mp3','title':'02  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>535</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0008melvinsportlandwonderballroom20150907.mp3','title':'03  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0009melvinsportlandwonderballroom20150907.mp3','title':'04  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>537</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0010melvinsportlandwonderballroom20150907.mp3','title':'05  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>538</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0011melvinsportlandwonderballroom20150907.mp3','title':'06  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0012melvinsportlandwonderballroom20150907.mp3','title':'07  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>540</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0013melvinsportlandwonderballroom20150907.mp3','title':'08  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
+        <v>541</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0014melvinsportlandwonderballroom20150907.mp3','title':'09  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" t="s">
+        <v>542</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0001-melvins-showboxmarket-20141018.mp3','title':'01  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
+        <v>543</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0002-melvins-showboxmarket-20141018.mp3','title':'02  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" t="s">
+        <v>544</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0003-melvins-showboxmarket-20141018.mp3','title':'03  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" t="s">
+        <v>545</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0004-melvins-showboxmarket-20141018.mp3','title':'04  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>546</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0005-melvins-showboxmarket-20141018.mp3','title':'05  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" t="s">
+        <v>542</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0006-melvins-showboxmarket-20141018.mp3','title':'01  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" t="s">
+        <v>543</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0007-melvins-showboxmarket-20141018.mp3','title':'02  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" t="s">
+        <v>544</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0008-melvins-showboxmarket-20141018.mp3','title':'03  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" t="s">
+        <v>545</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0009-melvins-showboxmarket-20141018.mp3','title':'04  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0010-melvins-showboxmarket-20141018.mp3','title':'05  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" t="s">
+        <v>547</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0011-melvins-showboxmarket-20141018.mp3','title':'06  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" t="s">
+        <v>548</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0012-melvins-showboxmarket-20141018.mp3','title':'07  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" t="s">
+        <v>549</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0013-melvins-showboxmarket-20141018.mp3','title':'08  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" t="s">
+        <v>550</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ZOOM0014-melvins-showboxmarket-20141018.mp3','title':'09  Melvins - Showbox Market - October 18th, 2014'},</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
@@ -21521,7 +21889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
@@ -22240,6 +22608,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2047</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2046</v>
+      </c>
+      <c r="D1" t="str">
+        <f>"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"','poster':'"&amp;C1&amp;"'},"</f>
+        <v>{'file':'ANDI20160601andrewflipgodbluntswitchtransferdisaster.mp4','title':'@androflipgod BLUNT SWITCH TRANSFER DISASTER marginal way seattle wa','poster':'ANDI20160601andrewflipgodbluntswitchtransferdisaster.jpg'},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2049</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D7" si="0">"{'file':'"&amp;A2&amp;"','title':'"&amp;B2&amp;"','poster':'"&amp;C2&amp;"'},"</f>
+        <v>{'file':'ANDI20160601andrewflipgodbonelesstransfer.mp4','title':'@androflipgod BONELESS TRANSFER marginal way seattle wa','poster':'ANDI20160601andrewflipgodbonelesstransfer.jpg'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2051</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ANDI20160601andrewflipgodfourthdimensionmarbletransfer.mp4','title':'@androflipgod FOURTH DIMENSION MARBLE TRANSFER OUT marginal way seattle wa','poster':'ANDI20160601andrewflipgodfourthdimensionmarbletransfer.jpg'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ANDI20160601andrewflipgodfrigidtransfer.mp4','title':'@androflipgod FOURTH DIMENSION FRIGID TRANSFER OUT marginal way seattle wa','poster':'ANDI20160601andrewflipgodfrigidtransfer.jpg'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2055</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2054</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ANDI20160601andrewflipgodintopooltransferwithalady.mp4','title':'@androflipgod LADIES NIGHT POOL TRANSFER marginal way seattle wa','poster':'ANDI20160601andrewflipgodintopooltransferwithalady.jpg'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2057</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2056</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ANDI20160601andrewflipgodpoolmethodtransfer.mp4','title':'@androflipgod POOL METHOD TRANSFER OUT  marginal way seattle wa','poster':'ANDI20160601andrewflipgodpoolmethodtransfer.jpg'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2059</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'file':'ANDI20160601andrewflipmarbletransfer.mp4','title':'@androflipgod  MARBLE TRANSFER marginal way seattle wa','poster':'ANDI20160601andrewflipmarbletransfer.jpg'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22366,7 +22864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C249"/>
   <sheetViews>
@@ -25370,7 +25868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -25814,7 +26312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -26169,7 +26667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
@@ -26604,7 +27102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -26743,7 +27241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H87"/>
   <sheetViews>
@@ -27816,299 +28314,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" t="s">
-        <v>533</v>
-      </c>
-      <c r="C1" t="str">
-        <f>"{'file':'"&amp;A1&amp;"','title':'"&amp;B1&amp;"'},"</f>
-        <v>{'file':'ZOOM0006melvinsportlandwonderballroom20150907.mp3','title':'01  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C23" si="0">"{'file':'"&amp;A2&amp;"','title':'"&amp;B2&amp;"'},"</f>
-        <v>{'file':'ZOOM0007melvinsportlandwonderballroom20150907.mp3','title':'02  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>535</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0008melvinsportlandwonderballroom20150907.mp3','title':'03  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>536</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0009melvinsportlandwonderballroom20150907.mp3','title':'04  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>537</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0010melvinsportlandwonderballroom20150907.mp3','title':'05  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>538</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0011melvinsportlandwonderballroom20150907.mp3','title':'06  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>539</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0012melvinsportlandwonderballroom20150907.mp3','title':'07  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>540</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0013melvinsportlandwonderballroom20150907.mp3','title':'08  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" t="s">
-        <v>541</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0014melvinsportlandwonderballroom20150907.mp3','title':'09  Melvins - Wonder Ballroom - Portland - September 7th, 2015'},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>542</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0001-melvins-showboxmarket-20141018.mp3','title':'01  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" t="s">
-        <v>543</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0002-melvins-showboxmarket-20141018.mp3','title':'02  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" t="s">
-        <v>544</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0003-melvins-showboxmarket-20141018.mp3','title':'03  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" t="s">
-        <v>545</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0004-melvins-showboxmarket-20141018.mp3','title':'04  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" t="s">
-        <v>546</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0005-melvins-showboxmarket-20141018.mp3','title':'05  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" t="s">
-        <v>542</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0006-melvins-showboxmarket-20141018.mp3','title':'01  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" t="s">
-        <v>543</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0007-melvins-showboxmarket-20141018.mp3','title':'02  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" t="s">
-        <v>544</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0008-melvins-showboxmarket-20141018.mp3','title':'03  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" t="s">
-        <v>545</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0009-melvins-showboxmarket-20141018.mp3','title':'04  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B19" t="s">
-        <v>546</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0010-melvins-showboxmarket-20141018.mp3','title':'05  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B20" t="s">
-        <v>547</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0011-melvins-showboxmarket-20141018.mp3','title':'06  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" t="s">
-        <v>548</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0012-melvins-showboxmarket-20141018.mp3','title':'07  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" t="s">
-        <v>549</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0013-melvins-showboxmarket-20141018.mp3','title':'08  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" t="s">
-        <v>550</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>{'file':'ZOOM0014-melvins-showboxmarket-20141018.mp3','title':'09  Melvins - Showbox Market - October 18th, 2014'},</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
 </file>
</xml_diff>